<commit_message>
New Corpus - missing sentiment analysis - INCONSISTENT STATE!
</commit_message>
<xml_diff>
--- a/data/ch_5_subsidies_reform/random_50_subsidies_in_tca.xlsx
+++ b/data/ch_5_subsidies_reform/random_50_subsidies_in_tca.xlsx
@@ -387,1304 +387,1338 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2895357895</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.1353/wvh.2018.0005</t>
+          <t>https://openalex.org/W2949246419</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Duafala (2018)</t>
+          <t>Rocha (2017)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>The Historiography of the West Virginia Mine Wars</t>
+          <t>Levantamento florístico das espécies ocorrentes na Universidade Federal do Maranhão - UFMA, Campus Codó</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>The Historiography of the West Virginia Mine Wars A. P. Duafala Between 1900 and 1922, the coalfields of Southern West Virginia witnessed some of the most intense labor violence in US labor history. This violence twice escalated into what can only be described as war, during the 1912–1913 Paint Creek–Cabin Creek strike and the 1920–1921 Mingo War. Both state and federal troops were dispatched to the area on multiple occasions to quell the violence, and the state's coal miners lived under some of the most authoritarian conditions in the country. In August 1921, a force of approximately ten thousand union coal miners began an armed march on Logan and Mingo Counties, vowing to depose Logan sheriff Don Chafin and free their imprisoned union brothers. This incident resulted in the week-long Battle of Blair Mountain and comprised what has often been described as the largest armed insurrection on US soil since the American Civil War. Despite the sensational nature of these events and significant press coverage at the time, the West Virginia Mine Wars have largely disappeared from the nation's collective consciousness. Over the years, there have been numerous interpretations and revisions of the history of the Mine Wars. While contemporary accounts of these events in West Virginia attributed this violence to the degenerative effects of "mountain culture," historians have found that they resulted from a more complex blend of cultural, social, political, and economic forces. The mid-century institutional labor historians largely accepted the "mountain culture" narrative and cast the region's inhabitants as incapable of shaping their own destiny, requiring outside intervention in the form of the United Mine Workers of America (UMWA). This conceptual model was challenged by the New Left historians, whose focus on bottom-up history attempted to restore agency to the West Virginia coal miners. The New Left interpretation of the Mine Wars as a liberation struggle continues to define the historiography of the topic to the present, with important exceptions. In recent decades, a new generation [End Page 71] of scholars, composed of historians, community activists, and Mine Wars descendants, have contributed in their own way to a broader understanding of the topic by connecting events at the community level to the wider themes of labor history. This article is intended to provide a thorough guide for those wishing to undertake further study of the West Virginia Mine Wars. Newspaper and magazine articles in many ways set the tone for early narratives of the Mine Wars. Publications as diverse as the Huntington Socialist and Labor Star, the New York Times, Nation, Survey, Literary Digest, Atlantic Monthly, and the International Socialist Review all ran articles chronicling events in the coalfields.1 The majority of these articles, written by muckraking journalists, were designed to "titillate their readers and to inspire support for industrial reform."2 This approach led to an oversimplification of the conflict and its root causes and fueled the mountain-culture stereotypes. This image of Appalachian culture, built on sensationalized coverage of the late-nineteenth-century Hatfield-McCoy Feud, cast the region's inhabitants as prone to violence and outside of the American cultural mainstream. That narrative not only advanced the cultural "othering" of the Appalachian people, allowing the exploitation of the region's population and natural resources, it also permitted the nation to turn a blind eye to Appalachia's problems and the external forces that exacerbated them.3 Since the late nineteenth century, while the popular press regaled the American public with accounts of the violent manifestations of mountain culture, historians, anthropologists, and sociologists have been trying to define just what this culture is, with equally harmful results. At the turn of the century, William Goodell Frost, president of Berea College, pointed to the region's geographic, sociocultural, and economic isolation to explain the inhabitants presumed backwardness. Frost believed the Appalachian people possessed the characteristics of the original American colonists, both at their best, exemplified by fierce independence, and at their worst, represented in the violent streak displayed in hillbilly feuds. The writers of the day emphasized the role of the mountains in the development, or lack thereof, of the Appalachian people. In 1901, geographer Ellen...</t>
+          <t>ABSTRACT With the increasing urban development on the natural environments, that ends up influencing_x000D_
+the loss of much of the biodiversity of these environments. The floristic survey is essential_x000D_
+because it allows to know and identify the biological diversity, and to provide subsidy for the_x000D_
+elaboration of projects of management and conservation of these environments. The objective_x000D_
+of this work is to survey the plant species occurring at UFMA, Campus VII Codo and identify_x000D_
+ethnobotanical aspects of these species as ornamental, medicinal, food and toxic. The collection_x000D_
+was carried out between August 2016 and February 2017, in the morning shift, with the aid of_x000D_
+pruning shears, newspaper, cardboard, wood presses, sisal rope, field sheet, camera for_x000D_
+photographic registration of the species In their habitats, and the use of specialized taxonomic_x000D_
+literature to identify the specimens. Sixty-six species were registered at UFMA, Campus VII_x000D_
+Codo, distributed in 33 families and 57 genera. Fabaceae with eight species, Euphorbiaceae_x000D_
+with seven species, Convolvulaceae with five species, Asteraceae, and Malvaceae with four_x000D_
+species, Amaranthaceae, Arecaceae, Poaceae and Rubiaceae with three each, corresponding to_x000D_
+60.63% of the Total collected. With predominance of the herb form of life (51.52%), followed_x000D_
+by sub shrub species (18.18%), shrubs (10.61%), climbers (9.09%), trees (6.06%) and palm_x000D_
+trees (4.55%). As for the origin 76% are native; 12% are cultivated; 9% and 3% are naturalized_x000D_
+and undetermined respectively. Of the total collected 20 species have medicinal potential, 14_x000D_
+species are ornamental and 8 species are food, being six PANC's. This work pointed out that_x000D_
+the flora of the campus presents a relevant plant diversity serving not only for landscaping but_x000D_
+as a source of botanical material for practical classes and undergraduate research.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2518456030</t>
+          <t>https://openalex.org/W1165989156</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1353/cwe.2016.0053</t>
+          <t>https://doi.org/10.2991/ermm-15.2015.72</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Nash (2016)</t>
+          <t>Qu &amp; Song (2015)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Claiming the Union: Citizenship in the Post–Civil War South by Susanna Michele Lee</t>
+          <t>Analysis of Human Needs under Basic Principles of Marxism</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Reviewed by: Claiming the Union: Citizenship in the Post–Civil War South by Susanna Michele Lee Steven E. Nash (bio) Claiming the Union: Citizenship in the Post–Civil War South. By Susanna Michele Lee. (New York: Cambridge University Press, 2014. Pp. 270. Cloth, $95.00.) Susanna Michele Lee’s Claiming the Union sheds new light on something we thought we already knew. Lee examines the records of the Southern Claims Commission (SCC), the post–Civil War congressional commission tasked with assessing southerners’ claims for lost and damaged property, and interprets them differently from many scholars before her. The SCC records are a staple of Civil War loyalty scholarship, casting significant light on southerners marginalized or silenced by the Lost Cause’s facade of white unity. Claiming the Union is not another attempt to glean every last hint of wartime loyalty out of postwar records. Lee successfully places the wartime struggles over loyalty and citizenship in the SCC’s proper Reconstruction context. This placement of the SCC squarely within the Reconstruction era is insightful in and of itself. But Lee offers much more than that; she argues that the process embedded in the SCC’s direct engagement with southern civilians informed a “vernacular citizenship” that shaped postemancipation American citizenship (7). The overall result is a thoughtful and effective book that enriches our understanding of the complex nature of postemancipation American citizenship. In Claiming the Union, Lee carries key questions about the war (such as loyalty and African American agency) through to the postwar period. For instance, the issue of loyalty had significant postwar ramifications as Radical Republicans battled moderates within their party and Democrats over the issue of who should rule. Radicals argued that past loyalty was the crucial factor for postwar political participation, which led them to favor stringent standards for claims. Moderate Republicans and Democrats preferred a political foundation based on future loyalty that would allow former Confederates to regain their citizenship quickly. As Lee makes clear, [End Page 467] these debates had significant impact on the process of reunion by creating a vernacular citizenship. Less concerned with the formal legal definitions of citizenship, Lee layers the war’s impact on fundamental social relationships (master and slave, husband and wife, citizen and noncitizen) against the claims each group made upon the federal government. This dialogue between southern civilians and the federal government effected changes in the meaning of citizenship through practice—direct engagement with the SCC—rather than through legal reform in a postemancipation United States. Chapters on women, former slaves, and free blacks enhance Lee’s analysis of citizenship in the post–Civil War United States. The white male SCC commissioners initially looked for open opposition to secession and overt acts of Unionism in assessing the loyalty of these “noncitizens.” However, they quickly realized that their interrogatories were ill suited for southern dependents. In fact, the commissioners’ initial list of questions made no reference to people of color or women. Women’s and African Americans’ claims forced the government to wrestle with their professions of loyalty and their place within the postwar citizenry. It is here that some of the more subtle elements of Lee’s analysis shine through. In dealing with women, Lee reveals the sectional divisions between northern and southern womanhood and male perceptions of gender difference. Accustomed to elite and middle-class white women’s involvement in reform movements, the northern commissioners struggled to understand southern white women’s professed detachment from politics. The commissioners became especially incredulous when white southern women professed personal sympathies for Confederate family members while simultaneously espousing Unionist beliefs of their own. African Americans struggled to show their loyalty to white male commissioners who viewed them as inferior and incapable of citizenship. Their persistent claims to the Union, however, forced the commission to change its procedures to allow black southerners to assert their loyalty. Strategic professions that described all black men as loyal to the Union may not have fully swayed the white commissioners, but they helped foster stronger ties among former slaves and antebellum free blacks after slavery’s demise. One of the most basic and yet most useful contributions of Claiming the Union is its contextualization of the...</t>
+          <t>Marx said that "human nature is the sum of all social relations in its reality."Man is a product of social activities; he has physical and spiritual needs, both dialectical unity.The realization of human freedom is the highest value of the pursuit of comprehensive development of Marxism.Under the reform, opening up and socialist modernization continuous development strides background.The relationship between economic interests of the people is changing, their spiritual needs also changing, and the emergence of many new features.Adhering to the people-centered scientific concept of development, and meeting the spiritual needs of people for the realization of self-improvement, maintaining social stability is of great practical significance.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2773261982</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.18844/prosoc.v2i11.1902</t>
+          <t>https://openalex.org/W1033706841</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Mavļutova (2017)</t>
+          <t>Zou (2014)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Pension system of latvia: Case study approach</t>
+          <t>China's Rise: Development-oriented Finance And Sustainable Development</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>The current paper offers a case study approach for testing several options and hypotheses. The need for Pension Reform in Latvia has been the result of a steadily increasing aging of the population. By 2001 a new three-level pension system was introduced in Latvia aiming to reduce the effect of demographic risks and demonstrating the countryâ€™s intention to provide an optimal public or private compound in old-age provision. Nevertheless,the demographic prognosis of European Commission estimates that by 2060 the population in Latvia will reduce from 2.2 million to 1.7 million people, and the number of elderly people will almost double. The potential impact of demographic change on the age structure and the size of population is dramatic and still the main problem that cast the doubt on the ability of state mandatory pension scheme to provide the appropriate pension level.Personal financial planning, personal investments are important. The objective of this research work is to investigate whether the existing Pension system in Latvia is working effectively under changing economic environment. It also analyzes the role of Private voluntary pension scheme and the current demographical situation with a flow of emigration. The research work aims at offering several options for the improvement of the situation.Keywords: Economic development, Demography, Pension Levels, Private voluntary pension scheme, Solidarity,Retirement.</t>
+          <t>As a government institution specializing in development-oriented finance, the China Development Bank (CDB) has combined advanced international financial theories with China's practical conditions and has done remarkably well in removing financing bottlenecks, establishing market credit systems, and ensuring faster and better economic and social development. Its practice and theory in development-oriented finance represent a major distinctive feature of China's socialist market economy.Written in the setting of great history, great changes and great challenges, this book contains a systematic study of the theory and practice of development-oriented finance that has evolved along with China's reform and opening up. It provides an in-depth analysis of the ideological basis, theoretical contents, operating principles and innovative development of China's financial system.China's Rise: Development-Oriented Finance and Sustainable Development will promote further discussions and researches on China's modern economic and financial systems and in turn the sustainable development of the Chinese economy and the world economy at large.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2977720812</t>
+          <t>https://openalex.org/W4205735101</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.24840/2183-8976_2021-0006_0001_12</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Aggarwal (2016)</t>
+          <t>Sun (2022)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Impact of technological innovation on regulatory reforms : Case study of Indian telecom sector</t>
+          <t>A Visual Misalignment of Modernity. Documentary Photography of Contemporary Urban Transformation in Shanghai</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>During last two decades, Indian Telecom Sector has seen a major transformation from government monopoly regime to competitive environment. Subscriber base has grown manifold and India telecom sector become second largest in the world. All this could be_x000D_
-possible because of evolving positive regulatory environment which helped in increasing the competition and reducing the tariff to enable common people to reap the benefit of mobile service._x000D_
-Since the start of liberalization process, telecom regulatory regime in India has evolved from restrictive service specific to technology neutral unified access licensing regime. Under this regime, all service providers are allowed to provide both basic as well mobile service without putting any restriction on the choice of technology unlike the initial situation of separate license for separate service and that too with the condition to use a particular technology._x000D_
-This research paper explores the factors responsible behind this evolution of telecom regulatory regime in India. It also studies about the role of technological innovations as well as various actors of the sector in this evolution process.</t>
+          <t>The built environment of contemporary Shanghai has accumulated relatively continuous historical fragments, providing a unique, complete and diachronic sample of urban transformation for documentary photography. As an objective and material fact, how the transformation has become a subjective and cultural fact that was visualized by photography remains a significant issue. &amp;#x0D; A series of art movements in China since 1976 thrived the individual’s expression, artistic or documentary, by photography. Before long, the unprecedented and nationwide urbanization realizing the comprehensive modernization after the Reform and Opening up Policy in 1978 has far surpassed the construction of the past. During the urbanization in Shanghai, architectural spectacles and highly mixed urban development has emerged, meanwhile, the historical trace of everyday life has inevitably either vanished or transformed. It is a significant interaction between the material transformation pursuing the Chinese subjective modernity by codifying “Plans” to realize the comprehensive modernization and the visualization of the specific spatial impact that reconstructed everyday life underlying the overall transformation. &amp;#x0D; Concentrating on three representative and sequential photographers whose long-term documentation illustrated the urban transformation in contemporary Shanghai: Guo Bo acted as a professional architect and a photographer as well who depicted the everyday life in vanishing residential lanes “Lilong” after the Reform; Lu Yuanmin delved into the street and gleaned the surreal micro-reactions during the transformation; And Xi Zi applied his lens to produce an urban specimen of the remaining existence of the crumbling residential housing amongst new developing areas, this paper discusses how the visual misalignment as a distinct feature and approach of the recognition of the urban transformation was revealed by documentary photography.&amp;#x0D; Although focusing on different motifs, their representations with self-consciousness as an intertextuality of urban transformation demonstrated a common sense that brought the overall transformation as a material fact of the comprehensive modernization in Shanghai back to everyday experience as a cultural fact. The coherence and distance, the intimacy and indifference, the familiarity and strangeness in the documentation endeavor sensitively to represent the visual experience of modernity in everyday life which reveals a phenomenon of misalignment in visual culture of the urban transformation in Shanghai.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://openalex.org/W3184766108</t>
+          <t>https://openalex.org/W2088687213</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1016/j.jamda.2021.05.014</t>
+          <t>https://doi.org/10.3390/atmos6030361</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Beane et al. (2021)</t>
+          <t>Xu et al. (2015)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Research to Improve Care and Outcomes for Persons With Dementia and Their Caregivers: Immediate Needs, Equitable Care, and Funding Streams</t>
+          <t>Characteristics of Organic and Elemental Carbon in PM2.5 and PM0.25 in Indoor and Outdoor Environments of a Middle School: Secondary Formation of Organic Carbon and Sources Identification</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>The articles in the July 2021 issue of JAMDA address the range of topics relevant for persons living with dementia and their caregivers—including but not limited to risk screening, 1 Yang Y. Lv C. Li H. et al. Community-based model for dementia risk screening: The Beijing Aging Brain Rejuvenation Initiative (BABRI) brain health system. J Am Med Dir Assoc. 2021; 22: 1500-1506 Abstract Full Text Full Text PDF Scopus (1) Google Scholar assessment, 2 Morandi A. Grossi E. Lucchi E. et al. The 4-DSD: A new tool to assess delirium superimposed on moderate to severe dementia. J Am Med Dir Assoc. 2021; 22: 1535-1542 Abstract Full Text Full Text PDF Scopus (1) Google Scholar medical comorbidities, 3 Richards K.C. Allen R.P. Morrison J. et al. Nighttime agitation in persons with dementia as a manifestation of restless legs syndrome. J Am Med Dir Assoc. 2021; 22: 1410-1414 Abstract Full Text Full Text PDF Scopus (2) Google Scholar behavioral distress, 4 Kang B. Pan W. Karel M.J. McConnell E.S. Rejection of care and aggression among older veterans with dementia: The influence of background factors and interpersonal triggers. J Am Med Dir Assoc. 2021; 22: 1435-1441 Abstract Full Text Full Text PDF Scopus (1) Google Scholar , 5 Mühler C. Mayer B. Bernabei R. et al. Gender differences in BPSD presentation regarding nursing home residents with cognitive impairment suffering from pain—results of the Services and Health for Elderly in Long TERm Care (SHELTER) study. J Am Med Dir Assoc. 2021; 22: 1442-1448 Abstract Full Text Full Text PDF Scopus (1) Google Scholar , 6 Harrison T.C. Blozis S.A. Schmidt B. et al. Music compared with auditory books: A randomized controlled study among long-term care residents with Alzheimer's disease or related dementia. J Am Med Dir Assoc. 2021; 22: 1415-1420 Abstract Full Text Full Text PDF Scopus (1) Google Scholar quality of life, 7 Pu L. Bakker C. Appelhof B. et al. The course of quality of life and its predictors in nursing home residents with young-onset dementia. J Am Med Dir Assoc. 2021; 22: 1456-1464 Abstract Full Text Full Text PDF Scopus (1) Google Scholar care preferences, 8 Towsley G.L. Wong B. Baier R.R. Neller S. An efficacy trial of long-term care residents with Alzheimer's disease using videos to communicate care preferences. J Am Med Dir Assoc. 2021; 22: 1559-1560 Abstract Full Text Full Text PDF Scopus (1) Google Scholar functional and behavioral care, 9 Galik E.M. Resnick B. Holmes S.D. et al. A cluster randomized controlled trial testing the impact of function and behavior focused care for nursing home residents with dementia. J Am Med Dir Assoc. 2021; 22: 1421-1428 Abstract Full Text Full Text PDF Scopus (3) Google Scholar medication use, 10 Dys S. Tunalilar O. Carder P. Cognition-enhancing, antipsychotic, and opioid medication use among assisted living and residential care residents in Oregon. J Am Med Dir Assoc. 2021; 22: 1548-1552 Abstract Full Text Full Text PDF Scopus (1) Google Scholar , 11 Xu H. Garcia-Ptacek S. Secnik J. et al. Changes in drug prescribing practices are associated with improved outcomes in patients with dementia in Sweden: Experience from the Swedish Dementia Registry 2008–2017. J Am Med Dir Assoc. 2021; 22: 1477-1483 Abstract Full Text Full Text PDF Scopus (1) Google Scholar , 12 den Brok M.G.H.E. van Dalen J.W. Abdulrahman H. et al. Antihypertensive medication classes and the risk of dementia: A systematic review and network meta-analysis. J Am Med Dir Assoc. 2021; 22: 1386-1395 Abstract Full Text Full Text PDF Scopus (2) Google Scholar telemedicine, 13 Yi J. Pittman C. Price C.L. et al. Telemedicine and dementia care: A systematic review of barriers and facilitators. J Am Med Dir Assoc. 2021; 22: 1396-1402 Abstract Full Text Full Text PDF Scopus (1) Google Scholar health services use, 14 Hakala A. Tolppanen A.M. Koponen M. et al. Does recent hospitalization increase antipsychotic initiation among community dwellers with Alzheimer’s disease. J Am Med Dir Assoc. 2021; 22: 1543-1547 Abstract Full Text Full Text PDF Scopus (1) Google Scholar ,15 Reppermund S. Heintze T. Srasuebkul P. Troller J.N. Health profiles, health services use, and transition to dementia in inpatients with late-life depression and other mental illnesses. J Am Med Dir Assoc. 2021; 22: 1465-1470 Abstract Full Text Full Text PDF Scopus (1) Google Scholar continuity of and transitions in care, 16 Aaltonen M. El Adam S. Martin-Matthews A. et al. Dementia and poor continuity of primary care delay hospital discharge in older adults: A population-based study from 2001 to 2016. J Am Med Dir Assoc. 2021; 22: 1484-1492 Abstract Full Text Full Text PDF Scopus (1) Google Scholar ,17 Knox S. Downer B. Haas A. Ottenbacher K.J. Mobility and self-care are associated with discharge to community after home health for people with dementia. J Am Med Dir Assoc. 2021; 22: 1493-1499 Abstract Full Text Full Text PDF Scopus (1) Google Scholar caregiving, 18 Fossey J. Fowler J.A. Charlesworth G. et al. Online education and cognitive behavior therapy improve dementia caregivers’ mental health: A randomized trial. J Am Med Dir Assoc. 2021; 22: 1403-1409 Abstract Full Text Full Text PDF Scopus (1) Google Scholar , 19 Zhang J. Wang Z. Li Y. et al. Effects of a caregiver training program on oral hygiene of Alzheimer's patients in institutional care. J Am Med Dir Assoc. 2021; 22: 1429-1434 Abstract Full Text Full Text PDF Scopus (2) Google Scholar , 20 Liu J. Spouse and adult-child dementia caregivers in Chinese American families: Who are more stressed out?. J Am Med Dir Assoc. 2021; 22: 1512-1517 Abstract Full Text Full Text PDF Scopus (1) Google Scholar policy, 21 MacNeil-Vroomen J.L. van der Steen J.T. Holman R. et al. Hospital deaths increased after reforms regardless of dementia status: An interrupted time-series analysis. J Am Med Dir Assoc. 2021; 22: 1507-1511 Abstract Full Text Full Text PDF Scopus (1) Google Scholar and the human rights of persons with dementia. 22 Cohen-Mansfield J. The rights of persons with dementia and their meanings. J Am Med Dir Assoc. 2021; 22: 1381-1385 Abstract Full Text Full Text PDF Scopus (1) Google Scholar The issue also includes articles that present the scientific background of 3 of the topics presented at the 2020 National Research Summit on Care, Services, and Supports for Persons With Dementia and Their Caregivers sponsored by the National Institute on Aging. 23 National Research Summit on CareServices, and supports for persons with dementia and their caregivers. https://www.nia.nih.gov/sites/default/files/2021-01/DementiaCareSummitReport.pdfDate accessed: March 13, 2021 Google Scholar ,24 Reuben D.B. Wolff J.L. The Future of Dementia Care, Caregiving, and Services Research. J Am Med Direc Assoc. 2021; 22: 1361-1362 Abstract Full Text Full Text PDF Scopus (1) Google Scholar Those 3 articles address person-centered care and the workforce, 25 Wagner L. VanHaitsma K. Kolanowski A. Spetz J. Recommendations to deliver person-centered long-term care for persons living with dementia. J Am Med Dir Assoc. 2021; 22: 1366-1370 Abstract Full Text Full Text PDF Scopus (3) Google Scholar chronic care and dementia care management, 26 Coe N. Boyd C. Chodosh J. Chronic care, dementia care management and financial considerations. J Am Med Dir Assoc. 2021; 22: 1371-1376 Abstract Full Text Full Text PDF Scopus (3) Google Scholar and integrating the financing and delivery of medical and supportive services. 27 Leff B. Stevenson D. Integrating the financing and delivery of medical and supportive services for people living with dementia. J Am Med Dir Assoc. 2021; 22: 1377-1380 Abstract Full Text Full Text PDF Scopus (3) Google Scholar Reflecting on the scope of research presented in this issue, this editorial highlights 3 important areas related to future research for persons with dementia and their caregivers, focusing on the what, the who, and the how.</t>
+          <t>Secondary organic carbon (SOC) formation and its effects on human health require better understanding in Chinese megacities characterized by a severe particulate pollution and robust economic reform. This study investigated organic carbon (OC) and elemental carbon (EC) in PM2.5 and PM0.25 collected 8–20 March 2012. Samples were collected inside and outside a classroom in a middle school at Xi’an. On average, OC and EC accounted for 20%–30% of the particulate matter (PM) mass concentration. By applying the EC-tracer method, SOC’s contribution to OC in both PM size fractions was demonstrated. The observed changes in SOC:OC ratios can be attributed to variations in the primary production processes, the photochemical reactions, the intensity of free radicals, and the meteorological conditions. Total carbon (TC) source apportionment by formula derivation showed that coal combustion, motor vehicle exhaust, and secondary formation were the major sources of carbonaceous aerosol. Coal combustion appeared to be the largest contributor to TC (50%), followed by motor vehicle exhaust (25%) and SOC (18%) in both size fractions.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2158433155</t>
+          <t>https://openalex.org/W4391642314</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://doi.org/10.3406/pole.2004.1205</t>
+          <t>https://doi.org/10.18260/1-2--39118</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Schmitter &amp; Gispert (2004)</t>
+          <t>Thomas et al. (2024)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Europe et défis démocratiques</t>
+          <t>For Us, By Us: Recommendations for Institutional Efforts to Enhance the Black Student Experience in Engineering</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Going against the trend of post-modern and pessimistic assessments of the future of European democracies, this article proposes a model of flexible and pragmatic reform. The author's ambition is to surpass the limits of democratic theory through concrete innovation and experimental initiative. In the context of a dynamic conceptualization of European political systems, Schmitter makes a series of suggestion to open up the institutional configuration of« real existing democracies » in order to reinforce their legitimacy. In light of the challenges and opportunities provided by a changing social and political environment, he points to neglected resources for incremental reform. Beyond immediate tactical considerations, he invites political scientists to embrace a new role. Research, in his opinion, must no longer be separated from political and institutional practice.</t>
+          <t>Abstract Introduction: The pursuit of education in engineering is a challenging endeavor for students. However, for Black students, this challenging experience is also coupled with racialized challenges such as experiences with racism, isolation, microaggressions, and visibility. This study focuses on the recommendations from Black graduate students in engineering to institutions. These recommendations explicitly focus on what institutions could do to enhance the experiences of Black students navigating their engineering education. This work uses an assets-based approach to prioritize the recommendations and reflections of those that have successfully navigated these environments. Awareness of the opportunities to enhance the collective experience of Black engineering students, as identified by current Black engineering graduate students, enables the establishment of an intentional agenda that institutions can employ to increase satisfaction, retention, and positive outcomes among Black engineering students. Theoretical Framework: The Person-Environment (PE) Fit Theory seeks to gauge the correlation between one’s personality type and their environment to see if there is a “fit” between the two. It relies on the congruence between personal and situational factors to lead to positive outcomes such as persistence, satisfaction, or success. This work is situated in this theory as it supports the investigation of congruence described by Black graduate students and the academic environments they have navigated. The recommendations provided by participants will serve to highlight the areas where greater congruence is necessary to promote positive outcomes for the students. Methods: Graduate students currently enrolled in doctoral engineering programs were recruited for this study. A total of sixteen individuals participated in this study with all identifying as Black. The qualitative analysis of the data was conducted in two cycles. As a first-cycle analysis, transcripts were coded deductively for recommendations. The code ‘recommendations’ was defined as ideas, thoughts, and/or solutions stated by participants in suggesting ways that the experience for Black students could be improved. Recommendations. could apply to undergraduate and/or graduate level and be regarding any aspect of the engineering students’ experiences from classes to student organizations. All excerpts coded as recommendations were then exported. Pattern coding was applied as a second-cycle coding mechanism to categorize recommendations according to their focus. Several categories, or themes, were derived from the recommendation data. Findings: The following three themes were the most reported across the participants. Underlying many of the recommendations was a desire for the institution to be intentional and accountable in their efforts to foster environments more inclusive to and aware of the Black student experiences. The specific themes were: faculty awareness and development, intentional recruitment and accountability, and metrics to assess diversity, equity, and inclusion. Faculty Awareness and Development: Participants conveyed an urgent need for faculty awareness and development, specifically in terms of their individual cultural competence, attitudes and behaviors around inclusivity, and empathy; to be mandated and monitored by institutions. Many students expressed a belief that opportunities to talk and share their experiences would aid in the development of material that could be utilized for effective interventions and training of faculty with the goals of promoting equity and inclusion at the forefront. Participants also shared similar sentiments related to faculty providing equal treatment to all students and better understanding the demographics, backgrounds, identities, and cultural norms of students with whom they work. Students expressed the significance of feeling supported by faculty, despite their ethnic backgrounds. Across the participants, the critical role that faculty play in students’ satisfaction and success, was evident. Intentional Recruitment: Participants described an “easy” solution to the difficulty related to recruiting Black faculty and students—intentionality. The perception across the participants was that institutions lack intentionality in their recruitment of Black faculty and students, which influenced disbelief that institutions truly want different, and particularly, better, outcomes for Black students. Participants recognized the importance of critical mass and urged that representation matters. Myriad solutions to enhance recruitment were provided such as having institutions attend the National Society of Black Engineers (NSBE) Annual Convention and diversifying administrations in a way that would influence top-down foci on diversity. However, at the core of a complex problem in underrepresentation, a low-hanging strategy that institutions are not currently perceived to employ is intentionality abou</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4232551778</t>
+          <t>https://openalex.org/W3022886587</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://doi.org/10.5334/bcm.b</t>
+          <t>https://doi.org/10.1016/j.mnl.2020.03.001</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Dursun-Özkanca (2021)</t>
+          <t>Warshawsky &amp; Fitzpatrick (2020)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Literature Review</t>
+          <t>Marian K. Shaughnessy, DNP, RN</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>This &lt;i&gt;Security Sector Reform (SSR) Paper&lt;/i&gt; offers a universal and analytical perspective on the linkages between Security Sector Governance (SSG)/SSR (SSG/R) and Sustainable Development Goal-16 (SDG-16), focusing on conflict and post-conflict settings as well as transitional and consolidated democracies. Against the background of development and security literatures traditionally maintaining separate and compartmentalized presence in both academic and policymaking circles, it maintains that the contemporary security- and development-related challenges are inextricably linked, requiring effective measures with an accurate understanding of the nature of these challenges. In that sense, SDG-16 is surely a good step in the right direction. After comparing and contrasting SSG/R and SDG-16, this &lt;i&gt;SSR Paper&lt;/i&gt; argues that human security lies at the heart of the nexus between the &lt;i&gt;2030 Agenda&lt;/i&gt; of the United Nations (UN) and SSG/R. To do so, it first provides a brief overview of the scholarly and policymaking literature on the development-security nexus to set the background for the adoption of &lt;i&gt;The Agenda 2030&lt;/i&gt;. Next, it reviews the literature on SSG/R and SDGs, and how each concept evolved over time. It then identifies the puzzle this study seeks to address by comparing and contrasting SSG/R with SDG-16. After making a case that human security lies at the heart of the nexus between the UN’s &lt;i&gt;2030 Agenda&lt;/i&gt; and SSG/R, this book analyses the strengths and weaknesses of human security as a bridge between SSG/R and SDG-16 and makes policy recommendations on how SSG/R, bolstered by human security, may help achieve better results on the SDG-16 targets. It specifically emphasizes the importance of transparency, oversight, and accountability on the one hand, and participative approach and local ownership on the other. It concludes by arguing that a simultaneous emphasis on security and development is sorely needed for addressing the issues under the purview of SDG-16.</t>
+          <t>Marian K. Shaughnessy was a nationally known nurse leader and philanthropist. She was the founder of the Marian K. Shaughnessy Nurse Leadership Academy at the Frances Payne Bolton School of Nursing, Case Western Reserve University where she served as an adjunct professor. Dr. Shaughnessy held leadership board positions in a wide number of Cleveland non-profits and was a member of the board of University Hospitals Medical Center of Cleveland and served as vice-chair of the Quality and Professional Committee and a member of the Clinical Council, University Hospital Medical Group. She also served on the Advisory Committee for Notre Dame School of Nursing in South Euclid, OH. She helped launch the national Nurses on Boards Coalition for the American Nurses Foundation in order to present a nursing perspective to America's boardrooms. Her nursing career included leadership positions and consulting in perioperative care delivery at the Cleveland Clinic Foundation and Lakewood Hospital, and Critical Care at Cleveland Metropolitan General Hospital. She was a member of the American Nurses Association, Association of Operating Room Nurses, Association of Nurse Executives and Sigma Theta Tau. This interview was conducted in September, 2019. She will be missed. Marian K. Shaughnessy was a nationally known nurse leader and philanthropist. She was the founder of the Marian K. Shaughnessy Nurse Leadership Academy at the Frances Payne Bolton School of Nursing, Case Western Reserve University where she served as an adjunct professor. Dr. Shaughnessy held leadership board positions in a wide number of Cleveland non-profits and was a member of the board of University Hospitals Medical Center of Cleveland and served as vice-chair of the Quality and Professional Committee and a member of the Clinical Council, University Hospital Medical Group. She also served on the Advisory Committee for Notre Dame School of Nursing in South Euclid, OH. She helped launch the national Nurses on Boards Coalition for the American Nurses Foundation in order to present a nursing perspective to America's boardrooms. Her nursing career included leadership positions and consulting in perioperative care delivery at the Cleveland Clinic Foundation and Lakewood Hospital, and Critical Care at Cleveland Metropolitan General Hospital. She was a member of the American Nurses Association, Association of Operating Room Nurses, Association of Nurse Executives and Sigma Theta Tau. This interview was conducted in September, 2019. She will be missed. NW: How did you become interested in leadership? MKS: I was always eager to accept a challenge and assume leadership roles in organizations. My leadership experiences began early in my career. While an undergraduate student at Indiana University School of Nursing, I served as president of the local student nurses organization. Throughout my career, I always wanted to experience different things and challenge myself by taking on additional responsibilities. Although direct clinical care is what most people think of when they speak about the nursing profession, I always believed there was something more. I considered joining the Air Force but was not interested in making a 4-year commitment, so I became a travelling nurse working in hospitals that were in dire need of greater support. The challenges varied, and I had to figure out how to handle many difficult clinical and leadership situations. Travel nursing taught me to seize the opportunities to lead. When my dad became ill, my mother asked me to return home. I was a critical care nurse, so I started working as a clinical instructor in critical care. It was during that time that I decided to return to school for an MSN in medical surgical nursing at the Frances Payne Bolton School of Nursing, Case Western Reserve University. My first major leadership role was as an associate director of the operating room at the Cleveland Clinic. It was the most impactful role of my career. It required assuming the executive role because it involved managing a large budget and over 400 staff members, including the physicians. This dynamic leadership opportunity required tremendous advocacy skills and political expertise. It was during that experience when I realized nurses at all levels, from the bedside to the boardroom, need more education in business skills, including finance and organizational management. Nurses should not continue to be part of a patriarchal system, that is, we should do everything we can to change the physician–nurse hierarchy. We should not be the least educated profession. We must elevate our education and status, and contribute as well-educated and well-prepared team members. Now more than ever, nurses must seize the opportunity to be leaders in health care and beyond. Nurse leaders will be the agents of change responsible for providing others with a path for positive changes in the health care field and in society. NW: How have your board experiences added t</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://openalex.org/W3124310963</t>
+          <t>https://openalex.org/W2045763234</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1111/j.1475-679x.2011.00412.x</t>
+          <t>https://doi.org/10.1080/02722010509481374</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Cassar (2011)</t>
+          <t>O’Neill (2005)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Discussion of The Value of Financial Statement Verification in Debt Financing: Evidence from Private U.S. Firms</t>
+          <t>How Two Cows Make a Crisis: U.S.-Canada Trade Relations and Mad Cow Disease</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Journal of Accounting ResearchVolume 49, Issue 2 p. 507-528 Discussion of The Value of Financial Statement Verification in Debt Financing: Evidence from Private U.S. Firms GAVIN CASSAR, GAVIN CASSAR University of Pennsylvania.Search for more papers by this author GAVIN CASSAR, GAVIN CASSAR University of Pennsylvania.Search for more papers by this author First published: 07 February 2011 https://doi.org/10.1111/j.1475-679X.2011.00412.xCitations: 28 I appreciate the detailed comments from the editor (Philip Berger) and helpful discussions with Richard Lambert and Teri Yohn. The data used in this study are publicly available from the Federal Reserve Board. Read the full textAboutPDF ToolsRequest permissionExport citationAdd to favoritesTrack citation ShareShare Give accessShare full text accessShare full-text accessPlease review our Terms and Conditions of Use and check box below to share full-text version of article.I have read and accept the Wiley Online Library Terms and Conditions of UseShareable LinkUse the link below to share a full-text version of this article with your friends and colleagues. Learn more.Copy URL Share a linkShare onEmailFacebookTwitterLinkedInRedditWechat REFERENCES Akhavein, J.; W. S. Frame; and L. White. The Diffusion of Financial Innovation: An Examination of the Adoption of Small Business Credit Scoring by Large Banking Organizations. Journal of Business 78 (2005): 577–96. 10.1086/427639 Web of Science®Google Scholar Allee, K. D., and T. L. Yohn. The Demand for Financial Statements in an Unregulated Environment: An Examination of the Production and Use of Financial Statements by Privately-Held Small Businesses. The Accounting Review 84 (2009): 1–25. 10.2308/accr.2009.84.1.1 Web of Science®Google Scholar American Institute of Certified Public Accountants (AICPA) and Financial Accounting Standards Board (FASB) . Enhancing the Financial Accounting and Reporting Standard-Setting Process for Private Companies. Norwalk , CT : FASB, 2006. Google Scholar Ang, J. S. On the Theory of Finance for Privately Held Firms. Journal of Small Business Finance 1 (1992), 185–203. Google Scholar Asquith, P.; A. Beatty; and J. Weber. Performance Pricing in Bank Debt Contracts. Journal of Accounting and Economics 40 (2005): 101–28. 10.1016/j.jacceco.2004.09.005 Web of Science®Google Scholar Barth, M. E.; D. P. Cram; and K. K. Nelson. Accruals and the Prediction of Future Cash Flows. The Accounting Review 76 (2001): 27–58. 10.2308/accr.2001.76.1.27 Web of Science®Google Scholar Bates, T. Commercial Bank Financing of White- and Black-Owned Small Business Start-Ups. Quarterly Review of Economics and Business 31 (1991): 64–80. Web of Science®Google Scholar Bates, T. A. Financing Small Business Creation: The Case of Chinese and Korean Immigrant Entrepreneurs. Journal of Business Venturing 12 (1997): 109–24. 10.1016/S0883-9026(96)00054-7 Web of Science®Google Scholar Berger, A. N., and W. S. Frame. Small Business Credit Scoring and Credit Availability. Journal of Small Business Management 45 (2007): 5–22. 10.1111/j.1540-627X.2007.00195.x Web of Science®Google Scholar Berger, A. N.; W. S. Frame; and N. Miller. Credit Scoring and the Availability, Price and Risk of Small Business Credit. Journal of Money, Credit, and Banking 37 (2005): 191–222. 10.1353/mcb.2005.0019 Web of Science®Google Scholar Berger, A. N., and G. F. Udell. Collateral, Loan Quality and Bank Risk. Journal of Monetary Economics 25 (1990): 21–42. 10.1016/0304-3932(90)90042-3 Web of Science®Google Scholar Berger, A. N., and G. F. Udell. Line of Credit and Relationship Lending in Small Firm Finance. Journal of Business 68 (1995): 351–81. 10.1086/296668 Google Scholar Berger, A. N., and G. F. Udell. The Economics of Small Business Finance: The Roles of Private Equity and Debt Markets in the Financial Growth Cycle. Journal of Banking and Finance 22 (1998): 613–73. 10.1016/S0378-4266(98)00038-7 Web of Science®Google Scholar Berger, A. N., and G. F. Udell. Small Business Credit Availability and Relationship Lending: The Importance of Bank Organizational Structure. The Economic Journal 112 (2002): F32–F53. 10.1111/1468-0297.00682 Web of Science®Google Scholar Bharath, S. T.; S. Dahiya; A. Saunders; and A. Srinivasan. Lending Relationships and Loan Contract Terms. Review of Financial Studies (2011): Forthcoming, doi: 10.1093/rfs/hhp064. Google Scholar Blackwell, D. W.; T. R. Noland; and D. B. Winters. The Value of Auditor Assurance: Evidence from Loan Pricing. Journal of Accounting Research 36 (1998): 57–70. 10.2307/2491320 Web of Science®Google Scholar Blanchflower, D. G.; P. B. Levine; and D. J. Zimmerman. Discrimination in the Small-Business Credit Market. The Review of Economics and Statistics 85 (2003): 930–43. 10.1162/003465303772815835 Web of Science®Google Scholar Bygrave, W. D.; M. Hay; E. Ng; and P. Reynolds. Executive Forum: A Study of Informal Investing in 29 Nations Composing the Global Entrepreneurship Monitor. Venture Capital 5 (2003): 101–16. 10.1080/1369106032000097021 Google Scholar Cano-Rodriguez, M. Big Auditors, Private Firms and Accounting Conservatism: Spanish Evidence. European Accounting Review 19 (2010): 131–59. 10.1080/09638180902989426 Web of Science®Google Scholar Cassar, G. Financial Statement and Projection Preparation in Start-Up Ventures. The Accounting Review 84 (2009): 27–51. 10.2308/accr.2009.84.1.27 Web of Science®Google Scholar Cassar, G., and B. Gibson. Budgets, Internal Reports and Manager Forecast Accuracy. Contemporary Accounting Research 25 (2008): 707–37. 10.1506/car.25.3.3 Web of Science®Google Scholar Cassar, G., and S. Holmes. Capital Structure and Financing of SMEs: Australian Evidence. Accounting and Finance 43 (2003): 123–47. 10.1111/1467-629X.t01-1-00085 Google Scholar Cassar, G., and C. D. Ittner. Initial Retention of External Accountants in Start-Up Ventures. European Accounting Review 18 (2009): 313–40. 10.1080/09638180902731562 Web of Science®Google Scholar Cavalluzzo, K. S., and L. C. Cavalluzzo. Market Structure and Discrimination: The Case of Small Businesses. Journal of Money, Credit and Banking 30 (1998): 771–92. 10.2307/2601128 Web of Science®Google Scholar Cavalluzzo, K. S.; L. C. Cavalluzzo; and J. D. Wolken. Competition, Small Business Financing, and Discrimination: Evidence from a New Survey. Journal of Business 75 (2002): 641–79. 10.1086/341638 Web of Science®Google Scholar Core, J. Discussion of Chief Executive Officer Incentives and Accounting Irregularities. Journal of Accounting Research 48 (2010), 273–87. 10.1111/j.1475-679X.2010.00367.x Web of Science®Google Scholar Cowen, C. D., and A. M. Cowen. A Survey Based Assessment of Financial Institution Use of Credit Scoring for Small Business Lending. Office of Advocacy, The United States Small Business Administration, 2006. Google Scholar Dechow P. M., and I. D. Dichev. The Quality of Accruals and Earnings: The Role of Accrual Estimation Errors. The Accounting Review 77 (2002): 35–59. 10.2308/accr.2002.77.s-1.35 Web of Science®Google Scholar Dechow, P.; W. Ge; and C. Schrand. Understanding Earnings Quality: A Review of the Proxies, Their Determinants and Their Consequences. Journal of Accounting and Economics 50 (2010): 344–401. 10.1016/j.jacceco.2010.09.001 Web of Science®Google Scholar Diamond, D.W. Debt Maturity Structure and Liquidity Risk. The Quarterly Journal of Economics 106 (1991): 709–37. 10.2307/2937924 Web of Science®Google Scholar Frame, W. S.; A. Srinivasan; and L. Woosley. The Effect of Credit Scoring on Small-Business Lending. Journal of Money, Credit and Banking 33 (2001): 813–25. 10.2307/2673896 Web of Science®Google Scholar Guay, W., and R. Verrecchia. Discussion of an Economic Framework for Conservative Accounting and Bushman and Piotroski (2006). Journal of Accounting and Economics 42 (2006): 149–65. 10.1016/j.jacceco.2006.03.003 Web of Science®Google Scholar Guenther, D. A.; E. L. Maydew; and S. E. Nutter. Financial Reporting, Tax Costs, and Book-Tax Conformity. Journal of Accounting and Economics 23 (1997): 225–48. 10.1016/S0165-4101(97)00009-8 Web of Science®Google Scholar Houghton, K. A. Audit Reports: Their Impact on the Loan Decision Process and Outcome: An Experiment. Accounting and Business Research 53 (1983): 15–20. 10.1080/00014788.1983.9729182 Google Scholar Hribar, P., and D. W. Collins. Errors in Estimating Accruals: Implications for Empirical Research. Journal of Accounting Research 40 (2002): 105–34. 10.1111/1475-679X.00041 Web of Science®Google Scholar International Accounting Standards Board (IASB) . International Financial Reporting Standard for Small and Medium-sized Entities. London , UK : IASB, 2007. Google Scholar Jimenez, G.; V. Salas; and J. Saurina. Determinants of Collateral. Journal of Financial Economics 81 (2006): 255–81. 10.1016/j.jfineco.2005.06.003 Web of Science®Google Scholar Johnson, D. A.; K. Pany; and R. White. Audit Reports and the Loan Decision: Actions and Perceptions. Auditing: A Journal of Practice and Theory 2 (1983): 38–51. Web of Science®Google Scholar Kim, J.-B.; D. A. Simunic; M. , T. Stein; and C. H. Yi. Voluntary Audits and the Cost of Debt Capital for Privately-Held Firms: Korean Evidence. Contemporary Accounting Research (2011): Forthcoming, doi: 10.1111/j.1911-3846.2010.01054.x. Google Scholar Lim, C.-Y., and H.-T. Tan. Non-Audit Service Fees and Audit Quality: The Impact of Auditor Specialization. Journal of Accounting Research 46 (2008): 199–246. 10.1111/j.1475-679X.2007.00266.x Web of Science®Google Scholar McKinley, S.; K. Pany; and P. M. J. Reckers. An Examination of the Influence of CPA Firm Type, Size, and MAS Provision on Loan Officer Decisions and Perceptions. Journal of Accounting Research 23 (1985): 887–96. 10.2307/2490846 Web of Science®Google Scholar Minnis, M. The Value of Financial Statement Verification in Debt Financing: Evidence from Private Firms. Journal of Accounting Research 49 (2011): 457–506. 10.1111/j.1475-679X.2011.00411.x Web of Science®Google Scholar Moskowitz, T. J., and A. Vissing-Jorgensen. The Returns to Entrepreneurial Investment: A Private Equity Premium Puzzle. American Economic Review 92 (2002): 745–78. 10.1257/00028280260344452 Web of Science®Google Scholar Nair, R. D., and L. E. Rittenberg. Alternative Accounting Principles for Smaller Businesses: Proposals and Analysis. Journal of Commercial Bank Lending (1983 April): 2–21. Google Scholar Nair, R. D., and L. E. Rittenberg. Messages Perceived from Audit, Review, and Compilation Reports: Extension to More Diverse Groups. Auditing: A Journal of Practice and Theory 7 (1987): 15–38. Web of Science®Google Scholar Ortiz-Molina, H., and M. F. Penas. Lending to Small Businesses: The Role of Loan Maturity in Addressing Information Problems. Small Business Economics 30 (2008): 361–83. 10.1007/s11187-007-9053-2 Web of Science®Google Scholar Pany, K., and C. H. Smith. Auditor Association with Quarterly Financial Information: An Empirical Test. Journal of Accounting Research 20 (1982): 472–81. 10.2307/2490754 Web of Science®Google Scholar Petersen, M.A. Information: Hard and Soft.” Working paper, Northwestern University , 2004. Google Scholar Petersen, M. A., and R. G. Rajan. The benefits of lending relationships: Evidence from small business data. Journal of Finance 49 (1994): 3–37. 10.1111/j.1540-6261.1994.tb04418.x Web of Science®Google Scholar Petersen, M. A., and R. G. Rajan. Does Distance Still Matter? The Information Revolution in Small Business Lending. Journal of Finance 57 (2002): 2533–70. 10.1111/1540-6261.00505 Web of Science®Google Scholar Pillsbury, C. M. Limited Assurance Engagements. Auditing: A Journal of Practice and Theory 4 (1985): 63–79. Web of Science®Google Scholar Reckers, P. M. J., and K. Pany. Quarterly Statement Reliability and Auditor Association. Journal of Accountancy 14 (1979): 97–100. Google Scholar Richardson, S. A.; R. G. Sloan; M. T. Soliman; and I. Tuna. Accrual Reliability, Earnings Persistence and Stock Prices. Journal of Accounting and Economics 39 (2005): 437–85. 10.1016/j.jacceco.2005.04.005 Web of Science®Google Scholar Roberts, M. R., and A. Sufi. Renegotiation of Financial Contracts: Evidence from Private Credit Agreements. Journal of Financial Economics 93 (2009): 159–84. 10.1016/j.jfineco.2008.08.005 Web of Science®Google Scholar Scholtens, B. Analytical Issues in External Financing Alternatives for SBEs. Small Business Economics 12 (1999): 137–48. 10.1023/A:1008045531070 Web of Science®Google Scholar Sloan, R. G. Do Stock Prices Fully Reflect Information in Accruals and Cash Flows About Future Earnings? The Accounting Review 71 (1996): 289–315. Web of Science®Google Scholar Strawser, J. R. The Role of Accountant Reports in Users’ Decision-Making Processes: A Review of Empirical Research. Journal of Accounting Literature 10 (1991): 181–208. Google Scholar Wiklund, J., and D. Shepherd. Aspiring for, and Achieving Growth: The Moderating Role of Resources and Opportunities. Journal of Management Studies 40 (2003): 1919–41. 10.1046/j.1467-6486.2003.00406.x Web of Science®Google Scholar Citing Literature Volume49, Issue2May 2011Pages 507-528 ReferencesRelatedInformation</t>
+          <t>Introduction In 2003, Canada and the United States announced their first cases of bovine spongiform encephalopathy (BSE), or mad cow disease. In May, a single infected cow was discovered in Alberta. In December, the U.S. Department of Agriculture (USDA) announced the U.S.'s first case: a dairy cow in Washington State had tested positive for BSE. Soon after, DNA testing showed that the Washington cow had been born, and most likely infected, in Canada. (1) In comparison to the European experience with BSE, two single cases among the vast cattle population of North America appear insignificant. Certainly, these cases have few implications for public health. However, the economic impact of both cases was significant for both countries, albeit far greater in Canada. Most particularly, both countries immediately lost their export market, and have yet to fully regain them. Initially, in the wake of these cases, U.S.-Canada relations remained cordial. The U.S. did not blame Canada for the BSE case, instead setting about reforming its own internal control measures. But, as the export ban lingered, relations began to deteriorate. The U.S. ultimately rejected the assessment of international experts that the U.S. and Canada treat BSE as a joint problem. In September 2004, the Canadian Conservative Party leader accused the U.S. of protectionism, and of using this case to punish Canada for its lack of full support in the war on Iraq. (22) The crux of the dispute between the two NAFTA partners has been over the U.S. decision to continue banning the import of live cattle from Canada--a decision that has had devastating effects on Canada's industry, which had become dependent on sending cattle to the U.S. for slaughter and processing. On December 29, 2004, the U.S. announced its intention to lift this ban in March 2005. However, in the wake of two further cases of Canadian BSE discovered in January 2005, and heavy opposition from some, but not all, U.S. stakeholders, a judge in Montana granted a preliminary injunction to halt lifting the ban. Canadian cattlemen, in turn, have threatened to take the U.S. to NAFTA and WTO tribunals. This article tells this story, focusing on issues of comparative and transboundary management in highly integrated agricultural systems. As one analysis puts it, BSE is a dramatic example of the importance of transboundary management systems, when human, animal, or plant health is threatened through inadvertent importation of dangerous diseases (Caswell and Sparling, 2004, pp. 1-2). It is also a broader story of the politics of transboundary in open economies, and of the ways in which these risks can undermine or potentially derail trade and integration agreements. In this case, the U.S. government rapidly closed the border for the beef trade with Canada. Subsequently, diplomatic efforts on both sides, aimed at establishing a standard of minimal risk to justify re-starting trade in live cattle have (at least at this time of writing) been derailed by political and economic interests in the U.S.. This case is likely to have broader implications for future U.S.-Canada relations in the context of agricultural trade. It also fails to inspire confidence in the ability of the three NAFTA partners--the U.S., Canada and Mexico--to resolve similar crises in the future. A detailed examination of the U.S. and Canada's response to these two cases of BSE in 2003 illustrates much of what these two countries have in common in terms of management policies--and also, the important ways in which they differ. The next part of this article discusses the separate but parallel development of BSE policies in each country, before detailing how the economic impacts on the Canadian beef sector lead to a significant divergence in each country's experience. This divergence led to a lengthy, and highly politicized, disagreement between them over the U.S.'s continued embargo of beef and cattle products from Canada. …</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2076543347</t>
+          <t>https://openalex.org/W3205453842</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1080/17525090902992289</t>
+          <t>https://doi.org/10.1111/ajr.12808</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Hoi &amp; Tong (2009)</t>
+          <t>Stewart &amp; McMillan (2021)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Social work in Hong Kong: from professionalization to ‘re-professionalization’</t>
+          <t>Australia's Rural Health Multidisciplinary Training program: Preparing for the rural health workforce that Australia needs</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>The development of professional social work in Hong Kong can be traced back to the 1960s. Similar to development of the profession in other countries, it began with social work education, and then later grew in response to the ever-changing environment. This paper will first highlight the history of the social work profession, and then outline the present situation of social work in Hong Kong. Following the introduction of managerial reform, social workers have encountered many changes. Although the image of social workers is positive in general and service quality is being monitored, morale is negatively affected. The paper addresses the major challenges that social work in Hong Kong is currently facing: implementation of the Lump Sum Grant system and capacity building through continuing professional development. Research shows that social workers are dissatisfied with the Lump Sum Grant system, and that this system demoralizes social workers. The paper also argues that compulsory continuing professional development is needed for capacity building and to promote resilience among social workers, in order both to strengthen the profession and to safeguard the interests of service recipients.</t>
+          <t>The Australian health landscape has changed significantly, and we must meet these changes and challenges head on, it has been nearly 25 years since the first University Departments of Rural Health (UDRH) and Rural Clinical Schools (RCS) were established. The first 7 UDRHs were established in 1997 followed by the first RCSs in 2000. The RCS and UDRHs, along with dental faculties offering extended rural placements, and the Northern Territory Medical Program were consolidated under the Rural Health Multidisciplinary Training (RHMT) program in 2016, with regional training hubs introduced in 2017. In this time, Australian universities have responded to and demonstrated targeted strategies that can effectively improve the percentage of health professional graduates choosing to work in rural and remote communities. There are now 21 universities funded under the RHMT program operating 19 RCSs and 16 UDRHs. The RHMT program aligns with the outcomes of the Australian Government’s Stronger Rural Health Strategy.1 In May 2020, the Australian Government received a commissioned independent evaluation of the RHMT program.2 We have had the privilege of working with the Australian Government Department of Health as they develop the response to the evaluation, aiming to leverage aspects of the program that are very effective and to contemporise the program to reflect innovation and changes to health student clinical training and service provision. This editorial will reflect on the history, the impact and the strengthening of focus of the program. Australian health training models are primarily delivered in metropolitan centres, geared towards enrolling metropolitan students, producing health professionals who are most likely to practise in high-density metropolitan centres within familiar health systems. Evidence demonstrates that these training models are not producing the necessary numbers of rural and remote health workforce/s required to service the health and well-being needs of rural, remote and very remote communities.3-5 While Australia has one of the highest ratios of doctors-per-head of population in the world, this workforce is disproportionately distributed across the country, concentrated in urban centres.6, 7 General practitioners can be trained for a concentrated range of office and community care settings, or they can be trained to deliver comprehensive general practice, emergency care and components of other medical specialist care required in rural hospitals and community settings; such doctors are rural generalists. At present, of around 1500 new general practice vocational training enrolments each year across Australia, there are approximately 150 Fellow of the Australian College of Rural and Remote Medicine (FACRRM) (10%) enrolments annually and around 85 Fellowship in Advanced Rural General Practice (FARGP) (6%).8 This does not match the proportion of the Australian population who live in rural, remote or very remote locations. It certainly is not enough to fill the existing employment vacancies in these areas, and it does not address or replace the ageing cohort of existing rural doctors as they retire. Increasing support for the training of rural generalists will thus increase the proportion of the workforce that is suitably trained for rural practice. Increased retention rates of rural practitioners occur when there is identification, engagement and recruitment of rural origin students, and when students and junior doctors are given early and well-supported rural and remote clinical placements.9-13 This approach applies to health professionals who have lived experience in rural and remote communities; they are more likely to make the decision to work rurally. Attracting more people from rural communities to train as health professionals is an important and broadly adopted strategy in building a sustainable rural health workforce.14 Few will understand the life and the needs of rural and remote communities better than those from these communities, including Aboriginal and Torres Strait Islander communities. As a pharmacist and a Deputy Commissioner, Faye McMillan attests to the success of this approach in the growth of the Aboriginal and Torres Strait Islander Health workforce, with her own experiences growing up in rural NSW and continuing to live and work in rural areas. As a rural generalist and Rural Health Commissioner, Ruth Stewart has seen health services, training providers, educators, health professionals and communities co-designing solutions that work for them, making a difference to the lives of rural people. To improve rural health, we need to better understand it. We need to understand the whys of health outcomes and evaluate which interventions and models of care are acceptable and effective. Evidence to inform such answers is growing as a result of research undertaken through the network of UDRH and RCSs. The ongoing presence and engagement of this network within rural communities dee</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://openalex.org/W3199090793</t>
+          <t>https://openalex.org/W1815652405</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Gulati (2021)</t>
+          <t>Chomitz (2010)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>COVID-19: Impact Analysis on the Indian Economy, International Tax and Transfer Pricing (preprint)</t>
+          <t>The challenge of low-carbon development : climate change and the World Bank Group - phase two</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>COVID-19, as we all know, has been a curse to the mankind. While we all wished for the year 2020 to end soon, to make a fresh start to our handicapped lifestyle, work style, etc., but little did we know that the year 2021 will be even more challenging due to subsequent wave hitting some countries._x000D_
-_x000D_
-India did reasonably well last year in controlling the spread of pandemic by imposing a strict two-month lockdown from end of March 2020 to end of May 2020. Of course, that came at a huge cost as it impacted the businesses in numerous ways, including disruption in supply chain, reduced logistical activities, demand and supply risk, change in consumer preferences, restricted access to markets, management and people impact, liquidity challenges, impact on brand value, etc. It also impacted the people physically, mentally, and economically as quite a few lost their loved ones, lost their income source – in form of losses in business leading to shut down, or job losses. _x000D_
-_x000D_
-India, being a developing country, with a huge population, had challenges unique to itself. It was a dilemma of lives vs. livelihood for the government, but with little choice left, the restrictions were gradually eased with adequate safety instructions to ensure that the economy gets back on its feet. The economy did show few signs of recovery (at least on paper), mostly a V-shaped one, with a hope of reinvigorating it once again, but all of this was short-lived. Little did we know or, rather, had an inkling – but conveniently chose to ignore – the possibility of subsequent wave of the virus – this time even more venomous. _x000D_
-_x000D_
-It all started again somewhere in the month of March this year when the cases rose rapidly, and it was in the month of April that the things started to get out of control. This compelled state governments to take their own calls – the Central government chose not to interfere this time. Whether that was the right way to deal with it or not is another story for another time. Nonetheless, this led India to surpass Brazil in second most cases in the world behind the USA. The total COVID-19 cases in India as on 8 May 2021 stands at 21.89 million</t>
+          <t>Unabated, climate change could derail development, with a one in four chance of a six-degree Celsius hike in temperature this century. Although industrialized countries are historically responsible for the build-up of heat-trapping greenhouse gases (GHGs), the United Nations' goal of stabilizing atmospheric GHG levels requires urgent and concerted worldwide efforts. Choices and investments made in the next two decades, in buildings, power plants, transport systems, and forest use, will irreversibly shape the global climate's future. The first volume of this climate change evaluation (Independent Evaluation Group, or IEG 2009) looked at World Bank Group (WBG) support for key areas of policy reform. This second volume focuses on two other areas of intervention: (i) development, transfer, and demonstration of technical and financial innovations; and (ii) finance and implementation.</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4322503887</t>
+          <t>https://openalex.org/W1971914773</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1080/14701847.2023.2184011</t>
+          <t>https://doi.org/10.1353/tech.2008.0008</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Redondo (2023)</t>
+          <t>Adelman (2008)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Human nature, objective social structure, and social reforms: unionized Spanish workers attitudes towards social legislation, 1870–1930</t>
+          <t>The Postal Age: The Emergence of Modern Communications in Nineteenth-Century America (review)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>This paper addresses the question of why labour legislation produces diverse, often opposing, responses among sectors of the population that apparently benefit from it. In particular, it explores the changes in the attitudes of unionized Spanish workers to the social reforms between 1870 and 1930. These workers had previously rejected state intervention in labour relations. Since 1870, most continued without calling for social laws, but occasionally demanded the application of those already approved. A second current among them, organized in anarcho-syndicalist associations, reiterated their opposition to those reforms. A third trend, grouped around socialist organizations, initially rejected labour legislation, but ended up supporting it. The analysis presented here aims to explain these trade-union attitudes by examining their expressions in the press, in their manifestos and public statements, and in the labour conflicts. It shows that these attitudes were based on one of the two assumptions about the social relations that shaped workers conceptions and actions at the time: “sociable human nature” and “objective social structure.” Its main thesis is that these two assumptions about what society was emerged from the partial reformulation or rejection of prior conceptions that had driven trade-union actions until the late nineteenth century.</t>
+          <t>Reviewed by: The Postal Age: The Emergence of Modern Communications in Nineteenth Century America Joseph M. Adelman (bio) The Postal Age: The Emergence of Modern Communications in Nineteenth Century America. By David M. Henkin . Chicago: University of Chicago Press, 2006 Pp. xv+221. $38. The middle of the nineteenth century, David Henkin notes, gave rise to such diverse practices as collecting autographs from famous people, valentine greetings, and junk mail—and, most important, an explosion in letter writing that transcended class and geographic boundaries. In The Postal Age, Henkin challenges technological explanations for this expansion, which attribute the growth of communication to the invention of the telegraph and the spread of railroads. Instead, he argues that sending a letter, once "an event rather than a feature of ordinary experience" (p. 17), became a staple of everyday life through a burgeoning "postal culture," in which Americans became increasingly aware of their presence and participation in a communications network that spanned the nation. In making this argument, Henkin extends our understanding of the early national post office—rendered familiar in Richard John's seminal Spreading the News—through the middle of the nineteenth century. Whereas John's argument centered on the post office as a broadcast medium for the dissemination of information through newspapers, Henkin argues that this culture, fueled by two reductions in postage rates at mid-century, coincided with a rapid increase in the need for long-distance communication to shape a network that enveloped the country. [End Page 272] Henkin moves skillfully through a broad range of topics and materials, examining the writings of postal reformers such as Pliny Miles, prescriptive literature, and hundreds of letters written by Americans both ordinary and famous. Divided into two parts, the book first examines how Americans came to see themselves as part of this new network. The postage-rate reductions and introduction of prepayment entrenched the letter as the medium of communication for a mobile and rapidly expanding population. Letters thus eclipsed newspapers as the post's primary business, first as the newspaper industry shifted its focus to local events, and then as a series of new regulations made postage cheaper and more flexible. In chapter 3, Henkin returns to familiar ground from his earlier work, City Reading (1999), charting the geography of the post office as an urban social space, detailing the ways in which the post office was a locus of interaction, and therefore a potentially dangerous and subversive space, especially for women. The second part of the book focuses on the cultural consequences of the expansion of the network through a series of case studies. First, Henkin deconstructs the personal letter, tracing its lineage from business correspondence and underscoring the tension between the private letter and its public transmission. He then examines how the construction of intimacy in personal letters played out in two great dislocations of the mid-nineteenth century: the California gold rush and the Civil War. In these two cases the (hoped for) temporary nature of the dislocation made the intimacy of letters all the more pressing. On the other hand, the new opportunities created by cheap postage also led to a decided lack of intimacy. The book therefore closes with an examination of the rise of mass mailing. Henkin demonstrates that the reduction in postal rates made possible the creation of new genres of mail, including valentines and circulars, and that the new mass of mail led to a new cultural space: the dead letter office. The Postal Age is, by the author's own admission, a brisk survey of the subject, and leaves several questions unanswered. Though Henkin very clearly states that he is most interested in postal culture and letter writing, he seems to dismiss too quickly the importance of behind-the-scenes advances in technology and the law. Even more striking, Henkin's focus on the middle third of the nineteenth century occasionally underplays the scope of the transformation of the postal system from one designed for big-city political and commercial elites to one designed for the mass of Americans. However, these are minor quibbles with an otherwise well-argued and engaging book. This is a vital addition to the small...</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4379471502</t>
+          <t>https://openalex.org/W3036912819</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://doi.org/10.7251/ace2237029b</t>
+          <t>https://doi.org/10.11648/j.ijae.20200503.12</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Bjelić et al. (2022)</t>
+          <t>Mahajan (2020)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>MACROECONOMIC STABILITY AND EUROPEAN UNION INVESTMENTS</t>
+          <t>Agriculture Trade Scenario in India and Its Global Comparisons</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>The quantity and quality of investments represent a condition for sustainable and long-term economic growth. Therefore, in economic theory, the rate of economic growth is a function of investment. This research includes an analysis of the impact of selected key macroeconomic indicators (independent variables) on the state and trend of investments in the European Union as a dependent variable. The research covers the period from 2012 to 2021. The following independent variables are chosen: GDP growth rate, interest rate, inflation, unemployment, income from indirect and direct taxes, public debt and budget deficit. The research shows the impact of these variables on the investments of the European Union, the dependent variable. The results of the regression analysis show that interest rates, unemployment, revenues from indirect taxes, as well as the public deficit and public debt have a negative and statistically significant direction in relation to investments. The GDP growth rates as well as direct tax revenues are statistically insignificant, but they have a positive regression coefficient on investments. Inflation rate is also an insignificant variable, but with negative impact on investments. The chosen model in the context of the joint action of all independent variables is statistically significant given that the coefficient of determination is 0.99. The results of the F test indicate statistical significance below 5%, so the model offers enough degrees of freedom (df) to vary the variables and statistically acceptable rating. Finally, the obtained results are significantly consistent with previous research and theoretical assumptions.</t>
+          <t>Indian economy has undergone structural changes over time with the anticipated decline in the share of agriculture in GDP.Despite a fall in its share from 55. 1 percent of GDP in 19501 percent of GDP in -51 to 15.35 percent in 2015-16-16, the importance of agriculture has not diminished mainly for two reasons.First, country achieved self-sufficiency in food production at the macro level, but still a food deficit country facing massive challenges of high prevalence of malnourished children and high incidence of poverty.Second, the dependence of the rural workforce on agriculture for employment has not declined in proportion to the sectoral contribution to GDP.It is in this context of rapid transformation of trading environment in India and the world as a whole, an attempt has been made to examine the growth pattern of agricultural sector in India.The study also examined the commodity composition and structural changesinagricultural exportsand direction of agricultural exports of India from 1991-92 to 2013-14.The study reveals that in 24 years of post-reform period, the growth of agriculture and allied sector has not been stable.It is more or less dependent on monsoon which shows the backwardness of the Indian agriculture sector and failure of new reforms to improveagriculture sector.Trends in imports and exports show that integration of Indian agriculture with global economy has improved considerably during post reform period.But still percentage of imports in total imports is quite less and percentage of exports to totalexports has shown declining trend during the post reform period particularly post-WTOperiod.Regarding the international comparisons of India with other countries, the study depicts that India lags behind the world in all the major indicators of agricultural growth.India is also facing critical situation as regards the production and yield of selected commodities.As most of the farming in India is monsoon dependent.Irrigation problems have to be addressed by the government.Indian agricultural productivity is very less as compared to world standards due to use of obsolete farming technology.Sustainability in agriculture is of utmost importance.When proper technology (in water management at the regional, state and national levels as well as crop plan of what to produce and where to produce) is used, it will be a win-win situation for both the farmers and the country.</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2583124101</t>
+          <t>https://openalex.org/W3150136042</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Çakmak et al. (2010)</t>
+          <t>Bachev (2021)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Visions for the Future of Water in Seyhan Basin, Turkey: A Backcasting Application</t>
+          <t>Understanding and evaluating the “missing” governance pillar of sustainability – the case of the Bulgarian agriculture</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>This paper reports backcasting results on the future of water in the Seyhan Basin, Turkey. The participative backcasting methodology uses prior information obtained from stakeholders about the present, future and estimated states of water to optimize time use during the implementation. The study involved a broad range of stakeholders spanning from central decision makers to farmers. Reliable scenarios exploiting all kinds of information sources are crucial in developing dependable and feasible policy options to tackle the challenges residing in water management issues. Perception of the current water system and a structured view of the future in the Seyhan Basin have been determined. The desirable goal has been set as reaching sustainable irrigation by 2030. Necessary actions to reach the desired objective were grouped into four categories, namely policy, infrastructure, legal issues and extended education. After determining specific activities in each category, the relationships and timing of the activities are set and potential obstacles are identified. The findings suggest that the participation of non-governmental organizations (NGOs) with high human capital to policy, legal and infrastructural actions is crucial. Use of water saving technologies, such as pressurized and prepaid irrigation systems, dominate the scenario. NGOs related to irrigation are expected to play a key role in finding funds that are necessary for the infrastructural investments. Support for capacity building in irrigation related NGOs will be vital in reaching the objective. Lastly, subsidies on pressurized irrigation systems will also be inevitable.</t>
+          <t>The importance of “good governance” for achieving agrarian sustainability has been increasingly studied in the last two decades. What has been a recent development is the inclusion of governance into (agrarian) sustainability as a new “fourth” pillar. Still there is no consensus on: what is governance sustainability; how to measure governance sustainability; how to integrate governance into the overall sustainability; what are critical factors determining sustainability levels, etc. The goal of this article is to present a holistic framework for defining and assessing the governance sustainability in agriculture, and assess the level of governance sustainability of Bulgarian agriculture at national, sub-sectoral, regional, ecosystem, and farming organization levels. The study has demonstrated that it is possible and important to assess the “missing” Governance Pillar of agrarian sustainability. Governance sustainability of Bulgarian agriculture is at a good but close to the inferior level. There is a considerable variation in the level of governance sustainability and application of the principles for good governance in different subsectors, agro-ecosystems, administrative regions, and types of farming organizations. At current stage, most critical for improving the governance sustainability are progressive changes in: farmers' participation in decision-making, agrarian administration efficiency, administrative services digitalization, possibility for lands extension, management board external control, level of informal system efficiency, subsidies in income, extent of CAP implementation, acceptability of legal payments, and land concentration. Suggested and other similar frameworks have to be further discussed, tested, improved and adapted to the specific conditions of agricultural systems and the needs of decision-makers. Accuracy has to be improved through the inclusion of appropriate indicators, improvement of precision of the information, increasing representation of surveyed farms, and experimenting with diverse types of agro-systems.</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2590510509</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.58680/rte20065104</t>
+          <t>https://openalex.org/W2942732018</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Lewis (2006)</t>
+          <t>Longo et al. (2019)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>AT LAST: “What’s Discourse Got to Do with It?” A Meditation on Critical Discourse Analysis in Literacy Research</t>
+          <t>Low alcohol wines: blending with an early harvest or dealcoholisation of a later harvest?</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>What's love got to do with it? Tina Turner wants to know in her song by that title. In this commentary, I want to ask a similar question about discourse in literacy research that uses critical discourse analysis (CDA).1 1 do so as someone who uses critical discourse analysis as both theory and method and, nonetheless, often asks herself this basic question: What's discourse got to do with it? To answer this question, 1*11 ask another: Why is it that at this time in the evolution of literacy studies, critical discourse analysis has become the method of choice for an increasing number of literacy researchers? The critical linguistic turn that has occurred in the humanities and social sciences for the last three decades has finally taken hold in the field of literacy education. It should come as no surprise that researchers trained to look closely at language processes are taking the opportunity to do so at this political moment. With the literacy practices and identities of young people and their teachers at stake, and a good deal of our own research and knowledge deemed unscientific and irrelevant by the current federal administration, it makes sense that literacy educators would want to understand how language has worked against us in these matters and how it can work for us in the future. WoodsideJiron's (2004) analysis of California's reading policies and Bloome and Carter's (2001) analysis of lists in reading education reform are two examples of uses of critical discourse analysis that help us understand how language instantiates particular policies. More importantly, these studies explicate the implications for how particular policies position readers and teachers in relation to texts and to each other. My point here is that critical discourse analysis has provided one wave of criticism in a sea of policies and practices that threaten to drown out dissenting voices. The increasing use of CDA methods also may stem from critiques of expressivist writing theories and progressivist pedagogies in the late 1980s and throughout the 1990s. Critical takes on expressivism and progressivism often argue that these theoretical and peda-</t>
+          <t>Over the past 20 years the level of alcohol in wine has increased in most grapegrowing regions due to global warming and consumer preferences towards full-body, riper flavour wines. This has raised a number of issues related to consumer health including increased calorie intake and risk from alcohol-related illness and disease, tax policy interventions and wine sensorial quality. The adoption of low alcohol wines (broadly defined as containing 5.5-11%v/v alcohol) is one solution to addressing these challenges, thus still allowing the enjoyment of wine. Several methods have been implemented to reduce wine alcohol content, but removal of alcohol from wine at a post-fermentation stage (dealcoholisation) is the most accepted at the industrial scale (Schmidtke et al. 2012). Among the dealcoholisation processes, membrane-based technologies, such as reverse osmosis and evaporative perstraction (membrane contactor), are the most widely employed. However, these processes also cause significant losses of important volatile compounds such as esters, which are known to confer fruity aromas to wine (Longo et al. 2017). Aside from these chemical and sensory alterations, dealcoholisation requires a high capital outlay and may have poor eco-sustainability because of high energy inputs and water requirements (Margallo et al. 2015). A more attractive and ecosustainable approach would be to harvest grapes at an early stage of ripening, when they naturally contain lower concentrations of fermentable sugars. Unfortunately, insufficiently ripened fruit may not have adequate phenolic and aromatic profiles to produce consumer acceptable wines. Early harvested grapes tend to produce wines low in flavour intensity and higher in bitterness and herbaceous characters (Pineau et al. 2011, Bindon et al. 2013). Nevertheless, a wine made from early harvested grapes could be legitimately blended with wines obtained from later harvested grapes in order to produce a less alcoholic wine or fermented together, as shown more recently in a study by Schelezki et al. (2018a, 2018b). A better understanding of how changes in aromatic compounds arise during dealcoholisation or blending processes, particularly fermentative by-products and grape-derived compounds, and how these changes impact the sensory profile of reduced alcohol wines is lacking. Research on the reduction of alcohol content has mainly focussed on small decreases in alcohol content (1-2%v/v), with minimal emphasis on understanding how chemical changes in wine affect sensory characteristics at greater alcohol reductions. As a part of a bigger project on lower alcohol wines conducted at the ARC Training Centre for Innovative Wine Production (Ristic et al. 2016), Rocco Longo established several trials to: evaluate wine blending as a tool to produce wines with more balanced, riper flavours and lower levels of alcohol assess the effect of dealcoholisation on the volatile composition and sensory profile of wines produced from mature fruit identify potential differences in the volatile and sensory composition of wines produced from early harvest regimes and dealcoholisation strategies understand how changes in chemical composition during alcohol reduction affects the sensory profile of wine.</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2184590789</t>
+          <t>https://openalex.org/W2603103181</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Afanasyev et al. (2014)</t>
+          <t>Raju &amp; Rao (2009)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Reformatory potential of the mine engineering education in the Russia history of the post-reform period</t>
+          <t>Market Timing Ability of Selected Mutual Funds in India: A Comparative Study</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>The period between the 80 th years of the XIX century and the early XX century is considered to be the time of explosive development of different industry sectors in Russia, especially mountain profile - the coal and oil production, and metallurgy. This growth has necessitated an increase in qualified engineering personnel within these sectors of economy, though in Russia there was only one higher educational institution of mountain profile - the Capital Mining Institute. Transformations in the sphere of higher mining education are considered by the example of the main activity of the Mining Institute Directors during the post-reform period. (Afanasyev V.G., Voloshinova I.V., Mokeev A.B., Podolsky S.I. Reformatory potential of the mine engineering education in the Russia history of the post-reform period. Life Sci J 2014;11(8s):49-52) (ISSN:1097-8135). http://www.lifesciencesite.com. 8</t>
+          <t>(ProQuest: ... denotes formulae omitted.)IntroductionThe mutual fund industry is a fast growing sector of the Indian financial markets. They have become major vehicle for mobilization of savings, especially from the small and household savers for investment in the capital market. Mutual funds entered the Indian capital market in 1964 with a view to provide the retail investors the benefit of diversification of risk, assured returns, professional management. Since then they have grown phenomenally in terms of number, size of operations, investor base and scope. With the ushering in of economic reforms in the early 1990s, the Government of India opened the way for the entry of private sector and foreign players into this industry. Consequently, this has emerged as a highly competitive financial service industry today. In India, the mutual fund industry came into being with the establishment of Unit Trust of India in 1964. Public sector banks and financial institutions began to establish mutual funds in 1987. The private sector and foreign institutions were allowed to set up mutual funds in 1993. Mutual funds have all come forward with varying schemes suitable to the needs of saving populace. By March 2005, there were 29 mutual funds and over 450 schemes in India, with assets under management of Rs. 1,49, 600 cr.In this study, we analyze the empirical results pertaining to the overall performance of selected mutual fund schemes in terms of various performance measures. The focus in evaluating the overall performance has been on fund manager's skills in security selection, which involve micro forecasting-forecasting of price movements of individual stocks and identifying under or overvalued stocks. But in constructing a portfolio, timing of investment is as important as selection of securities. Selection of good securities at the wrong time may not help the fund managers to achieve the investment/diversification objectives. Starting to ride the bullish trend by buying securities at its peak or offloading the securities in bearish trend at its turning point will adversely affect the rate of return. Therefore, market timing is a vital activity in the investment decision making process. It is possible for fund managers to generate superior performance by timing the market correctly, in addition to stock selection techniques. Thus, it could be possible that differential returns are generated not only by careful 'micro' security selection efforts but also by engaging in successful 'macro' market timing activities in the volatile stock markets. Successful fund managers are those who are capable of assessing correctly the direction of the market, whether bull or bear, by positioning their portfolios accordingly. If managers are expecting a declining market, they could change their portfolio suitably by increasing the cash percentage of the portfolio or by adjust their equity investments in favor of defensive securities having lower beta. In case of a rising market, fund managers could reduce the cash position or adjust their equity portfolio in favor of aggressive securities having higher beta. By adjusting their portfolios correctly to the market timing, fund managers can generate superior returns compared to the market.Review of LiteratureIn their pioneering work, Treynor and Mazuy (1966)-hereafter TM-developed a model for testing the market timing abilities of the fund managers and found significant timing ability in only 1 out of 57 funds in their sample. Henriksson and Merton (1981)- hereafter HM- developed another model for testing market timing ability, which was later validated and applied by Henriksson (1984), and found that only 3 funds out of 116 exhibited significant positive market timing ability.Kon and Jen (1979) found a large number of funds engaged in the market timing activities, but while extending their analysis, Kon (1983) found little evidence that they were successful. Chang and Lewellen (1984) also tested market timing and security selection skills of the fund managers and found little evidence of both. …</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2094308991</t>
+          <t>https://openalex.org/W2003855635</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1108/17410381311327963</t>
+          <t>https://doi.org/10.1177/095207670401900308</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Huang et al. (2013)</t>
+          <t>Metcalfe (2004)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>A supply chain configuration model for reassessing global manufacturing in China</t>
+          <t>European Policy Management: Future Challenges and the Role of the Commission</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Purpose Global manufacturers have faced unprecedented cost pressures in China because of Chinese currency appreciation, rising labour costs, higher oil prices and reduced value‐added tax rebates. This paper aims to reassess the decision of operating global manufacturing facilities in China. Design/methodology/approach A mixed integer programming model is developed for a typical global manufacturing supply chain that includes production in the Pearl River Delta region and trade in Hong Kong. A case study with a footwear product is used to illustrate model application and present detailed analyses. Findings The modelling results affirm the need of relocating labour‐intensive production that mainly competes on low costs. Nevertheless, coastal China offers considerable benefits from industrial clustering and a logistics advantage in comparison with inland China and Asian countries where labour costs are still relatively low. Hong Kong remains a robust location choice for trade operations because of its favourable tax policies. Practical implications Retaining production in China faces high risks from Chinese currency appreciation, while relocation to lower‐cost Asian countries is more vulnerable to risks from high oil prices. An intermediate trade operation in Hong Kong can be used to hedge against risks from unfavourable tax policy changes at manufacturing locations. Originality/value China has risen to an important position in global manufacturing because of its cost advantages. This paper analyzes the new phenomenon of dramatically increasing cost pressures in China. It develops a first‐of‐its‐kind supply chain configuration model for the popular front‐shop‐back‐factory business model in China.</t>
+          <t>As the Prodi Commission comes to the end of its term of office, the Kinnock reforms of internal management systems are now well under way. While these are welcome, they are only a preliminary step in a much broader and more difficult process of change. As the EU institutions have to work with and through the administrations of the member states, it is essential to develop the management of organizational networks. These networks are a negotiated multi-level order in which the Commission is only one actor. This article explores the nature of these networks, their common features and problems, arguing that the Commission use its unrivalled position to act as a strategic node for their future development.</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2016432953</t>
+          <t>https://openalex.org/W4247574616</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1016/0304-4181(88)90016-4</t>
+          <t>https://doi.org/10.18356/257892a3-en-fr</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Kowaleski (1988)</t>
+          <t>NA (2012)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>The history of urban families in medieval England</t>
+          <t>No. 45814 International Bank for Reconstruction and Development and Serbia</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Few medieval historians have turned their attention to the history of families in urban England. But the groundwork for such studies has been laid in previous scholarship on the merchant class, on women and work in towns, and on borough law and customs. Future studies, more specifically focused on families in towns, will draw upon a wide variety of sources including wills, property records, marriage litigation, coroner's rolls, poll taxes, borough customs, and, most importantly, borough plea rolls. These studies should allow us to explore how the special characteristics of the medieval urban environment – continual in-migration, economic opportunity, commercial and industrial diversity, extremes of wealth, high population density, and borough legal structures – affected family formation, life-cycle, demography, and domestic life in medieval towns.</t>
+          <t>Global Environment Facility Grant Agreement (Transitional Agriculture Reform Project) between the Republic of Serbia and the International Bank for Reconstruction and Development (acting as an Implementing Agency of the Global Environment Facility) (with schedule, appendix and Standard Conditions for Grants Made by the World Bank out of Various Funds, dated 20 July 2006). Belgrade, 27 July 2007</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>https://openalex.org/W637074070</t>
+          <t>https://openalex.org/W2599191843</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1017/s0066622x00002604</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Mitra (1992)</t>
+          <t>Butler (2015)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Power, Protest and Participation: Local Elites and Development in India</t>
+          <t>‘The radicals in these Reform times’: Politics, Grand juries, and Ireland’s Unbuilt Assize Courthouses, 1800–50</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>This book, first published in 1992, examines the attitudes of local elites – the hinge between Indian state and rural society – towards protest and participation in development, illuminating arguments about the nature of the state as well as the development process. It looks at the role of local elites in India both as the representatives of the state and of the rest of rural society, and explains their importance in the country’s development. The book deals with the elites’ contribution to the credibility of the state and examines the strategies through which they manipulate the allocation of resources and influence the pace and direction of social change. It contrasts the rural elites in two areas, one more economically advanced than the other. The elites in the first area were shown to be capable of combining institutional participation with radical protest, whilst in the other they tended to rely on state channels to achieve reform. The author concludes that despite the different settings, both groups were informed, active and responsive to political conditions. This contrasts with the conventional view that local elites of the dominant castes oppress the lower ones by obstructing reforms, for reasons of self-interest.</t>
+          <t>It is the aim, in this article, to identify the reasons why certain designs for courthouses in early-nineteenth-century Ireland remained unexecuted, and to do so by analysing surviving drawings and placing them in the political context at this time of Irish local government and of the efforts of Westminster politicians to institute reform. The funding and erection of courthouses were managed by grand juries, an archaic form of local government which gave few rights to smaller taxpayers and was widely perceived as an unaccountable institution associated with the ancien régime . In addition to hosting court sittings, courthouses were used by these grand juries for their private meetings and functions. By exploring the agendas and pretensions of these bodies, and by looking at the fluctuating availability of funding sources that were needed to initiate building work, I will argue through a series of Irish case studies that a renewed focus on elite patronage and its associated politics allows a new insight into courthouse building, which places less emphasis than is often the case on, for example, the role played by the changing legal profession in the architectural development of the courthouse. In nineteenth-century Ireland, courthouses demarcated the visible and tangible presence in the urban landscape of the law and state-sanctioned justice. Laws passed by the Irish parliament and then, after its abolition in 1800, by the Westminster government, were enforced in assize courthouses by travelling judges on established ‘circuits’, visiting each city or county town twice a year (in the spring and summer). These judges travelled with great splendour through the countryside, and were welcomed by a high sheriff at the county border and escorted with military pageantry, ritual, and procession to their destination.</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>https://openalex.org/W1863736110</t>
+          <t>https://openalex.org/W2076839998</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1111/j.1532-5415.1985.tb07107.x</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Pelton &amp; Bhasin (2000)</t>
+          <t>Thomasma (1985)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Key policy, regulatory and standards issues in global satellite communications</t>
+          <t>Personal Autonomy of the Elderly in Long‐term Care Settings</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>The field of satellite communications is becoming at least as constrained and shaped by policy, regulatory and standards issues as it is by technology. Satellite communications is currently facing a host of challenging issues, including national economic competition, open trade issues, standards and protocols, spectrum and frequency allocation, definition of essential space services requiring public funding, institutional reform, international industrial patterns of change and consolidation, technology transfer, and the proper role of government in future space communications development. This article seeks to identify possible areas for reform with regard to 'paper satellites', multi-purpose frequency allocations, longer range spectrum planning, new standards-making approaches to seamless satellite-fiber interconnectivity, and reforms to more open international trade and licensing of satellite systems. Specific issues addressed include:_x000D_
-_x000D_
-Global trade and access to national markets in the new 'open markets' trading environment. Interoperability standards and protocols. Issues of compatibility among the satellite systems of the world. Access to needed frequency allocations for satellite services amid growing global demand for broad band multi-media services and the need to revise ITU planning processes. The difference in policy perspective and objectives between developed and developing countries in the field of satellite communications and its applications. The on-going problem of 'paper satellites' and the fact that 'due diligence' has not solved this problem. Needed regulatory reforms to encourage new types of interactive broadband, multi-media satellites. Institutional reforms of key entities (the ITU, INTELSAT, Inmarsat, etc.) in the coming decade._x000D_
-_x000D_
-Technology transfer issues, especially those that involve sensitive or strategic issues as well as streamlined methods to protect international property rights. New patterns of industrial cooperation, merger and as the new global market emerges. The proper role of governmental R&amp;D support in developing new technology, applications and markets.</t>
+          <t>My son, take care of your father when he is old; Grieve him not as long as he lives. Even if his mind fails, be considerate with him; Revile him not in the fullness of your strength. For kindness to a father will not be forgotten. Sirach 3:12–14 The next great civil rights issue in the United States may well be that of persons in long-term care facilities. If statistical projections of an increasingly aging population are to be believed, the rights of persons who require some form of institutionalization for their care and protection will become the object of greater and greater attention. Indeed, even if familiar, the projections about a population shift towards an age group with a high proportion of dependent persons are awesome. According to these projections, there will be a ten-fold increase in the over-85 population over the next 50 years. Millions of persons will need some form of care that will, by its very nature, inhibit cherished values and freedoms. Providing this care is a great public and private duty for any nation. Providing it with an emphasis on personal autonomy is a challenge worthy of the highest virtues of health professionals, health administrators, and those responsible for public welfare. Enhancing personal autonomy of the institutionalized elderly is difficult. Two reasons stand out. First, the very nature of the institution means that meals must be served at certain hours so that everyone is fed, recreation time is programmed to address the possibility of boredom and listlessness, visiting hours are established, and so on. Institutional programs are all formulated and conducted in the best interests of the residents, but the residents themselves often have little say in the conduct of the institution, its rules, and its policies, even though these directly affect them. Second, as articles in this and other journals emphasize, the wishes of residents regarding health care decisions are frequently disregarded in favor of general policies designed to protect the institution from liability. As a consequence, a large percentage of public sector medical costs are devoted to the maintenance of institutionalized people. Often the confused and debilitated status of residents requires some form of paternalism. Yet, as more and more persons enter partially dependent states, greater sophistication will be required in responding to their modes of self-determination. The ever-expanding medicalization of long-term care means that technological medical care will assert more and more influence on the lives of people who have conditions that do not respond effectively to this technology. Furthermore, inadequate state and federal regulations governing long-term care facilities and licensing are now being scrutinized. However, reform-minded regulations often provide only a minimum of attention to personal autonomy, focusing instead on other important standards, such as maintenance, cleanliness, and certification of workers. It is therefore encouraging to learn that the Retirement Research Foundation of Park Ridge, Illinois, has recently launched an initiative to enhance the personal autonomy of elderly individuals in long-term care facilities. The Foundation's request for proposals stresses fundamental ethical issues involving a variety of aspects of long-term care. The Foundation “will fund projects which have practical and policy relevance, are interdisciplinary in their approach, and have as their core the real and lived experience of elderly individuals.” Through this initiative, the Foundation hopes to stimulate research on the needs and wishes of the elderly as well as the formation of policies and structures that will enhance autonomy through ethical analysis. It also hopes to stimulate other foundations to apportion funds for this important social problem. All inquiries and concept papers should be addressed to Brian Hofland, PhD, Program Officer, The Retirement Research Foundation, 325 Touhy Avenue, Park Ridge, IL 60068.</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4245535009</t>
+          <t>https://openalex.org/W2058088878</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://doi.org/10.4324/9781936331215</t>
+          <t>https://doi.org/10.1086/261457</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Levine (2010)</t>
+          <t>Pollak &amp; Wales (1987)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Zoned Out</t>
+          <t>Specification and Estimation of Nonseparable Two-Stage Technologies: The Leontief CES and the Cobb-Douglas CES</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Researchers have responded to urban sprawl, congestion, and pollution by assessing alternatives such as smart growth, new urbanism, and transit-oriented development. Underlying this has been the presumption that, for these options to be given serious consideration as part of policy reform, science has to prove that they will reduce auto use and increase transit, walking, and other physical activity. Zoned Out forcefully argues that the debate about transportation and land-use planning in the United States has been distorted by a myth?the myth that urban sprawl is the result of a free market. According to this myth, low-density, auto-dependent development dominates U.S. metropolitan areas because that is what Americans prefer. Jonathan Levine confronts the free market myth by pointing out that land development is already one of the most regulated sectors of the U.S. economy. Noting that local governments use their regulatory powers to lower densities, segregate different types of land uses, and mandate large roadways and parking lots, he argues that the design template for urban sprawl is written into the land-use regulations of thousands of municipalities nationwide. These regulations and the skewed thinking that underlies current debate mean that policy innovation, market forces, and the compact-development alternatives they might produce are often 'zoned out' of metropolitan areas. In debunking the market myth, Levine articulates an important paradigm shift. Where people believe that current land-use development is governed by a free-market, any proposal for policy reform is seen as a market intervention and a limitation on consumer choice, and any proposal carries a high burden of scientific proof that it will be effective. By reorienting the debate, Levine shows that the burden of scientific proof that was the lynchpin of transportation and land-use debates has been misassigned, and that, far from impeding market forces or limiting consumer choice, policy reform that removes regulatory obstacles would enhance both. A groundbreaking work in urban planning, transportation and land-use policy, Zoned Out challenges a policy environment in which scientific uncertainty is used to reinforce the status quo of sprawl and its negative consequences for people and their communities.</t>
+          <t>Previous articleNext article No AccessSpecification and Estimation of Nonseparable Two-Stage Technologies: The Leontief CES and the Cobb-Douglas CESRobert A. Pollak and Terence J. WalesRobert A. Pollak Search for more articles by this author and Terence J. Wales Search for more articles by this author PDFPDF PLUS Add to favoritesDownload CitationTrack CitationsPermissionsReprints Share onFacebookTwitterLinkedInRedditEmail SectionsMoreDetailsFiguresReferencesCited by Journal of Political Economy Volume 95, Number 2Apr., 1987 Article DOIhttps://doi.org/10.1086/261457 Views: 21Total views on this site Citations: 19Citations are reported from Crossref Copyright 1987 The University of ChicagoPDF download Crossref reports the following articles citing this article:Wenting Zhan, Wei Pan, Gang Hao Productivity Measurement and Improvement for Public Construction Projects, Journal of Construction Engineering and Management 148, no.66 (Jun 2022).https://doi.org/10.1061/(ASCE)CO.1943-7862.0002282Thomas Brasch, Arvid Raknerud The impact of new varieties on aggregate productivity growth*, The Scandinavian Journal of Economics 84 (May 2022).https://doi.org/10.1111/sjoe.12464Shashika D. Rathnayaka, Eliyathamby A. Selvanathan, Saroja Selvanathan Modelling the consumption patterns in the Asian countries, Economic Analysis and Policy 15 (Feb 2022).https://doi.org/10.1016/j.eap.2022.02.004Bilgehan Karabay Vertical Fragmentation and International Sourcing, SSRN Electronic Journal (Jan 2017).https://doi.org/10.2139/ssrn.2989546James J. Heckman Introduction to a Theory of the Allocation of Time by Gary Becker, The Economic Journal 125, no.583583 (Mar 2015): 403–409.https://doi.org/10.1111/ecoj.12228Stefan Boeters, Luc Savard The Labor Market in Computable General Equilibrium Models, (Jan 2013): 1645–1718.https://doi.org/10.1016/B978-0-444-59568-3.00026-2Stefan Boeters, Luc Savard The Labour Market in CGE Models, SSRN Electronic Journal (Jan 2011).https://doi.org/10.2139/ssrn.1987650Jürgen Antony A class of changing elasticity of substitution production functions, Journal of Economics 100, no.22 (Feb 2010): 165–183.https://doi.org/10.1007/s00712-010-0118-3Stefan Boeters, Michael Feil Heterogeneous Labour Markets in a Microsimulation–AGE Model: Application to Welfare Reform in Germany, Computational Economics 33, no.44 (Nov 2008): 305–335.https://doi.org/10.1007/s10614-008-9161-3Eyal Winter Optimal incentives for sequential production processes, The RAND Journal of Economics 37, no.22 (Jun 2006): 376–390.https://doi.org/10.1111/j.1756-2171.2006.tb00021.xAlexandre Gohin The specification of price and income elasticities in computable general equilibrium models: An application of latent separability, Economic Modelling 22, no.55 (Sep 2005): 905–925.https://doi.org/10.1016/j.econmod.2005.06.005K.K. Gary Wong A New Approach to Modelling Gnp Functions: an Application of Two-Stage Technologies and Modifying Function Framework, Australian Economic Papers 43, no.33 (Sep 2004): 315–339.https://doi.org/10.1111/j.1467-8454.2004.00233.xRonald G. Felthoven, Catherine J. Morrison Paul Multi‐Output, Nonfrontier Primal Measures of Capacity and Capacity Utilization, American Journal of Agricultural Economics 86, no.33 (Aug 2004): 619–633.https://doi.org/10.1111/j.0002-9092.2004.00605.xIkerne Del Valle, Inmaculada Astorkiza, Kepa Astorkiza Fishing effort validation and substitution possibilities among components: the case study of the VIII division European anchovy fishery, Applied Economics 35, no.11 (Jan 2003): 63–77.https://doi.org/10.1080/00036840210158949Carlo Perroni, Thomas F. Rutherford Regular flexibility of nested CES functions, European Economic Review 39, no.22 (Feb 1995): 335–343.https://doi.org/10.1016/0014-2921(94)00018-UClinton R. Shiells, David W. Roland-Hoist, Kenneth A. Reinert Modeling a north American free trade area: Estimation of flexible functional forms, Review of World Economics 129, no.11 (Mar 1993): 55–77.https://doi.org/10.1007/BF02707487Michael J. Mueller Endogenous taxes in a vertically integrated, natural resource extracting firm, Energy Economics 13, no.11 (Jan 1991): 55–60.https://doi.org/10.1016/0140-9883(91)90056-6Dennis O. Olson, Yeung-Nan Shieh Estimating functional forms in cost-prices, European Economic Review 33, no.77 (Sep 1989): 1445–1461.https://doi.org/10.1016/0014-2921(89)90057-3John Baffes, Utpal Vasavada On the choice offunctional forms in agricultural production analysis, Applied Economics 21, no.88 (Oct 2011): 1053–1061.https://doi.org/10.1080/758531242</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4235672226</t>
+          <t>https://openalex.org/W2169814545</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://doi.org/10.22541/au.157590106.66877572</t>
+          <t>https://doi.org/10.1596/1813-9450-2444</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Neal (2019)</t>
+          <t>Hellman et al. (2000)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Ethics in the Criminal Justice System</t>
+          <t>Seize the State, Seize the Day: State Capture, Corruption, and Influence in Transition</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Our keepers of the peace and enforcers of the law are surrounded by crime and criminals, but something separates them from criminality. The criminal justice system is complex, but one thing grounds it’s practitioners: a foundation of ethics. According to Peak (2012), “ethics involves doing what is right or correct and is generally used to refer to how people should behave in a professional capacity” (p. 278). This paper will explore the role that ethics plays in the three facets of justice: law enforcement, the courts, and corrections. Additionally, this paper will look at the results that ethical criminal justice practitioners have on the criminal justice system, as well as examine what results when ethics are replaced by selfishness and corruption. Ethics are foundational to the criminal justice system and to the achievement of it’s overarching goals: preservation of peace and fulfillment of justice. Without ethics, peace and justice are improbabilities and corruption is a foregone conclusion.Keywords : morals, deontological, absolute, relative, noble cause, corruptionEthics in the Criminal Justice SystemA thin line separates order from chaos. Criminal justice professionals walk that line, and hold it. The criminal justice system is the complex interworking of law enforcement, courts, and corrections. The common denominator among honest and productive criminal justice professionals is a foundation of ethics on which they build everything that they do. Ethics are far from simple, however; they are as complex as the criminal justice system itself, and the lack of ethics are detrimental to the pursuit of justice. Ethical rules of conduct are infinitely important to the successful operation of a criminal justice organization and the successful achievement of the criminal justice system’s overarching goals.EthicsEthics are defined by Merriam-Webster (n.d.) as “the discipline dealing with what is good and bad and with moral duty and obligation.” Ethics are far from simple, however; the main concern being whose ethics or which ethics we’re talking about. Any discussion of ethics demands further definitions. There are two subcategories of ethics, absolute ethics and relative ethics.Absolute ethics refer to issues where there is either good or bad, right or wrong. These kinds of ethics seem to be sewn into the fabric of our very being, and are nearly universally accepted within a specific society. Examples of absolute ethics include: murder is wrong, extortion is wrong, honesty is good, loyalty is good.Relative ethics, on the other hand, are much more complicated and would be best described as issues that have several shades of grey, rather than being black-and-white. As Khan (2006) wisely says, “ethics can be taught” and continues by saying that ethics must be examined critically in order to fully understand (para. 2). Additionally, Eastvedt (2008) shares, “Without a doubt, there are some philosophical problems when considering ethical concepts … [S]ome people may charge that what may be ethical to one person, may not be considered ethical to others.” Some examples of relative ethical decisions include: the best way to handle homelessness issues within a community and how we can limit the number of drug overdoses. The right or good answer to these questions is mind-dependant.Deontological ethics must also be examined, as it is commonplace within the criminal justice system. Peak (2012) describes deontological ethics as the kind of decision “which does not consider consequences, but instead examines one’s duty to act” (p. 278). Rather than the outcomes motivating the action, it is a sense of duty that drives the action. Criminal justice practitioners are often driven to make ethical decisions out of a sense of duty rather than out of an internal sense of right or wrong. In this case, duty determines right and wrong.Ethics in Law EnforcementEthics is foundational to law enforcement and its importance is highlighted in the intense search for honest, moral, and ethical law enforcement candidates. The average law enforcement hiring process takes between six and eight months and includes a highly invasive background check, a lengthy interview, followed by a polygraph to check for accuracy. Law enforcement organizations expect complete honesty throughout all parts of the application process and demand that honesty to continue through all aspects of the job. Honesty, integrity, and ethical officers are the backbone of any law enforcement organization. Several topics within law enforcement fall into what could be called relative ethical topics and should be explored. Additionally, there are several solutions that will ensure ethicality within criminal justice organizations.Deception, or lying, is in some ways an essential part of the policing process but can also be taken too far into criminality. Accepted lying refers to deception that is generally considered part of the job and can include all kinds of trickery used to apprehend or entrap suspects (Peak, 2012). Deviant lying, however, is described by Peak (2012) as “officers committing perjury to convict suspects or being deceptive about some activity that is illegal or unacceptable” (p. 281). Eastvedt (2008) lists “lying or dishonesty” as “ways for people in the criminal justice community to seriously damage and destroy their integrity” (p. 66). Deception is a curious topic when discussing ethics, but it is clear that the often-debated line must not be crossed.Gratuities is another grey area of ethics. Like deception, minor gratuities are a normal part of a law enforcement officer’s day, but gratuities in excess is synonymous with corruption. Peak (2012) cites the Knapp Commission’s terminology of “grass-eaters” or “meat-eaters” to describe police officers’ relationship to gratuities. A grass-eater is described as on officer who accepts gratuities that are given voluntarily and will sometimes solicit minor gratuities. Meat-eaters, on the other hand, are officers who regularly, and even aggressively, solicit gratuities and search out situations where they can exploit people for person gain. Gratuities are surely a slippery slope that can result in officers sliding into all types of corruption (Peak, 2012).Gratuities have the potential to be the start of a slippery slope to greed, of which there is temptation abound in the criminal justice field. Law enforcement officers are in a seemingly endless cycle of temptation and they are surrounded my crimes and criminality. The temptation to greed can motivate officers to a myriad of types of corruption including crimes relating to drugs, bribes, prostetution, and other abuses of power.Several solutions, or partial solutions, exist for law enforcement organizations when it comes to hiring and maintaining an ethical workforce. As previously mentioned, strict expectations on hiring the right people cannot be overstated. Additionally, proper ongoing ethics training, including regular training on policy and procedure, is necessary. Chilton (1998) asserts that standardization is necessary in ethics training in order to avoid what he calls “the ‘Pinocchio Theory’ problem of personal, idiosyncratic moral judgments in the administration of criminal justice” (p. 40). Law enforcement organizations would also be wise to set strong organizational values in an attempt to “shape the standards of professional behavior”(Peak, 2012, 285). An organization’s culture is often perpetrated by it’s public organizational values.Ethics in the CourtsThe Delaware Judiciary (n.d.) describes one of their core visions as to “insure equal application of the judicial process to all cases, which are fairly decided based upon legally relevant factors.” This equal application and fair decision must be rooted in an ethical foundation. “Because an understanding of judicial ethics is part and parcel of a true appreciation for the core values of the judiciary-judicial independence, integrity, and impartiality-this cannot be an optional project” (Rosenblum, 2007, p. 403). Several standards of conduct exist that relates to ethics in the courtroom, including the Model Code of Judicial Conduct, the Code of Conduct for Federal Judges, and the Ethics Reform Act of 1989. Judges, who preside over a court, and attorneys, who battle each other in court, are both held to high ethical standards.Judges are sworn to administer justice within their courtroom. Judges swear to do this without respect to the people involved but with respect to the Constitution and the laws of the United States (Legal Information Institute, n.d.). This would imply that a judge should not import their emotions, opinions, convictions, or biases into their courtroom decisions. However, this is not the case as judges are human like the rest of us. Ethical behavior by a judge would eliminate favoritism, bias, and impropriety, and carry over into their personal conduct. Appleby &amp; Blackham (2018) assert that there is a current trend toward the “transparent ethical regulation for serving judges” which is said to “promote public confidence in the judicial institution” (p. 506). These ethical codes are independent and do not - can not - eliminate a judge’s personality or emotions to bleed over into their decision making. This is another case of relative ethics, in which there is no specific line between ethical and unethical actions.Attorneys, both on the prosecution and defense side of the courtroom, are also faced with challenges of ethics. Attorneys “must be legally and morally bound to ethical principles as agents of the courts” (Peak, 2012, p. 288). Attorneys are ethically bound to put justice over winning, which unfortunately is rarely the case in today’s court proceedings. Ethical principles also prohibit misconduct such as deception or lying, bribery, concealment of evidence, among other things.Ethics in CorrectionsOn a large scale, there are several ethical issues spanning the correctional system. Albanese (as cited in Khan, 2006) “scrutinizes the moral and ethical ramifications of correctional philosophies, such as retribution, incapacitation, deterrence, and rehabilitation and sentencing methods” (p. 49). These large scale issues are one of the most heavily debated topics in current politics ad media.On a more personal level, correctional officers are subject to most of the same ethical standards as law enforcement officers. Deception plays a very similar role in the day-to-day functioning of a correctional officer. Additionally, several norms exist for correctional officers that function as a sort of code of conduct. These norms include: “always go to the aid of an officer in distress, do not ‘rat,’ never make another officer look back in front of inmates” (Peak, 2012, p. 289), among others. While these norms are important and necessary, it is important for correctional officers to not elevate their code of conduct over absolute ethics.Contraband is a significant facet of how correctional facilities operate, and poses similarly significant ethical issues for correctional officers. Everything from drugs to weapons to cell phones are smuggled into prisons, sometimes at the knowledge of officers or even by officers themselves. This creates numerous opportunities for corruption, greed, and other unethical behavior.Eastvedt (2008) declares that unethical behavior by correctional officers can have significant effects on the organization as a whole:Granted, it may be true that unethical behaviors occurring behind the walls of correctional facilities rarely hit the 6 o’clock news or the front page of the newspaper. However, when it does happen, everyone within the organization is seriously affected. Administrators are held accountable, and staff may be discredited. Morale among the troops can plummet dramatically. Inmates may use the incident to question and challenge line officer authority, making it increasingly difficult for correctional staff to do their jobs. Maintaining security within the jail or prison becomes, at least for a time, a more challenging and daunting task and increases risk to staff and inmates alike. (p. 62)Unethical behavior has a significant negative effect on the entire organization, but that correlation is not limited to just corrections, but extends into all facets of the criminal justice system. Unethical behavior does not just impact the individual, but it sheds negative light on the system as a whole. A single unethical person can be the proverbial bad apple that spoils the whole bunch.ConclusionIt is clear that ethical criminal justice practitioners have an infinitely positive impact on the criminal justice system and that justice crumbles when ethics are replaced by selfishness and corruption. The lack of ethics creates an untrustworthy system, which is not supported by the public. Upholding ethics within the criminal justice system will not only result in justice, but it will also ensure cooperation with the public. Ethics are foundational to the criminal justice system and to the achievement of it’s overarching goals: preservation of peace and fulfillment of justice. Without ethics, peace and justice are improbabilities and corruption is a foregone conclusion.ReferencesAppleby, G., &amp; Blackham, A. (2018). The Shadow Of The Court: The Growing Imperative To Reform Ethical Regulation Of Former Judges.International and Comparative Law Quarterly , 67 (3), 505–546. doi: 10.1017/s0020589318000143Chilton, B. S. (1998). Constitutional conscience: Criminal justice and public interest ethics. Criminal Justice Ethics , 17 (2), 33–41. Retrieved from https://search-proquest-com.libraryresources.waldorf.edu/docview/209772011?accountid=40957Eastvedt, S. R. (2008). Criminal Justice Ethics: A View From the Top.American Jails , 22 (5), 61–62,65-67. Retrieved from https://search-proquest-com.libraryresources.waldorf.edu/docview/222222387?accountid=40957Khan, E. (2006). Professional Ethics in Criminal Justice: Being Ethical When No One is Looking. Corrections Compendium , 31 (5), 48–49. Retrieved from https://search-proquest-com.libraryresources.waldorf.edu/docview/211858471?accountid=40957Legal Information Institute. (n.d.). 28 U.S. Code § 453 - Oaths of justices and judges. Retrieved from https://www.law.cornell.edu/uscode/text/28/453.Merriam-Webster. (n.d.). Ethic. Retrieved from https://www.merriam-webster.com/dictionary/ethic.Peak, K. J. (2012). Justice administration: Police, courts, and corrections management (7th ed.). Upper Saddle River, NJ: Prentice Hall.Rosenblum, E. F. (2007). Judicial Ethics For All: An Expansive Approach to Judicial Ethics Education. Justice System Journal ,28 (3), 394–404. Retrieved from https://search-proquest-com.libraryresources.waldorf.edu/docview/194780465?accountid=40957The Delaware Judiciary. (n.d.). Mission, Vision &amp; Goals. Retrieved from https://courts.delaware.gov/jpcourt/mission.aspx.</t>
+          <t>In decade of transition, fear of leviathan state is giving way to increased focus on oligarchs who the state. In the capture economy, the policy and legal environment is shaped to the firm`s huge advantage, at the expense of the rest of the enterprise sector. This has major implications for policy. The main challenge of the transition has been to redefine how the state interacts with firms, but little attention has been paid to the flip side of the relationship: how firms influence the state-especially how they exert influence on and collude with public officials to extract advantages. Some firms in transition economies have been able to shape the rules of the game to their own advantage, at considerable social cost, creating what Hellman, Jones, and Kaufmann call in many countries. In the capture economy, public officials and politicians privately sell underprovided public goods and range of rent-generating advantages a la carte to individual firms. The authors empirically investigate the dynamics of the capture economy on the basis of new firm-level data from the 1999 Business Environment and Enterprise Performance Survey (BEEPS), which permits the unbundling of corruption into meaningful and measurable components. They contrast state capture (firms shaping and affecting formulation of the rules of the game through private payments to public officials and politicians) with influence (doing the same without recourse to payments) and with administrative corruption (petty forms of bribery in connection with the implementation of laws, rules, and regulations). They develop economywide measures for these phenomena, which are then subject to empirical measurement utilizing the BEEPS data. State capture, influence, and administrative corruption are all shown to have distinct causes and consequences. Large incumbent firms with formal ties to the state tend to inherit influence as legacy of the past and tend to enjoy more secure property and contractual rights and higher growth rates. To compete against these influential incumbents, new entrants turn to state capture as strategic choice-not as substitute for innovation but to compensate for weaknesses in the legal and regulatory framework. When the state underprovides the public goods needed for entry and competition, captor firms purchase directly from the state such private benefits as secure property rights and removal of obstacles to improved performance-but only in capture economy. Consistent with empirical findings in previous research on petty corruption, administrative corruption-unlike both capture and influence-is not associated with specific benefits for the firm. The focus of reform should be shifted toward channeling firms' strategies in the direction of more legitimate forms of influence, involving societal voice, transparency reform, political accountability, and economic competition. Where state capture has distorted reform to create (or preserve) monopolistic structures supported by powerful political interests, the challenge is particularly daunting. This paper - product of the Governance, Regulation, and Finance Division, World Bank Institute; the Public Sector Group, Europe and Central Asia Region; and the Office of the Chief Economist, European Bank of Reconstruction and Development - is part of an empirical project on governance in transition. For an electronic version of this paper and related research papers and governance data, visit www.worldbank/wbi/governance/. The authors may be contacted at jhellman@worldbank.org or dkaufmann@worldbank.org.</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>https://openalex.org/W1495483984</t>
+          <t>https://openalex.org/W1966646743</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://doi.org/10.5772/28453</t>
+          <t>https://doi.org/10.1016/j.envsci.2009.01.001</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Gräupl &amp; Ehammer (2011)</t>
+          <t>Piorr et al. (2009)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>The LDACS1 Link Layer Design</t>
+          <t>Integrated assessment of future CAP policies: land use changes, spatial patterns and targeting</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Air transportation is an important factor for the economic growth of the European Union, however, the current system is already approaching its capacity limits and needs to be reformed to meet the demands of further sustainable development (Commission of the European Communities, 2001). These limitations stem mainly from the current European air traffic control system. Air traffic control within Europe is fragmented due to political frontiers into regions with different legal, operational, and regulative contexts. This fragmentation decreases the overall capacity of the European air traffic control system and, as the system is currently approaching its capacity limits, causes significant congestion of the airspace. According to the European Commission airspace congestion and the delays caused by it cost airlines between €1.3 and €1.9 billion a year (European Commission, 2011). For this reason, the European Commission agreed to adopt a set of measures on air traffic management to ensure the further growth and sustainable development of European air transportation. The key enabler of this transformation is the establishment of a Single European Sky1 (SES). The objective of the SES is to put an end to the fragmentation of the European airspace and to create an efficient and safe airspace without frontiers. This will be accomplished by merging national airspace regions into a single European Flight Information Region (FIR) within which air traffic services will be provided according to the same rules and procedures. In addition to the fragmentation of the airspace the second limiting factor for the growth of European air transportation lies within the legacy Air Traffic Control (ATC) concept. In the current ATC system, which has been developed during the first half of the twentieth century, aircraft fly on fixed airways and change course only over navigation waypoints (e.g. radio beacons). This causes non-optimal paths as aircraft cannot fly directly to their destination and results in a considerable waste of fuel and time2. In addition, it concentrates aircraft onto airways requiring ATC controllers to ascertain their safe separation. The tactical control of aircraft by ATC controllers generates a high demand of voice communication which is proportional to the amount of air traffic. As voice communication</t>
+          <t>The recent and upcoming reforms of the Common Agricultural Policies (CAPs) aim at strengthening the multifunctional role of agriculture, acknowledging the differences in economic, environmental and social potentials within European regions. This paper presents results from an integrated assessment of existing and future policies within the framework set up in the FP6 EU project MEA-Scope. Spatial explicit procedures allow for the MEA-Scope modelling tools to provide information related to regional, environmental and socio-economics settings. The impact of different policy scenarios on structural change, land abandonment and cropping pattern of typical farms has been assessed based on linked agent-based (ABM) and Linear Programming (LP) models at regional and farm scale for two study areas. For the German case study area Ostprignitz-Ruppin (OPR), the issue of policy targeting has been addressed by relating non-commodity outputs (NCOs) to soil quality and protection status. For the Italian case study area (Mugello), changes in landscape patterns in terms of increased fragmentation or homogeneity as affected by changes in agricultural intensity have been analysed using semivariance analysis. The spatial explicit approach highlighted the relevance of case study research in order to identifying response structures and explaining policy implementation patterns.</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>https://openalex.org/W1743767548</t>
+          <t>https://openalex.org/W3129904926</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Mello &amp; Moccero (2006)</t>
+          <t>Bitzan (2018)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Brazil's Fiscal Stance during 1995-2005: The Effect of Indebtedness on Fiscal Policy Over the Business Cycle</t>
+          <t>Transportation Policy and Economic Regulation : Essays in Honor of Theodore Keeler</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Brazil's fiscal adjustment since the floating of the real in 1999 has been impressive, even in periods of lacklustre growth. This suggests a remarkable fiscal effort to ensure public debt sustainability. To better gauge the magnitude of this adjustment effort, this paper applies the methodology used by the OECD Secretariat to distinguish changes in the fiscal stance that are due to policy action from those that are related to the automatic stabilisers built into the tax code, the social security system and unemployment insurance. The paper's main finding is that discretionary action tends to be essentially pro-cyclical in downturns, underscoring the presence of a strong sustainability motive in the conduct of Brazilian fiscal policy. Spending on mandatory items, such as personnel, are pro-cyclical in upturns too, which can create a ratcheting-up effect on government spending over time, an issue that will have to be addressed to improve the quality of on-going fiscal adjustment. An increase in the debt-to-GDP ratio by 1 percentage point is associated with a decrease in discretionary federal spending by 0.33 percentage point during 1997-2005. This responsiveness appears to have become stronger after the floating of the real in 1999. This Working Paper relates to the 2005 OECD Economic Survey of Brazil (www.oecd.org/eco/survey/brazil).</t>
+          <t>Transportation Policy and Economic Regulation: Essays in Honor of Theodore Keeler addresses a number of today's important transportation policy issues, exploring a variety of transportation modes, and examining the policy implications of a number of alternatives. Theodore Keeler had a distinguished career in transportation economics, helping to shape regulatory policies concerning the transportation industries and assessing the appropriateness of various policies. A distinguishing feature of his work is that it always had policy implications. As a tribute to Theodore Keeler, this book examines transportation policy issues across a variety of transportation industries, including aviation, railroads, highways, motor carrier transport, automobiles, urban transit, and ocean shipping. The book evaluates the economic impact and effectiveness of various policies, employing empirical analyses and new estimation techniques, such as Bayesian analysis. The book is designed for transportation professionals and researchers, as well as transportation economics students, providing an in-depth analysis of some of today's important transportation policy issues. Policy changes established in the last 35-40 years have introduced profound changes in the business environment of the transportation industry. Past policy changes promoted the free market's role in setting prices and determining service availability. While 21st century policy has focused on a variety of other issues, such as safety, road and air congestion, productivity growth, labor relations and exhaust emission, many still promote the role of competition. In addition to examining various transportation policy issues in the U.S., the book explores some approaches to dealing with transportation issues in different parts of the world. Contemporary transportation policy debates have broadened from their initial focus of primarily examining the merits of reforming economic regulations at national levels, to now examining a variety of issues such as alternative methods of social regulation (such as safety regulation and emission controls), new approaches to changing economic regulations, the potential for reforming international regulations, and the appropriate role for government in transportation.Examines transportation policy developments across a variety of modes, including some international analysisShows how new policy changes, such as changes in regulation, affect overall transportation system performanceFeatures chapters that use innovative methodologies, such as Bayesian techniques, qualitative analysis, and an attribute-incorporated Malmquist productivity indexExamines the ways that policy impacts depend on a variety of factors, and shows how economic tools can be used to gain greater insights into the likely impacts of policy and the desirability of various policiesAnalyzes transport prices, quality of service, safety, the use of information technology and operating issues, highlighting how transportation enhances quality of life</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2904449631</t>
+          <t>https://openalex.org/W2114340074</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Saputra (2017)</t>
+          <t>Daemmrich &amp; Cameron (2010)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Peraturan Daerah No 9 Tahun 2016 Tentang Penataan Organisasi Perangkat Daerah Pemerintah Provinsi Jawa Tengah</t>
+          <t>U.S. Healthcare Reform: International Perspectives (TN)</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Implementation of regional autonomy (decentralization) is an effort to improve the performance of governance in the region both in the legislature (DPRD) and executive (head area), and also the local bureaucracy, each district / city has full authority to formulate policies, vision, mission and program development closer to the needs and desires of each region. Such changes in a system formed by the central government to the regions will affect the working system, payroll system, budget, administration, scope of work and so that the settings will be adjusted to the policy of strategic stats and abilities that exist in each area. This makes each region should establish, or even to readjust the system bureaucratic work in the area to fit the character of their respective regions to create regional administration in accordance with strategic planning and the ability of each area Government formed to carry out efforts in achieving the objectives of the state, in accordance with the will to be achieved by all the people, which includes order, ensure fairness, doing public works, improve welfare, and preservation of natural resources and the environment. In order to achieve that all governments need to operationalize the organ executing the duties of government in real terms in the lives of everyday people, Organ executor is called bureaucracy. Therefore, the realm of political science, known as a bureaucratic state machine (state machinery) in charge to realize the will of the people is ideal. This the bureaucracy is a tool of the government in creating a governance process in order to achieve the goal, and in order for their objectives to the social order. Therefore the government should look again whether the working system (organization) has been running effectively and efficiently, or should be done restructuring of (reform of the bureaucracy) to fit the dynamic conditions in the community. Reform of the bureaucracy is essentially a change effort or arrangement made conscious government in order to adjust the apparatus of government or government agency with the dynamic changes that occur in a dynamic environment in the community. Efforts are made to carry out the roles and functions correctly and consistently, in order to produce a benefit as mandated by the constitution. Bureaucratic reform should have a goal or objective meaning for improvement of good governance, objectives to be achieved. The targets include, first a lack of compatibility between the number and composition of employees with the needs of the work unit has been arranged based on the vision and mission so that employees have clarity and responsibility. Second, the creation of a match between the competences of the employees with terms of office.Third, the proportional distribution of employees in each unit of work in accordance with their respective workloads. Fourth, the institutional structure of the bureaucracy should see the layout rules (constitutional) that already exist. Parson in HM Ismail explained that the reorganization of the government organization can be reached in two ways, namely downsizing and rightsizing. Downsizing is necessary for improved efficiency in government, because government organizations large and has not been good fat and less efficient. Downsizing meant that government organizations can be made more streamlined and less bureaucratic. Rightsizing needed so that the size of government organizations that there is absolutely appropriate to the needs and conditions. So in addition to downsizing also need to consider the needs of the implications for the size of the organization, and most importantly is to adjust the organizational structure in various areas with the competence of institutions and personnel available. Keywords: Decentralization, Bureaucracy, Bureaucracy Reform</t>
+          <t>The national economic implications of rising healthcare costs were poorly understood, even as the United States, Germany, and the United Kingdom instituted reforms in early 2010. Presenting opportunities for cross-national policy learning, this case describes the political economy of healthcare reform. In late March 2010, a major healthcare reform act was signed into law in the United States, expanding coverage and regulating insurers. However, it was not clear that expanding coverage would resolve a longstanding dilemma of rising costs for insurance and care. As the Department of Health and Human Services implemented the new law, it drew on lessons from Germany, which had implemented changes to regulated but competitive insurance and provider markets, and the United Kingdom, which had introduced market-style initiatives while keeping insurance and delivery under the National Health Service.</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4313466386</t>
+          <t>https://openalex.org/W1992402973</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://doi.org/10.17835/2076-6297.2022.14.4.056-069</t>
+          <t>https://doi.org/10.1080/1360081042000260584</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Margarita &amp; Inna (2022)</t>
+          <t>Katz (2004)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Government Failures in The Implementation of Effective Contracts</t>
+          <t>Market-oriented reforms, globalization and the recent transformation of Latin American innovation systems</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>The paper examines the results of reforms in the remuneration system of university lecturers. Two stages of the transformation process have been considered: the transition to the new remuneration system in 2008 and the introduction of effective contracts in 2012. The paper explains how the political and bureaucratic mechanisms of the formation of the remuneration system have changed. We have made an attempt to describe the government failures in the implementation of effective contracts. It is assumed that the new mechanism remains over-regulated and is based on the idea of the local nature of the academic labor market. The imitation regulation is considered to be one of the most important reasons of the state failures. On the one hand, the government manifested the establishment of understandable and achievable indicators, on the other hand, the authorities failed to solve real problems of the production and transfer of the new knowledge. Governmental stakeholders in education are interested in maintaining and further expanding of their functions. Meanwhile, insufficient professionalism in decision-making and short-termism become the reasons for inefficient waste of budgetary resources for the indicators production and elaboration of various of insurance procedures. The study shows that for many universities the achievement of the target salary level is associated with serious difficulties. There are also significant differences in remuneration systems between universities. Interregional differences in the level of wages of university staff create different conditions for investment in the human capital of university lecturers and incentives for interregional staff turnover that weakens the resource potential of universities in a number of regions.</t>
+          <t>Market-oriented structural reforms were implemented in Latin America under the expectation that the transition from an "inward-oriented", "state-led" growth strategy to one which was more "market-led" and "outward-oriented" was going to be rewarded by a sustainable long-term improvement in the region's rate of economic expansion and productivity growth. The competitive discipline imposed by a more open and deregulated economic regime was expected to induce faster innovation and technological modernization efforts from firms and individuals and, thereafter, a gradual but steady "convergence" to world-wide income and productivity standards. A global look at the region's performance throughout the 1980s and 1990s tells us that such a priori expectation was far from realistic. The paper examines why this has been so.</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2978375441</t>
+          <t>https://openalex.org/W4244531289</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1890/1540-9295-12.3.148</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Lu (2005)</t>
+          <t>ESA (2014)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Study on the Main Problems and Key Factors of National Games Market Operation</t>
+          <t>Dispatches</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>With the deepening reform of market economy , a gradual transition in sports competition management is from the mandatory nature in the past to the market-oriented manner. It is also an increasingly challenging task to create economic benefits through successful market exploitation and management on the basis of maintaining the social benefits of the National Games. The author studied the main problems and key factorsof national games market operation. By using questionnaire survey,the author made a further analysis of the main problems and the key factors in market operation of the National Games. The author believes this thesis will be instructive for the market exploitation and operation of the National Games.</t>
+          <t>On February 20th, Indonesia announced legislation to protect all manta ray populations within its nearly 6 million km2 Exclusive Economic Zone. The move not only establishes the largest manta ray sanctuary in the world, it helps safeguard a diving-tourism industry that annually generates millions in revenue. Indonesia is home to both manta ray species, Manta birostris and Manta alfredi. Their gentle nature and spectacular size makes them favorites with recreational divers, but their slow reproductive cycle leaves them vulnerable to overfishing. Gestation may last over a year before females deliver perhaps just one live pup, sometimes 3–5 years apart. Indeed, a female may produce fewer than 20 offspring over her lifetime. “Sadly, over the past 10 years, mantas have been severely overfished to supply the trade in their gill rakers as a traditional medicinal product in the Guangzhou region of southern China”, says Mark Erdmann, senior advisor to Conservation International's Indonesian Marine Program (Jakarta, Indonesia). “Yet, they are not even recognized as such by most practitioners.” The mantas' dwindling numbers led to their being placed on the Appendix II list of the Convention on International Trade in Endangered Species of Wild Fauna and Flora (CITES). A million dollar ray of hope. Their new protection is in part due to recognition of the enormous economic value of these fish alive compared to their worth as a fisheries product. Last year, a study (PLoS ONE 2013; doi:10.1371/journal.pone. 0065051) showed that Indonesia's manta-diving-tourism industry was worth some US$15 million per year. “Over a manta's lifetime it could be worth $1 million to that industry”, explains Erdmann. “Compare that to the $500 a manta in a net is worth, then you can quickly see that this isn't only great conservation news, it's an economic no-brainer!” Several species of cartilaginous fish, including whale sharks and sawfish, are also protected across Indonesia. “An economic indicator that confirms a species' worth can help lawmakers make decisions that benefit their people in the long term”, comments Mary O'Malley (WildAid, San Francisco, CA). “Fishing such slow-reproducing animals will deplete populations quickly [leaving fishermen without manta fishing income]. Manta tourism income, however, is sustainable and brings income to other local businesses.” In a deal brokered in early February by the Wildlife Conservation Society (WCS), the Government of Madagascar, and Microsoft, the Makira Natural Park (MNP) in Madagascar became the first beneficiary of a government-backed carbon credit sale in Africa. “Through carbon credit sales from avoided deforestation, the Makira REDD+ [Reducing Emissions from Deforestation and Forest Degradation “plus” conservation] Project will finance the long-term conservation of one of Madagascar's most pristine remaining rainforest ecosystems, harboring rare and threatened plants and animals that represent 1% of the world's biodiversity while improving community land stewardship and supporting the livelihoods of the local people”, says WCS Director of Communications Stephen Sautner (New York, NY). “Through a unique funding distribution mechanism designed by the Government of Madagascar and WCS, the funds from carbon sales will be used by the Government for conservation, capacity building, and enforcement activities, and by WCS to manage MNP. The largest share of the sale – one-half of the proceeds – will go toward supporting local communities in the areas surrounding Makira for education, human health, and other development projects.” At nearly 400 000 ha, MNP is a bastion of biodiversity as well as a source of clean water for over 250 000 people in the surrounding areas. “Makira is a highly valued part of our global natural heritage and the revenues from this sale will protect this unique ecosystem, both through supporting park management and rewarding the communities who have helped make the reductions in deforestation possible”, continues Sautner. Each organization will actively contribute to the conservation of Makira, with Microsoft providing the funds through the carbon credit sale, the WCS managing the park, and the Government of Madagascar supporting general long-term conservation and enforcement strategies. As Sautner explains, “The benefit-sharing mechanism also reflects the interdependent governance structures needed to effectively reduce deforestation, including long-term park management, overarching national policy frameworks, and community-based management of different land-use zones surrounding the protected area.” The sale is an important first step and bodes well for the future of carbon credit sales in Madagascar and on mainland Africa. “With this recent sale, the project will be able to invest in validating and verifying the credits achieved through reducing deforestation in 2010 through 2013, thereby broadening the field of potential buyers [and building] toward a national regist</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2523064767</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.1355/cs38-2n</t>
+          <t>https://openalex.org/W2763181898</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Cronin (2016)</t>
+          <t>Mak (2019)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>he Mekong: A Socio-Legal Approach to River Basin Development.</t>
+          <t>Alternative Dispute Resolution of Shareholder Disputes in Hong Kong: Institutionalizing its Effective Use</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>The Mekong: A Socio-Legal Approach River Basin Development. By Ben Boer, Philip Hirsch, Fleur Johns, Ben Saul and Natalia Scurrah. Abingdon, Oxon: Routledge, 2016. Softcover: 251pp. This book is impressive assemblage of scholarship by four professors of and one researcher in human and environmental geography--all based at Australian universities. In eight chapters that bear no single author identification, the book presents the and hydropower development a socio-legal lens and legal pluralism that encompasses both formal or law as well as more informal law. The former includes executive decrees, legislation and action that can be enforced, and especially international governing investment designed reduce political and financial risk foreign capital. The latter ranges from customary rights water, fisheries and forest land, Environment Impact Assessments (EIAs) that lack objective criteria for decision making such as the formally agreed but unenforceable rules including the River Commission's (MRC) Procedures for Notification, Prior Consultation and Agreement (PNPCA) for proposed mainstream dams. The purpose of the book is not explore solutions conflicting local, national and transboundary interests, differing concepts of the objectives of development and the vastly uneven power of stakeholders but to assemble a nuanced account of how laws and institutions at different levels operate and shape water governance outcomes, claims and expectations in the Mekong (p. 35). Some fifty-three joint field interviews conducted in Cambodia, Laos, Thailand and Vietnam inform the range of understandings and expectations of that different actors hold in relation transboundary water governance in the Mekong, and the various factors (historical and contemporary, institutional, regulatory and careerist) by which those understandings and expectations have been shaped (p. 35). The book seeks particularly dispel two prevailing notions: first, the idea that better management of the river basin only awaits the messianic coming of (hard) law which it refutes by presenting an account of the basin as legally saturated, with arguments in regard hydropower in particular shown be, already highly juridified in various (p. 60) and, second, that various policy reform models should be recognized for their political significance and their negotiability, and navigated tactically through socio-legal inquiry and mobilizing a plural understanding of law (p. 60). The authors provide important historical background into how water development and water conflict have evolved in the Lower Basin (LMB) and the varied ways in which both hard and soft have played roles. The book will be of interest anyone concerned about the future of the Mekong, but the focus is on and theory--not moral issues or the impact on real people. Abuses of power and objective human rights constraints in all of the LMB countries are on the whole treated rather antiseptically. The authors frankly acknowledge that civil society has not been effective in using the influence the behaviour of developers or government decision making in any Lower country, with some limited exceptions concerning Thailand when it is not in the thrall of a military coup. Chapter 4 documents and analyzes the formation of the MRC under the 1995 Accord and its ambiguous--hence contestable, negotiable, and changeable--governance role (p. 87). While the conventional wisdom holds that the MRC has largely failed in its coordinating and governance roles, the authors argue that if the softer notion of regulation as exhortatory, goal setting, or framing use of knowledge is taken on board ... then the PNPCA is in fact a suite of measures by which the MRC seeks govern: its knowledge programs, guidelines and standards (p. …</t>
+          <t>The landscape of shareholder dispute resolution in Hong Kong has changed vastly since the launch of the Civil Justice Reform in 2009. Key initiatives - the voluntary court-connected scheme and reform of the statutory unfair prejudice provisions - were employed to promote the greater use of alternative dispute resolution (ADR) in shareholder disputes. While the Hong Kong government and judiciary introduced such schemes to prove the legitimacy of extra-judicial over court-based litigation processes, their success is still uncertain. In this book, socio-legal theory and sociological institutionalism are used to develop a theoretical framework for analyzing the key stages of institutionalization. The author analyzes how procedural innovations could acquire legitimacy through different types of legal and non-legal inducement mechanisms within the institutionalization process. Recommendations on codifying and innovating ADR policy in Hong Kong shareholder disputes are also made with comparison to similar policies in the United Kingdom, South Africa and New Zealand.</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>https://openalex.org/W3157969201</t>
+          <t>https://openalex.org/W410155293</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://doi.org/10.4018/978-1-7998-3964-4.ch011</t>
+          <t>https://doi.org/10.1177/229255030401200207</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Gupta &amp; Shrivastava (2021)</t>
+          <t>Taylor (2004)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Prelude of Investment</t>
+          <t>Working for Free</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>The government of India has taken multiple economic reforms such as Jan Dhan Yojna, UPI, demonetization, and digitalization moving India towards a cashless economy. The financial landscape of India has undergone a radical change with the insurance sector bearing the torch on the road of exponential growth. The insurance penetration recorded was only 3.69% in 2017. The shockingly low participation of individuals indicated the existence of challenges that need to be addressed. The first section of the chapter explores the various factors creating a dilemma for investment in the insurance sector. The other sections of the chapter focus on the current scenario of Insurance investment and the paradigm shift in the perception of customers towards insurance products. The basic purpose is to implement systems thinking of looking at the whole and holistic picture with the highest inclusion towards nation-building and improving the penetration percentage and density of insurance in India.</t>
+          <t>Surgeons believe in certain ideals. We believe we belong to a profession with intrinsic standards. These beliefs involve our duties to patients and our obligations to find the truth and patiently explain what we think in a way people can understand. We are translators and truth seekers and even though this sounds self-exalting, this is who we are. This explains the attractiveness of our work to idealistic young people, and even though the training is long, the goal is worthwhile._x000D_
+_x000D_
+After extended training the time to earn a living has come, but it is a mistake to suppress our idealistic natures and concentrate only on finances. It is too easy to forget Wordsworth’s observation: “getting and spending, we lay waste our powers.” The best kept secret is: volunteer jobs are the best jobs. True, you don’t get paid, but you don’t pay tax either and you can learn things you would never learn any other way. You will develop a breadth of experience that your specialty practice would never allow. A specialty is focusing and that is one of its problems, it can be too focused._x000D_
+_x000D_
+Doctors hate hospital committees, but committees are a good place to understand the bureaucratic mind and the world we live in. Hospitals need us to tell them when they have gone too far, and when they are proposing something doctors will not accept. Many draconian ideas are stopped in committee, and this is where your voice is needed._x000D_
+_x000D_
+Imagine teaching plastic surgery. You might be the first plastic surgeon a medical student meets. Your inspiration could inspire a lifetime career. Explaining your experience to a trainee is an exercise in clarity and analysis. You will learn a great deal as a teacher._x000D_
+_x000D_
+Imagine being chairperson of the ethics committee of a national surgical association. You would have the chance to find out what ethics are, how complaints are managed, and how ethics ideas change. No longer could you grumble about rules from Mount Olympus; you are now on the mount feeling fallible but understanding many sides of the questions and wondering how best to judge. You are seeking wisdom and fairness; representing and leading at the same time. The beauty of not being paid, even though the job is onerous and time consuming, is quite simple. You can never be successfully charged with staying in the job to feather your nest or as a paid lobbyist for one point of view. It is good to move on after a time and pass the job on to other colleagues._x000D_
+_x000D_
+Imagine travelling to another country with a team of surgeons, nurses, and anesthetists to teach surgical techniques. You will make a difference and gain an understanding of the skill of surgeons abroad and what they need to improve outcomes. You will learn that surgeons abroad are very well trained, know many techniques, but don’t have the staff, equipment, drugs or instruments which you take for granted. You will understand, “it’s the economy, stupid.” You will learn that the surgeons you meet are far better at innovation and using what they have than you are. You will go to teach and be taught. You will be humbled by the gratitude shown by patients you help._x000D_
+_x000D_
+Imagine working your way up the executive ladder of a local, provincial or national surgical association doing whatever duty is required and being involved in the debates of the issues as you take on various jobs along the way. These jobs are all unpaid, but think of the experience and insight you will gain._x000D_
+_x000D_
+Imagine sitting on the governing councils of the provincial college as it decides issues regarding our profession. You will realize that the issues involved are far more complex and have greater implications than coffee room rants we enjoy as “stand-up entertainment.”_x000D_
+_x000D_
+Consider being on the board that chooses scholarship winners. You will find it very difficult to decide because the candidates are so well qualified, but you will bring your seasoned judgment to the task._x000D_
+_x000D_
+Why volunteer? There is no pay, it takes time from your practice, and costs you money._x000D_
+_x000D_
+You do it because you want to find out how things work._x000D_
+_x000D_
+You do it to find out if you have skills other than surgery, and you do it because you believe it is worthwhile. In a cynical world where many actions are seen as self-promoting, you are an idealist and seek others like yourself. That is the reason you have to keep what you do quiet, for the more acclaim you get from volunteering, the more the reward ruins its intrinsic value._x000D_
+_x000D_
+You do it because it is a good thing to do._x000D_
+_x000D_
+If you find your practice less satisfying as the years go by, try some volunteering._x000D_
+_x000D_
+It might be what the doctor ordered._x000D_
+_x000D_
+_x000D_
+_x000D_
+_x000D_
+_x000D_
+John R Taylor</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4387164460</t>
+          <t>https://openalex.org/W1577904109</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1016/j.resourpol.2023.104200</t>
+          <t>https://doi.org/10.1080/00076791.2015.1041379</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Zhang et al. (2023)</t>
+          <t>Smith (2015)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Innovative strategies for green economic recovery: Enhancing efficiency in resource markets</t>
+          <t>The winds of change and the end of the Comprador System in the Hongkong and Shanghai Banking Corporation</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>The inefficiency and environmental degradation currently found in China's resource markets are hindering the country's green economic recovery. China has undergone significant economic transformations, but these have often been at the expense of environmental sustainability. This is particularly the case in resource markets. By employing a nonlinear autoregressive distributed lag (NARDL) model, this research investigates the impact of innovative strategies aimed at enhancing efficiency and sustainability in these markets. The years covered by the study are from 1985 to 2020. The study focuses on the role of technological advancements, policy reforms, and market-based incentives in fostering a green economic recovery. The results reveal that innovative strategies have a nonlinear, asymmetric impact on resource market efficiency. Specifically, technological innovations and market-based incentives show a more immediate effect, while policy reforms have a long-term impact. These findings offer a nuanced understanding of the pathways for green economic recovery in China, suggesting that a multi-faceted approach is essential if sustainable development is to be achieved.</t>
+          <t>There was a marked shift in attitudes towards racial and ethnic discrimination in the capitalist world in the 1960s. In Britain and other Western democracies, workplace discrimination became both illegal and socially unacceptable in the years around 1965. At about the same time, decolonisation accelerated. This article will show how the Hongkong and Shanghai Banking Corporation responded to this changing environment by reforming the way it treated non-British workers in Asian markets. Prior to the 1960s, workers had been assigned to ethnic layers, with ethnic Chinese individuals occupying the lowest group and British expatriates filling all executive posts. In the 1960s, this system was scrapped in favour of a less discriminatory one. This article, which is based on research in the company's archive as well as other primary sources, will explore how the bank shed the cultural and institutional legacies of colonialism, which included the so-called comprador system.</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2754918911</t>
+          <t>https://openalex.org/W3095428912</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.19044/esj.2020.v16n29p62</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Zembri (2007)</t>
+          <t>Adeniyi &amp; Olomola (2020)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Pour une approche géographique de la déréglementation des transports</t>
+          <t>Public Interest Litigation (PIL) as Strategic Legal Mechanism on Women’s Socio-Economic Rights in Nigeria: Making a Case for Girl Child Education</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Le terme de dereglementation (traduction de l’anglais « deregulation ») est apparu dans la decennie 1980 en Europe. _x000D_
-Il faut avant tout interpreter ce terme comme toute action de modification du cadre reglementaire de la gestion et du developpement des reseaux. Il ne s’agit pas d’un abandon pur et simple de ce cadre reglementaire : aucun systeme ne vit sans regle… Le sens general des reformes observees est celui du passage d’un role de gestionnaire de reseau, voire d’operateur exploitant en direct, a celui de regulateur et/ou d’instance d’arbitrage pour les collectivites publiques. _x000D_
-Du point de vue du legislateur, la grande variete de reformes dont nous tenterons de rendre compte sous forme typologique dans un premier temps, vise a rationaliser la gestion des services (qu’ils soient organises en reseaux ou non) et a la rendre in fine moins dependante de financements publics, tout en facilitant l’acces des utilisateurs a des prestations mieux adaptees a leurs demandes. On cherche donc autant que possible a supprimer toute rigidite (souvent synonyme de gestion publique) en rapprochant le niveau de decision du terrain et en faisant appel le cas echeant a des entrepreneurs prives, consideres a priori comme plus reactifs et plus soucieux que la puissance publique de l’efficacite de leurs investissements._x000D_
-Notre propos porte plus particulierement sur les reseaux de transport. La structure des reseaux, au sens d’ordonnancement de l’offre dans l’espace et dans le temps, bien que non visee specifiquement par les reformes, est revelatrice des formes d’adaptation des gestionnaires aux nouvelles regles. Elle revele egalement des difficultes non envisagees, qu’elles soient d’ordre technique ou organisationnel. Nous en envisageons quelques-unes dans les domaines ferroviaire et aerien._x000D_
-Le present ouvrage se decompose en sept chapitres, qui pourraient etre regroupes en deux grandes parties : _x000D_
--Les chapitres 1 a 4 rendent compte des evolutions, des strategies et des doctrines qui les sous-tendent. Il s’agit de faire un etat des lieux qui a notre connaissance n’a jamais ete realise, en associant differents modes et differents contextes. Nous rendons compte des differentes formes de dereglementation envisageables, en positionnant le champ des transports dans le contexte plus large des services publics en reseaux (chapitre 1). Nous presentons ensuite les cadres technique, politique et territorial des reformes engagees dans le domaine aerien et dans le domaine ferroviaire (chapitres 2 a 4)._x000D_
--les chapitres 5 a 7 presentent des approfondissements inedits selon un questionnement geographique. La geographie des transports porte une attention particuliere aux structures de reseaux, et aux consequences de la configuration et de la gestion de ces derniers sur les territoires desservis. Nous focalisons donc nos reflexions en premier lieu sur les structures de reseaux resultant des politiques deja menees (chapitre 5) : elles sont beaucoup plus diversifiees que l’on peut l’imaginer a la lecture de la litterature existante. Il est de surcroit interessant de rapprocher les choix qui ont ete effectues par les operateurs aeriens et par les exploitants ferroviaires, certaines similitudes pouvant etre relevees. Nous nous focalisons ensuite sur les territoires desservis (chapitre 6) : les modalites des politiques menees et les strategies des acteurs ont conduit a en favoriser (parfois de facon tres inattendue comme nous le voyons dans le cas du transport aerien), mais aussi parallelement a en penaliser. Cela nous amene a poser la question des politiques publiques qui peuvent etre menees dans un contexte dereglemente, tant pour ce qui concerne le developpement territorial que pour ce qui touche au transport lui-meme. La temporalite des effets est une question-cle : a partir de quel moment peut-on etre assure d’une stabilite suffisante du systeme pour le prendre en compte dans les politiques a mener ou les strategies d’acteurs a developper ?_x000D_
-Les effets observes revelent egalement des limites (chapitre 7) : limites techniques (les reseaux ne peuvent plus, sans investissements lourds, absorber les nouvelles configurations de flux issues du processus d’ouverture du marche), organisationnelles et financieres. Ces limites sont de nature a faire echouer certaines politiques de dereglementation ou a tout le moins d’en limiter la portee._x000D_
-Le volume s‘acheve par une serie de questions sans reponse a ce jour, que nous nous proposons d’explorer dans nos recherches a venir (chapitre conclusif).</t>
+          <t>The percentage of girl child illiteracy is higher in girls than boys in Africa. This is particularly so in Nigeria. It is trite that Girl-child issues are generally confined within women’sright in Nigeria. As important as education isto life and humanity, it however falls under socio economic rights in Nigeria, which by virtue of the interpretation of constitutional provisions are argued as non-justiciable. Hence, accessing education for the girl child as a justice system or mechanism has been a challenge in the country. In recent times, some countries have directed public Interest litigation into fighting some socio-economic issues. This is a development which has not been practiced earlier and success is being recorded. It can be said that Public Interest litigation has been able to deal particularly with the challenge of locus standi which hasto do with the opportunity of accessing justice on some rights issues. Focusing on girl-child education in Nigeria, as a socio-economic rights issue to which access to justice is a challenge and to which legal strategic mechanism can bring a change is a positive one. The paper looks at the impact of African girl child illiteracy at this time in the global environment for sustainable development, the legal impediments to accessing justice on socio economic rights; recent legal mechanisms as best practices of getting socioeconomic rights enforced in some developed countries; innovative and emerging ways of its realization and enforcement in Nigeria. It proffers suggestions on legal and strategic litigation introduction or enhancement mechanism, the challenges if any and the gains more importantly of the public litigation procedure. The paper attempts a desktop and library-based approach in a comparative analysis of legal framework, policies on education, literature review of existing scholarship, case study on strategic litigation in some jurisdictions on socio economic rights and applies it to suggest Public Interest Litigation PIL for girl child education in Nigeria. The paper is germane for women’s right advancement, law and or policy reform and citizen empowerment in Nigeria and Africa at large.</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>https://openalex.org/W356823414</t>
+          <t>https://openalex.org/W4206511092</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1353/lag.2021.0055</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Frank &amp; Gillette (1992)</t>
+          <t>Colón (2021)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Soviet military doctrine from Lenin to Gorbachev, 1915-1991</t>
+          <t>The Environmental Violence of Soy Cultivation in the Brazilian Amazon</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Preface Introduction Setting Soviet Military Doctrine: Form and Content by Robert B. Bathurst Bases of Soviet Military Doctrine by Bruce W. Menning New Thinking and Soviet Military Doctrine by Raymond L. Garthoff Development Lenin and Clausewitz: The Militarization of Marxism, 1914-1921 by Jacob W. Kipp Soviet Military Doctrine and the Origins of Operational Art, 1917-1936 by Jacob W. Kipp Developing Offensive Success: The Soviet Conduct of Operational Maneuver by David M. Glantz Soviet Military Doctrine in the Nuclear Era. 1945-1985 by Harriet Fast Scott The Dilemma in Moscow's Defensive Force Posture by Mary C. FitzGerald Issues The Soviet Military and Change: Implications for the West by Dale R. Herspring Reasonable Sufficiency and Changes in Soviet Security Thinking by Roy Allison Implementing Defensive Doctrine: The Role of Soviet Military Science by Kent D. Lee Soviet Military Doctrine: Past and Present by Valentin V. Larionov Four Models of Force Counterpositioning An Interpretation of General Larionov's Diagram by Lester W. Grau Soviet Military Strategy: Context and Future Prospects by Graham H. Turbiville and David M. Glantz Response by Valentin V. Larionov The Soviet Image of Future War: The Impact of Desert Storm by Mary C. FitzGerald Appendix Introduction Draft Statements on Military Reform (Excerpts) and Military Doctrine (Complete), USSR Ministry of Defense Index</t>
+          <t>The Environmental Violence of Soy Cultivation in the Brazilian Amazon Marcos Colón1 An area of great environmental complexity, inhabited by ancient traditional fishing communities and around 400 Afro-Brazilian (Quilombolas) families, is about to disappear (Locatelli, 2016). I refer to the region of Lago do Maicá (Santarém, Pará, Brazil), an area inhabited by about 1,500 families. Maicá is an ecological sanctuary, a natural cradle for unique species of aquatic fauna and Amazonian bird life. It was here, almost two centuries ago, that two leading British naturalists, Henry Walter Bates and Alfred Russel Wallace, spent three years studying animals and insects. Despite hardships, the men reveled in what they called the “glorious forest” (Bates, 2009 [1863], p. 371). It is estimated that by the end of their three years, they had collected more than 14,000 species of animals (mostly insects). Based on this long and demanding trip, Bates published his book The Naturalist on the River Amazons (Bates, 2009 [1863]), which is still regarded as a classic. Today, besides being a tourist attraction, the lake is also a source of income for the families who make a living from fishing, providing about 30 percent of the fish consumed in town (de Matos Vaz, 2017). Now part of the lake might be turned into a private port for soybean transshipment, which would make it easier for companies like the Brazilian Port Company of Santarém (Embraps) to export goods. The construction of large enterprises in this region will attack Indigenous ways of life and irreversibly damage the environment (Rajão et al., 2020). This will lead to accelerated destruction of the lower wetlands and the expansion of soybean monoculture and its associated high levels of toxicity (Karlsson Pollak, 2020). Santarém is one of the oldest cities in the interior of Amazônia, located at the meeting point of the Tapajós and Amazon Rivers. It was founded by Portuguese Jesuit priests in 1661, as the Portuguese colonized the region. Since then, Santarém has been a strategic production center, first for cacao, then for livestock, the extraction of rubber and jute, and, more recently, for soybean monoculture. Located 500 miles inland from the Atlantic Ocean, its geographical position is strategic for soybean production, whether the crop arrives by road on the sealed highway BR-163 or by barge on the Tapajós River. Crops can be easily trans-shipped down the Amazon River to the Atlantic coast for eventual movement to overseas markets (Colón, 2018). The port project was “sold” to the local population with the promise of generating income and employment in Santarém, in addition to significant taxes that would be collected by the state government. If history is a guide, this is unlikely to actually happen. [End Page 186] The Minnesota-based Cargill Corporation has operated a similar port nearby since the 1970s and stands as a clear example that this type of enterprise does not primarily benefit the local population. Further examples of this can be seen in my film Beyond Ford-lândia: An Environmental Account of Henry Ford’s Adventure in the Amazon (Colón, 2017), which examines the strategies used by these industries and explores the negative impacts that monoculture plantations can have on local populations. The building of a new port zone in the Lago do Maicá region is just part of the region’s soy farmers’ and trading companies’ plans to expand the flow of grains from the Mato Grosso region up to the north of the country, through the Tapajós-Teles Pires axis. Although the plan was embargoed by the Brazilian Court for lack of prior consultation before making purchases, the Embraps Company strategy has been to purchase land and install small projects such as gas stations that will later be used to sustain the activities of the port. How long will the economic power of corrupt politicians continue defying international laws (for instance the Convention 169 of the International Labour Organization) on behalf of a small number of mostly foreign company shareholders (see Colón, 2018)? How long will the Amazon rainforest be at the mercy of politicians and businesspeople who formulate...</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>https://openalex.org/W314657310</t>
+          <t>https://openalex.org/W271392665</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Maraldo (2006)</t>
+          <t>Gillispie (2006)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Saving Zen from Moral Ineptitude: A Response to "Zen Social Ethics: Historical Constraints and Present Prospects"</t>
+          <t>The Neesima Lectures II: The Flourishing of French Science, 1770-1830</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>The four articles on the historical constraints and present prospects of a Zen social ethics are ethical essays in an exemplary sense: although they reflect on what Zen social ethics actually is or has been, their primary concern is with what a Zen social ethics could be or should be. Insofar as the papers are descriptive, they describe a lack or a failure of ethics in the Zen tradition, the failure for example to avert complicity in Japanese militarism and the suffering caused from it. Even where they point to ethical resources within the Zen tradition they do so in the awareness that such resources were not explored, much less utilized, in the past. Yet ... Saving Zen from moral ineptitude is like saving fish from drowning. There are at least three possible senses to this saying: (1) It is nonsense to save fish from drowning and so it is unnecessary to try. From an inherentist perspective, the nature of water is everywhere and there is nowhere it does not reach (like Pao-ch'e's wind in Dogen's Genjokoan, or like Thales' water). (1) The only thing that needs to be done is to get rid of the discriminative thinking that is like putting an oxygen mask over our gills. (2) From an externalist perspective, it is not our concern where the fish--or Zen if you like--finds itself. Not that Zen is good and safe but that it will go the way it goes. It is not our job as scholars to be trying to save it. We can critique its failings but we're not reformers. (3) Our four authors do not speak from either of those two perspectives. Rather they take a kind of internalist perspective--not that they necessarily speak from within the Zen tradition or for it, but rather that they speak as concerned scholars and world citizens. They would say, yes indeed fish can drown. A fish out of water is out of its element; it cannot extract life-sustaining oxygen from the hydrogen in water--it cannot breathe. Traditional as Tom Kasulis intimates, just might drown if it forces itself into a culture with a predominately different ethical orientation--one based on integrity and responsibility rather than intimacy and responsiveness. Or, as Jin Park implies, if it is forced into the atmosphere of traditional normative ethics where clear distinctions between right and wrong are deemed essential. (On the other hand, it might teach normativists a new way to breathe if they take the plunge.) Or, as Dale Wright suggests, Zen might drown if it doesn't change, go beyond itself, and evolve its notion and practice of enlightenment to include competence in ethical reflection. Or indeed when in Christopher Ives' view we are the fish, we can drown in our own ideologies, much as Japanese Zen nearly did before and during World War II. In any case, something needs to be done. Zen needs to do something, or we need to do something with Zen. This is the contention of the four essays in this special issue. And to start off I will agree. I will also accept the convention of identifying a vast array of divergent teachings and practices simply as Zen, as well as the assumption that Zen so identified is a living tradition that has the potential for change. Being ethicists, we want to know, how should things change? What can Zen be? Our authors make suggestions with a good deal of caution and a heavy dose of historical consciousness of what can go wrong. Together they challenge common stereotypes, often perpetrated by Zen Buddhists themselves, that Zen is beyond good and evil, that wisdom and compassion naturally facilitate one another and enlightenment inherently has a moral dimension so morally blind Zen masters don't count as true Zen masters, or that, not relying on words and letters, Zen has detached itself from the realms of politics and social ethics, or that Zen has been of one piece with core Buddhist values. Critical scholars of Zen of course have already exposed these stereotypes as rhetoric removed from reality. …</t>
+          <t>In my lecture on American science, I ventured to characterize a dynamic structure of relations between science and the state, between knowledge and power, as one of the features defining modern political systems. I also suggested that it first took on identifiable form during the period of French scientific eminence at the end of the eighteenth century. The appropriate place to begin developing that proposition is with the ministry of Turgot, the statesman and encyclopedist who drew upon science and systematic knowledge in formulating policies intended to rehabilitate the French monarchy on the accession of Louis XVI in 1774. During the next half-century, say between the last years of d'Alembert and the death of Laplace in 1827, the French scientific establishment predominated in the world to a degree that no other national complex has since done or had ever done. Its eminence persisted through the lifetime of two generations rather well marked off one from the other. The earlier was that of Lavoisier, Laplace, and Monge in their most creative years, of Lagrange in his maturity, of Coulomb, Buffon and the young Lamarck, to name a few of the more famous-in a word, of the final generation of the old Royal Academy of Science, founded in the seventeenth century along with the Royal Society of London. Their successors were the first generation of the Institut de France and the Ecole Polytechnique, still the two senior technical bodies in France; I mention here a few names that appear in all our current textbooks-Ampere, Dulong, Petit, Fresnel, Fourier, Poisson, Cuvier, Bichat, Sadi Carnot, Cauchy. There was a contrast in spirit between those two generations. The outlook of the former was encyclopedist and pertained to the eighteenth century and to the Enlightenment. The outlook of the latter was positivist and pertained to engineering and to the nineteenth century. The succession in generations corresponds to large-scale political phases. The earlier extended from 1774, the beginning of attempts at reform, through the opening of the Revolution in 1789, down to the overthrow of the monarchy late in 1792. The Reign of Terror that ensued in 1793 and 1794 was something of a hiatus in science, though certainly not in politics. The second phase, like the careers of our second group, extended from the reorganization following the overthrow of Robespierre in mid-1794 through the Napoleonic period and the Restoration down to the July Revolution of 1830. In the work of this half-century of science, I believe that French cultural leadership in Europe reached its zenith. I mean that statement very broadly. The critical movement of classicism that distinguished the French intellectual spirit first made itself fully felt in the reign of Louis XIV in the seventeenth century, and in the realm of letters, architecture and manners. Thereafter it took the form of the system of rational ideas about nature, humanity, and society called the Enlightenment. Passing over from thought to action, that movement issued in the incorporation of science into polity amid the circumstances that are the subject of this lecture. Throughout, the sectors in which science came to be of moment to the state were broadly those in which its relation with society have transpired generally in modern history. They were three, as we observed in the case of the maturing of American science over a century later first, administration and public works, civil as well as military; second, education, as to both training and recruitment of elites; third, technology, in respect to industry and agriculture, to engineering and invention. I shall consider first the sense in which science figured in the measures introduced into administration by Turgot and by his entourage. Like their predecessors, the writers and philosophes of the type of Voltaire, Diderot and Rousseau, the enlightened reformers of the last decades of the Old Regime were critical of authority. …</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>https://openalex.org/W1494617239</t>
+          <t>https://openalex.org/W3137051881</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1086/ntj41789677</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Mogg (2002)</t>
+          <t>Strauss &amp; Wittenberg (1987)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Regulating Financial Services in Europe: a New Approach</t>
+          <t>PRICE AND QUANTITY EFFECTS OF TAX REFORM: AN APPLICATION TO WEST VIRGINIA</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>In March 2000, European leaders met in Lisbon, Portugal, to consider the state of the European economy. While there had been economic growth in Europe in the 1990s, it had been consistently lower than that of the European Union’s (“EU” or “Union”) main competitors, with unemployment levels remaining stubbornly high. Determined to blaze a new course in Europe, Heads of State and Government announced that “the Union has [today] set itself a new strategic goal for the next decade: to become the most competitive and dynamic knowledge-based economy in the world, capable of sustainable growth with more and better jobs and greater social cohesion.” These conclusions on economic reform contained a range of policies to stimulate key sectors of the European economy. Delivering this major goal would mean that the EU needed to equip itself with efficient, transparent, and above all, integrated European financial markets. To achieve this, European leaders called for the implementation of the European Commission’s 1999 Financial Services Action Plan by 2005. This target was as ambitious as it was essential, recognizing the fundamental strategic importance of integrated European financial markets for the whole European economy. The economic benefits of improving companies’ access to investment capital and encouraging investors in such an integrated market were seen as central to its achievement. Attention has focused on the importance of achieving higher levels of harmonization of regulations in securities markets. Although turnover on European stock exchanges reached record levels at the end of the 1990s, capital markets remained regulated by essentially outmoded EU legislation, some of which dates back two decades. This is one of the main reasons why levels of capitalization of European stock exchanges have remained considerably below those of the U.S. markets. And despite the 1992 deadline for completion of the EU’s internal market and the fact that many Member States had modernized their market regulations in the 1990s, little had changed at the European level to create a true level playing field. Against this background, and in order to achieve the ambitious goal set at the Lisbon summit, in July 2000, the Council of Economic and Finance Ministers established a high level group of independent figures, the Committee of Wise Men, chaired by Baron Alexandre Lamfalussy, to develop fresh thinking on the reform of the regulatory process for securities. The European Institutions in the course of 2001 endorsed their proposals, and their application is now being extended from securities to all financial services sectors in the Union. REGULATING FINANCIAL SERVICES IN EUROPE: A NEW APPROACH</t>
+          <t>This paper extends a methodology for ascertaining the industry-by-industry effects of tax changes on prices suggested originally by Aaron. The extension utilizes assumptions about the nature of final demand and allows one with an input-output table to derive the total effects of such tax changes in terms of quantities of output as well as employment. The new methodology is applied to West Virginia which substantially reformed its system of gross receipts taxation. The resulting analysis predicts a modest increase in output (+02 percent), and a modest decline in the price level (from -0.1 to -2 percent) as a result of the reforms enacted in 1985, and scheduled to take effect in mid 1987.</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2044203492</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.1177/0974930614521274</t>
+          <t>https://openalex.org/W628568233</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Adi et al. (2013)</t>
+          <t>Reimbladh &amp; Drugge (2006)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Do Privatisation Model, Contractual and Institutional Factors Play Any Role in Infrastructure Post-privatisation Efficiency? Exploring Port Concessions in Nigeria</t>
+          <t>Balanserat styrkort inom hälso- och sjukvården? : Ännu ett styrmedel?</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Privatisation is often seen as the key to achieving efficiency in infrastructure service delivery. In most cases, however, the model of privatisation and the right institutional environment under which they perform best are ignored in addressing the privatisation-to-efficiency debate. Recognising this, we seek to underscore the contractual and institutional factors influencing infrastructure post-privatisation efficiency in Landlord port models as applied in Nigeria’s port reform. In so doing, the study explores the Landlord port privatisation model in Nigeria. The paired t-test and Wilcoxon signed rank sum test are employed to determine if there are significant improvements in port output (general cargo throughput, liquid bulk throughput, number of vessels, gross registered tonnage and container traffic) and efficiency (average waiting time, turnaround time, berth occupancy rate) proxies between the pre-concession, transition and post-concession periods in Nigeria. The result of these tests indicates that although there are significant improvements in the port output proxies, efficiency in the port did not improve significantly. The study identified lack of appropriate legal framework, weak regulatory capacity, absence of efficiency targets in concession contract and non-adherence to investment targets as the major constraints to efficiency gain in the Landlord port model.</t>
+          <t>BackgroundDuring the 1990s, Swedish health care has experienced a vast technological progress while the financial situation has been challenging. To improve the situation at hand several organisational reforms and models have been implemented with the purpose of increased efficiency. This study focuses one of these methods, Balanced Scorecard. The Balanced Scorecard was originally developed for the private sector which causes problems when applying it in a health care setting where there is no overall financial objective and where the customer is hard to define. Beyond that, the health care organisations are complex with professionals making the day-to-day decisions while governed on an overall basis by politicians.PurposeThe purpose of this thesis is to examine the use of the Balanced Scorecard in a Swedish health care setting and to specify and evaluate the prerequisites for the Balanced Scorecard to accommodate efficient management control in health care organisations.Research methodTo be able to fulfil the purpose a case study was conducted at two Swedish public health care organisations. The data was collected by interviews with ten health care managers and a literature survey on the subject.ResultsThe Swedish health care has adapted the Balance Scorecard by changing several of its foundations. Until now, the Balanced Scorecard has been used primarily as a measurement system and a system for supporting discussion and the results of the scorecard can be attributed to an increased clarity and an improved attitude but where the quantifiable results are yet to come. For the Balanced Scorecard to work effectively there is a need for a well established control environment. Finally, management need to show their commitment to the model and give their employees proper training as a mean to increase the acceptance of the scorecard.</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>https://openalex.org/W1947701312</t>
+          <t>https://openalex.org/W2157996265</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>유명복 (2007)</t>
+          <t>Núñez (2003)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>파커 팔머의 교육사상에 대한 고찰</t>
+          <t>Melancholic sounds: singing madness in Restoration drama</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>The purpose of this study is to examine the educational philosophy of Parker Palmer. The grand ideas behind Parker Palmer's educational thoughts are spirituality in education, the inner life of teacher, and community of truth. The idea of nurturing spirituality be a part of educational reform. Palmer defines spiritual as diverse ways we answer the heart's longing to be connected with the largeness of life. He suggests that educational reform may need to start with the transformed heart of the teacher. Good teaching comes from the identity and integrity of the teacher. The meaning of this is that the prodigy of the teacher's task comes from within. Courage to teach retreats do not focus on pedagogical methods or content knowledge, but rather on exploring personal and professional beliefs and how these beliefs affect our teaching. A community of truth is the kind of community related to the way inquiry and discovery have always gone on in the scholarly world. People have to lear to listen each other and learn how to sustain their differences without letting conflict destroy their relationship.</t>
+          <t>The featuring of mad characters on the English stage can be traced as far back as the first dramatic performances in the Elizabethan Age, and more predominantly throughout the seventeenth century. Theatrical insanity reflects the Renaissance attraction and interest in melancholy and mental illnesses, and becomes an arena where tortured psyches interact and express themselves. Madness seems somehow related to music in the Elizabethan and Jacobean drama as part of this more generalised interest, but the reformed Restoration stage is to recall this tradition and develop it into a completely new musical achievement: the mad song. This paper analyses Restoration mad songs as a landmark in the evolution of the conception of madness, in terms of its relationship to music as an expressive means. On the basis of earlyseventeenth century dramatic performances and contemporary treatises on melancholy (Burton), the analysis will focus on Restoration madness as a climatic receptor of this tradition and the ways it transforms it. The attraction that Early Modern England held for melancholy and madness, at times synonymous terms, is now widely recognised. In particular, the period from 1580 to 1640 witnesses the heyday of this fascination. In those decades madness was all pervasive, and the interest in the topic can be traced in various cultural instances: medical treatises, like those of Burton or Bright; in the recurrent references to Bethlehem Hospital, Bedlam; or in the mad characters in the plays of Kyd, Shakespeare, Fletcher, Dekker, Middleton and Webster. Among the latter, two Shakespearean characters function as the main exponents of acted madness, and they both respond to the two different, gendered stereotypes associated to it: a wild, more active, potentially aggressive, even intellectual male madness, and a passive, sexually provocative female one. Hamlet and Ophelia become the very names of human madness, but they are accompanied by a long train of disturbed minds: Lady Macbeth, King Lear or the Gaoler’s daughter. In this way,</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4387932189</t>
+          <t>https://openalex.org/W2500999282</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1596/40525</t>
+          <t>https://doi.org/10.1002/9781118929421.ch21</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Valenzuela et al. (2023)</t>
+          <t>Peña &amp; Alberdi (2016)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>The Integrated Family Record System (SIFF), a Key Tool for Monitoring the Social Determinants of Health in Costa Rica</t>
+          <t>Housing Finance in Spain</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Costa Rica was one of the first countries in the Latin America and Caribbean region to choose the World Bank Program for Results (PforR) financing instrument to support the implementation of the Strategic Agenda for Strengthening Health Insurance by the Costa Rican Social Security Fund (CCSS), for its name in Spanish, Caja Costarricense de Seguro Social). The PforR’s unique features include using a country’s own institutions and processes and linking disbursement of funds directly to the achievement of specific program results, which helps building capacity within the country, enhances effectiveness and efficiency and leads to achievement of tangible, sustainable program results. The CCSS is the primary provider of health care in the country. The PforR “Strengthening Universal Health Insurance in Costa Rica" was approved by the World Bank's Board of Executive Directors in 2016, with the aim of improving the availability and quality of the universal health insurance system while boosting the institutional efficiency of the CCSS. Through the PforR, the CCSS successfully undertook strategic and complex health sector reforms that have had significant impact on quality of care, equity, and efficiency in Costa Rica’s health sector. This series of knowledge reports, developed by the World Bank in collaboration with the CCSS, aims to document the drivers of success, how challenges were faced, and crucial lessons learned during the design and implementation of the PforR and its associated transformative reforms. The overarching objective is to provide a practical guide for other countries interested in implementing similar programs.</t>
+          <t>This paper analyses the economic and institutional environment of the last 25 years in Spain with a focus on the evolution of housing finance and its impact on the housing market. The reforms in the mortgage market started in the mid-1970s but were not completed until the mid-1980s, when they gave rise to a fully deregulated system. The evolution of housing finance in Spain is divided into four periods: the development of the mortgage and housing market between 1986 and 1992; a recession from 1992 to 1996; the strong expansion of the market from 1996 to 2007 and the crisis from 2008 on. The main finance milestones during the last 25 years are analysed, including regulatory, policy and market changes and their linkages. This paper looks at the impacts of these elements in the residential market and finishes by looking into the future.</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4220879831</t>
+          <t>https://openalex.org/W4249695430</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1016/j.mcat.2022.112235</t>
+          <t>https://doi.org/10.1163/9789047422778_010</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Barzegari et al. (2022)</t>
+          <t>He (2007)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Effect of rare-earth promoters (Ce, La, Y and Zr) on the catalytic performance of NiO-MgO-SiO2 catalyst in propane dry reforming</t>
+          <t>8. A Review of Reform and Expectations for the Next Five Years</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>In this contribution, NiO-MgO-SiO2 catalysts containing 3 wt. % of CeO2, La2O3, Y2O3, and Zr2O3 were examined for propane dry reforming at 550-750 °C. The samples were synthesized by a co-precipitation route, followed by a hydrothermal treatment, and characterized by BET, XRD and TPX analyses. The results indicated that the addition of promoters enhanced the metal-support interaction and basic characteristics, while the acidic nature of the promoted catalyst was changed in a different way. The highest propane conversion of 39.6% was observed over Ce-promoter sample, while the un-promoted catalyst possessed a value of 36.8% at 700 °C. Nevertheless, La and Y-promoted catalysts possessed a relatively poor performance, whereby lower CO2 conversion and H2 yield along with the largest amount of by-products. The yield of H2 production decreased in the following order of promoters: Zr&gt;Ce&gt;un-promoted&gt;La&gt;Y. The best catalytic performance observed over ceria-promoted catalysts, supported through the sufficient number of active sites, high oxygen mobility, and redox properties (Ce4+/Ce3+) combined with appropriate acidic/ basic characteristics for reactants activation. The largest amount of coke deposition was detected over the Zr-promoted sample while the Ce-promoted catalyst possessed the lowest carbon formation. The influence of ceria loading on the textural and catalytic properties revealed that the higher loadings of ceria (&gt;3 wt. %) resulted in the formation of ceria island which negatively influenced the catalytic activity. Eventually, 3 wt. % ceria loading was suggested as the optimum loading achieving desirable activity, excellent coke formation resistance, and limited byproducts production over NiO-MgO-SiO2 catalyst.</t>
+          <t>2005 is the last year of the 10th Five-year Plan for economic and social development, and is also a year of periodic results since the start of overall economic reform. At the same time it is also a juncture year as the reforms of the 10th Five-year Plan come to an end and a new round begins as part of the 11th Five-year Plan. It is important to review the progress of reform during the 10th Five-year Plan, and visualize the prospects of reform during the 11th Five-year Plan. During 2001-2005, or the 10th Five-year Plan for economic and social development, a period which also marked five years of transition after China's accession to the WTO, reverse pressure to ease monetary conditions, brought about by the external global economic environment on domestic economic reform, forced China's economic reforms to make a breakthrough.</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>https://openalex.org/W3045481376</t>
+          <t>https://openalex.org/W3196922810</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1016/j.worlddev.2020.105084</t>
+          <t>https://doi.org/10.1051/e3sconf/202129201011</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Pegels &amp; Altenburg (2020)</t>
+          <t>Zhang &amp; Li (2021)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Latecomer development in a “greening” world: Introduction to the Special Issue</t>
+          <t>Research on Innovation Promotion and Application of Guangzhou New Energy Automobile Industry</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>The current transgression of ecological boundaries requires a transformation to a ‘Green Economy’, with rigorous and fast reductions of pollution and resource consumption. Transformative policy reforms towards this aim can lead to economic co-benefits, but they can also be costly, at least for certain economic actors. Furthermore, they can involve trade-offs between current and future wellbeing. Timing and sequencing of reforms is thus far from trivial. More research is needed to inform policymakers in search of the right coping strategies, in particular in economic latecomer countries with persisting poverty and a high need for short-term growth. The main research question of this article is thus: Which economic opportunities arise from orienting economic latecomer strategies towards green technologies and institutions now, versus growing first and cleaning up later? Literature already provides a fair basis of evidence on this question. However, it is biased towards industrialised countries, and towards a subset of green incentives and technologies, such as carbon pricing and renewable energy support. The aim of this article, therefore, is threefold. First and foremost, we review and structure existing evidence and the new evidence provided by this Special Issue along the economic arguments for “greening now” vs. “cleaning up later”. We thus aim to provide an analytical reference point for the growing body of evidence on economic co-benefits of green transformations, helping to structure the debate, to widen its perspective and encourage further research on emerging aspects. Second, we put this structure in the context of latecomer countries, making the identified issues relevant for their framework conditions and showing where and how the articles assembled in the Special Issue fit in the overall debate. Third, we broaden our assessment to include particularly under-researched areas of green transformations in latecomer countries, such as electric mobility, agriculture, steel, and waste management. In reviewing the evidence, we find that early greening is likely to bring economic co-benefits, for example in terms of efficiency-induced competitiveness and in gaining a foothold in the markets of the future. Delaying action, in contrast, risks permanent environmental damage, lock-in of polluting socio-technical pathways, and losses from asset stranding. Yet, the decision between “greening now” and “cleaning up later” is not dichotomous. Careful timing and sequencing of green policy reforms are key, and political decision makers can select and design their national policies in ways that turn changing framework conditions into economic opportunities.</t>
+          <t>The new energy automobile industry has now formed a complete industrial chain. The cities in the Bay Area have a clear division of labor, sufficient technical reserves, and strong policy support. They are emerging industries that are mainly supported. With the continuous upgrading and transformation of the industry, the transformation and upgrading of the Guangzhou automobile industry is on the agenda. This paper discusses the current situation and problems of Guangzhou automobile industry. Analysis of Several Important Influencing Factors of Guangzhou Automobile Industry Innovation in Transformation and Upgrading. Through multi-factor comparison and data analysis, this paper puts forward the corresponding optimization path, in order to accelerate the transformation , upgrading of Guangzhou automobile industry innovation ecosystem and improve the incentive mechanism of Guangzhou new energy automobile industry innovation.</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2469747201</t>
+          <t>https://openalex.org/W2923910044</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1093/obo/9780199756810-0280</t>
+          <t>https://doi.org/10.1093/oso/9780190888183.003.0006</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Bogović &amp; Čegar (2021)</t>
+          <t>Guardino (2019)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Education for Sustainable Development</t>
+          <t>What’s New? Media, Public Opinion, and Democracy in the 21st Century</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Education for Sustainable Development (ESD) is a concept referring to all teaching, learning and capacity building that seeks to develop a citizenry that can live more sustainably on the Earth. It focuses on learning processes and learning environments that can foster the qualities and competencies people need to contribute to more sustainable forms of being. Typically these qualities and related competencies include being caring, mindful, respectful, compassionate, and critical in the way we relate to each other to people elsewhere and future generations, but also to other species; systems thinking; dealing with uncertainty and (eco)anxiety; moral reasoning; anticipatory thinking; and the ability to make change. Within the 2030 Agenda for Sustainable Development, adopted by all United Nations Member States in 2015, ESD became a component of one of the seventeen Sustainable Development Goals (SDGs): SDG 4 ‘Quality Education.’ Newly emerging strands in the context of ESD, also seeking to transcend ESD, include a critical transgressive strand emphasizing the important of not just developing agency and competence that citizens need to learn to live equitably and meaningfully within planetary boundaries, but also helping learners in critiquing and changing or even disrupting structures and systems that normalize unsustainability. Another emerging strand is a posthuman, relational strand that emphasizes the importance of decentering the human and becoming aware of our inevitable entanglement with nature and other species. While receiving much attention in international governance and policy contexts, enactment of ESD in practice lags behind, in part due to different priorities in education at the country level and a lack of understanding of its meaning and its potential significance in reforming education and learning in times of global sustainability challenges. At the same time some scholars critique ESD for being overly instrumental, anthropocentric, and having colonizing tendencies that ignore Indigenous and local perspectives on both education and sustainability.</t>
+          <t>This chapter contextualizes the book’s historical analyses within more recent media developments. It emphasizes the continuing relevance of the book’s analyses of news media and public opinion in the 21st-century technological environment. The chapter connects durable tendencies in corporate news to newer commercial and technological developments in online communication and social media. It explains how emerging forms and uses of media technology often provide new means of influence for corporate media and other centers of concentrated political-economic power. The chapter also presents an empirical analysis of neoliberal news coverage during the 2017 debate over repealing the Affordable Care Act. It ends by discussing possible media reforms that focus on institutional and systemic changes in U.S. political communication.</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>https://openalex.org/W1977777100</t>
+          <t>https://openalex.org/W2947466336</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1080/095465590953460</t>
+          <t>https://doi.org/10.1108/s2516-285320190000002043</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Wright (2006)</t>
+          <t>Gustavsson et al. (2019)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>The Importance of Europe in the Global Campaign Against Terrorism</t>
+          <t>Procurement Research: Current State and Future Challenges in the Nordic Countries</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>ABSTRACT Terrorism and how to respond to it looms large in the current transatlantic debate, with the Europeans often being accused of failing to recognise terrorism as the major strategic issue of the early twenty-first century and thus putting their own security as well as that of others at risk. This is both true and false. It is true in the sense that fifteen years after the end of the Cold War, the Europeans still lack a global strategic vision, never mind how the threat from terrorism might impact upon it. But it is false in the sense that it understates what the Europeans can and are doing to reduce and manage terrorism on a global scale. The article is structured into four sections. The first examines terrorist activity in Europe post-9/11. The second deals with how the Europeans responded to 9/11 collectively within the EU. The third section focuses on what are termed the “outreach” activities of the Europeans via the United National Security Council, G-8, OSCE, NATO, and the European Union. And finally the article concludes that it is this outreach by the Europeans that holds the most promise for effectively countering international terrorism, that the Americans are dependent on this activity, and that the Europeans have to modify their strategic vision in order to deliver more effectively. I would like to acknowledge the assistance of Antionette Turkie in the data collection for this paper. Notes 1. See, for example, J. Stevenson, “How Europe and America Defend Themselves,” Foreign Affairs 82, no. 2 (March/April 2003): 75–86. 2. J. Dempsey, “EU terror strategy looks at grievances that fuel it,” Financial Times, 24 March 2004, 1. 3. See M. Kaldour, “American Power,” International Affairs 71, no. 1 (January 2003): 6. 4. G. Tremlett, “A Better Class of Terrorist,” The Guardian, 10 December 2004. 5. “Madrid car bomb explosion injures at least 42.” International Herald Tribune, (online) 9 February 2005, http://www.iht.com/articles/2005/02/09/europe/web.0209madrid.html 6. R. Cowan, “Real IRA blamed as bomb kills civilian,” The Guardian, 2 August 2002. 7. See D. Pallister, “Car bomb attack foiled in Derry,” The Guardian, 16 June 2003 and J. Humphreys, “10 held in raid on suspected dissident IRA training camp,” Irish Times, 4 August 2003. 8. T. Delpech, “International terrorism and Europe,” Chaillot Paper, No. 56, Paris: Institute for Security Studies, December 2002. 9. F. Butterfield, “Al Qaeda Man Pleads Guilty To Flying With Shoe Bomb,” New York Times, 5 October 2002. 10. See “Eight men in court: the charges,” Timesonline, 18 August 2004, http://www.timesonline.co.uk/article.0,2-1221076,00.html 11. “Turk charged with treason over bombings,” The Scotsman, 20 December 2003. 12. See “Explosives found in Russian air crash wreckage,” The Guardian, 27 August 2004 and N. Paton Walsh, “Moscow seeks UN resolution to speed extradition in terror cases,” The Guardian, 22 September 2004. 13. Two main problems are that while the media do report arrests, they often do not report that individuals were later released without charge or that they were charged with offences unrelated to terrorism—usually immigration or passport irregularities. Second, governments do not always report statistics in these categories. According to The Economist, between September 2001 and January 2003, “around 200 Muslim terrorist suspects have been arrested in Europe—more than in any other region… Some 150 have been arrested in the United States, around 100 in the Middle East, about 50 in North Africa and 40 in Latin America.” See “Tackling a Hydra,” The Economist, 30 January 2003. 14. H. Williamson, “September 11 terror accomplice jailed for 15 years,” Financial Times, 20 February 2003 and P. Finn, “Moroccan Convicted in Sept. 11 Attacks: German Court Delivers Maximum Sentence for Aiding Hamburg Cell,” Washington Post, 20 February 2003. See also R. Bernstein, “Germans blame US for Qaeda acquittal,” International Herald Tribune, 7 February 2004. 15. S. Morris and J. Wilson, “Al-Qaida money men get 11 years,” The Guardian, 2 April 2003. 16. J. Arquilla, D. Ronfeldt, and M. Zanini, “Networks, Netwar and Information-Age Terrorism,” in I. Lesser, B. Hoffman, J. Arquilla, M. Zanini, and B. Jenkins, eds., Countering the New Terrorism (Santa Monica CA: RAND, 1999), 39–84. See also B. Hoffman, Inside Terrorism (New York: Columbia University Press 1999), and J. Stern, The Ultimate Terrorists (Cambridge, MA: Harvard University Press, 1999). 17. H. Müller, “Terrorism, proliferation: a European threat assessment,” Chaillot Papers, no. 58, Paris: Institute for Security Studies, March 2003: 37–38. 18. See Delpech, (see note 8 above), 16. 19. “Tackling a Hydra,” The Economist, 30 January 2003 and Delpech, (see note 8 above). 20. France, for example, was the first country post-9/11 to employ air marshals on Air France flights. 21. For more detail see http://europa.eu.int/comm/110901/index.htm 22. For details see http://europa.eu.int/smartapi/cgi/sga_…lg = EN&amp;numdoc = 32002F0475&amp;model = guichett 23. The EU's list is somewhat different from the U.S.' The major difference has been the Europeans' reluctance to add Hezbollah and Hamas to their lists. In September 2003, however, the EU did add Hamas. It should also be noted that the EU's list is a minimum requirement and member states remain able to add others to their national lists. 24. “Terrorist and Financial Intelligence,” United States Treasury Office of Terrorism and Financial Intelligence, http://www.treas.gov/offices/enforcement/ accessed 13 February 2005. See also Stevenson (see note 1 above) and J. Winer and T. J. Roule, “Fighting Terrorist Finances,” Survival, 44, no. 3, (Autumn 2002): 87–104. 25. R. Watson, “Brussels backs creation of anti-terror czar,” The Times, 19 March 2004, 18. See also B. Brogan, “We must fight terrorism together, EU told,” The Daily Telegraph, 22 March 2004, 1. 26. I. Black, “Britain urges EU to tighten security: Blunkett calls for common rules on data retention,” The Guardian, 19 March 2004, 18. 27. A. Browne and R. Watson, “EU divided over proposal for new anti-terror czar,” The Times, 17 March 2004, 4. 28. Declaration on Combating Terrorism, Brussels, 25 March 2004. 29. J. Dempsey and M. Huband, “Big states back idea of ‘tsar’ to lead war on terrorism EU initiative,” Financial Times, 19 March 2004, 9. 30. D. McGrory and R. Ford, “Al-Qaeda cleric exposed as MI5 double agent,” The Times, 25 March 2004, 15. 31. See, for example, J. Kurlantzick, “Fear Moves East: Terror Targets the Pacific Rim,” Washington Quarterly, 24, no. 1 (Winter 2001). 32. United Nations Security Council, S/RES/1373 (2001) 28 September 2001. 33. The United Nations, S/2001/986, 19 October 2001. 34. United Nations Security Council, S/2004/820, 15 October 2004. 35. http://www.un.org.Docs/sc/committees/1373/INTRO.htm 36. “G8 Foreign Ministers' Progress Report in the Fight Against Terrorism, June 12 2002,” accessed via University of Toronto's G8 Information Centre http://www.g7.utoronto.ca/foreign/fm130602b.htm. For full details of the G8 Action Plan see “Building International Political Will and Capacity to Combat Terrorism – A G8 Action Plan,” http://www.g8.fr/evian/english/navigat…mbat_terrorism__a_g8_action_plan.html 37. G7 is the G8 minus Russia. However, Russia endorsed this Action Plan. 38. “Powell Welcomes OSCE Action Plan Against Terrorism, Dec. 4, 2001,” web version of Colin Powell's remarks following the OSCE Ministerial Conference, Bucharest, 4 December 2001, accessed via http://www.useu.be/Terrorism/EUResponse/ 39. “OSCE says it can be a valuable resource in fight against terrorism, Sept. 6, 2002,” accessed via http://www.useu.be/Terrorism/EUResponse/ 40. “Grossman Says OSCE has made excellent start against Terrorism, Dec. 6, 2002,” accessed via http://www.useu.be/Terrorism/EUResponse/ 41. “Annual Report of the Secretary General on Police-Related Activities in 2003,” OSCE Office of the Secretary General 11 June 2004, SEC.DOC/2/04/Rev.1, p. 31–32. See also OSCE Magazine, October 2004. 42. “High-level Meeting on Migration and Terrorism Opens in Prague, June 3, 2002,” accessed via http://www.useu.be/Terrorism/EUResponse/ 43. At its Prague Summit in November 2002, NATO agreed to a further membership expansion to include the three Baltic Republics plus Bulgaria, Slovenia, Slovakia, and Romania. 44. For full details of contributions see “Fact Sheet: NATO Coalition Contributes to Global War on Terrorism, Oct. 24, 2004” accessed via http://www.useu.be/Terrorism/EUResponse/ 45. “NATO's New Mission is Fighting Terrorism, Robertson Says, June 20, 2002,” accessed via http://www.useu.be/Terrorism/EUResponse/ 46. Lord Robertson, “Transforming NATO,” NATO Review, http://www.nato.int/docu/review/2003/issue1/english/art1.html 47. C. Bennett, “Combatting Terrorism,” NATO Review, http://www.nato.int/docu/review/2003/issue1/english/art2.html 48. Bennett, ibid. 49. The Action Plan also allows for the participation of the Mediterranean Dialogue partners in workshops and seminars and in other activities on a case-by-case basis. 50. These headings are Intensify Consultations and Information Sharing, Enhance Preparedness of Combating Terrorism, Impede Support for Terrorist Groups, Enhance Capabilities to Contribute to Consequence Management and Assistance to Partners' efforts against Terrorism. For full details see The Prague Summit and NATO's Transformation: A Reader's Guide (Brussels: NATO, 2002), 87–93. 51. The U.S. and EU members have generally good bilateral relations. The most difficult relationship is with France. But even this relationship is better than those relationships the U.S. enjoys in many other parts of the world. 52. For more detail see “Fact Sheet: Highlights of US-EU Cooperation July 2001-June 2002, June 28 2002” accessed via http://www.useu.be/Terrorism/EUResponse/ 53. See, for example, J. Wright, Terrorist Propaganda (London: Macmillan, 1990). 54. Seville Presidency Conclusions, 21–22 June 2002, Annex V, paragraph 4. 55. See Thessaloniki Presidency Conclusions, 19–20 June 2001, Annex 1. 56. J. Dempsey, “Brussels urges Iran to reform or face bar on trade talks revival,” Financial Times, 4 May 2004, 9 and S. Castle, “EU threatens aid cuts in terror crackdown,” The Independent, 23 March 2004. 57. On November 4, 2002, during a visit to Brussels Tom Ridge stated “one of the conclusions we drew early on—and I think it's one that our friends in Europe concluded, perhaps before much of the world—was that the reach of terrorism is global, that targets are global in nature, and that at the end of the day the 21st century world needs to find global solutions to global vulnerabilities.” “Homeland Security Advisor Ridge in Brussels for EU, NATO meetings – November 4 2002” accessed via http://www.useu.be/Terrorism/EUResponse/ 58. See J. Lindley French, “In the shade of Locarno? Why European Defence is Failing,” International Affairs, 78, no. 2 (October 2002): 789–811. 59. L. Freedman, “The Revolution in Strategic Affairs,” Adelphi Paper, no. 318, (IISS: OUP, 1998), 10. Additional informationNotes on contributorsJoanne Wright Joanne Wright is Professor of International Relations and Dean of the Faculty of History and Social Science at Royal Holloway, University of London. She has published two books on terrorism and several articles on issues of international and internal security. She is currently editing a special edition of the Journal of Constitutional Studies on re-conceptualising security post-9/11.</t>
+          <t>Abstract Purpose The purpose of the study is to map previous and current construction procurement research to further develop the research in the Nordic counties. Design/Methodology/Approach Mapping of previous and current research based on search in national database. The analysis is based on research perspectives, empirical contexts and research methods. Findings That the blind spots are partly overlapping, but that there is potential for knowledge transfer in some areas. There is also the potential for a Nordic research program on one or several of the blind spots. Research Limitations/Implications The study is limited to PhD and licentiate-thesis reports in Norway and Sweden. Further research should include the other Nordic countries and a more extensive literature review including journal articles to broaden the scope. Findings have implications on collaborative Nordic research initiatives, knowledge transfer and in a longer perspective on the level of procurement knowledge in industry and society. Practical Implications Findings provide a base for future research collaborations, initiatives and applications. Originality/Value Findings provide a comprehensive understanding of construction procurement research in the Nordic countries, starting with Norway and Sweden. This understanding is needed for developing research collaborations and applications. Keywords Procurement research Construction Mapping Project governance Building Infrastructure Citation Gustavsson, T.K., Kadefors, A., Lingegård, S., Laedre, O., Klakegg, O.J., Olsson, N. and Larsson, J. (2019), "Procurement Research: Current State and Future Challenges in the Nordic Countries", Lill, I. and Witt, E. (Ed.) 10th Nordic Conference on Construction Economics and Organization (Emerald Reach Proceedings Series, Vol. 2), Emerald Publishing Limited, Bingley, pp. 195-204. https://doi.org/10.1108/S2516-285320190000002043 Publisher: Emerald Publishing Limited Copyright © 2019, Tina Karrbom Gustavsson, Anna Kadefors, Sofia Lingegård, Ola Laedre, Ole Jonny Klakegg, Nils Olsson, Johan Larsson. License Published in the Emerald Reach Proceedings Series. Published by Emerald Publishing Limited. This article is published under the Creative Commons Attribution (CC BY 4.0) licence. Anyone may reproduce, distribute, translate and create derivative works of this article (for both commercial and non-commercial purposes), subject to full attribution to the original publication and authors. The full terms of this licence may be seen at http://creativecommons.org/licences/by/4.0/legalcode 1. Introduction The construction industry is characterised by interdisciplinary, fragmented and temporary project organisations and process discontinuities, which make construction highly dependent on governance and procurement. Lately, there has been an increased interest for research in construction procurement, for example on client’s procurement strategies (Eriksson et al. 2017), on project performance (Ahmad et al. 2016), collaborative frameworks (Hosseini et al. 2017), supply chain integration (Song et al. 2018) and social requirements (Petersen &amp; Kadefors 2018) to mention only a few. The Nordic countries share several contextual similarities in terms of, for example, public procurement regulations, models for standard contracts, construction industry culture and supplier market. Other aspects of the governance structure differ, as well as the procurement strategies used. This implies that there is considerable potential in comparing procurement research results between the Nordic countries, as well as in integrating and combining research initiatives. To lay a foundation for Nordic research collaboration on construction procurement, there is a need for a comprehensive overview of both previous and current procurement research. This overview should also identify future challenges for procurement research in the Nordic context. The purpose of this paper is to present such an overview and thereby contribute to the development of construction procurement research. It is a first step in this endeavour and it is limited to research performed in Norway and Sweden. 2. Framework Mapping this research is complicated by the multitude of concepts and language variations used to express similar or slightly different phenomena, or the same phenomenon seen from different perspectives, not to mention differences between different industries and research communities. To overcome this confusion the mapping reported here is limited to research related directly to three areas: the governance of construction procurement (GP in Tables 1 and 2) which includes political and market level factors that directly or indirectly affect construction procurement, construction procurement as governance tool (PGT in Tables 1 and 2), which includes the client’s procurement strategies and practices, and effects of construction procurement (EP in Tables 1 and 2), which includes efficiency, innovation, collabora</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2332828952</t>
+          <t>https://openalex.org/W3165697151</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1108/tcj-06-2019-0055</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Guetler (2015)</t>
+          <t>Fleck &amp; Ozlanski (2021)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Negotiating Formal Schooling, Multiple Identities, and Community Advocacy: (Counter)-Narratives of the Somali Bantu Refugees in the United States</t>
+          <t>Cash: never leave home with it?</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Negotiating Formal Schooling, Multiple Identities, and Community Advocacy: (Counter)-Narratives of the Somali Bantu Refugees in the United States examines the educational experiences of SomaliBantu refugees resettled in Upstate, New York. It explores how they negotiate their multiple identities race, gender, class, religion, culture, language, accent, and immigrant status within the formal school setting and environment. Additionally, it highlights the role of the Somali Bantu community organizations in advocating and implementing resettlement services and academic resources for their people. Using critical race theory as theoretical lens and methodology, a qualitative research was conducted to collect data from nine Somali Bantu participants. The findings suggest that the participants experienced both successes and challenges while negotiating formal schooling. Their multiple identities subjected them to bias and discrimination within the schools and the society. Nonetheless, the community organizations play a significant role in supporting their children’s academic achievement as well as sustaining their cultural values and language. Based on the findings, the study recommends strategies and reforms that are conducive for equity in education, academic achievement, and cultural tolerance for a successful transition and integration of the Somali Bantus and other refugees in the United States. Negotiating Formal Schooling, Multiple Identities, and Community Advocacy: (Counter)-Narratives of the Somali Bantu Refugees in the United States By Vivian Fiona Guetler B.A. Alpen-Adria Klagenfurt University, Austria, 2013</t>
+          <t>Theoretical basis The learning objectives aim to provide an understanding of the changing nature of consumer payments and the impact upon both businesses and consumers. This can be achieved by examining the case through the lens of stakeholder theory, which posits that businesses are “responsible … to ‘those groups and individuals who can affect or be affected by their actions.’” Collectively, those groups and individuals are known as stakeholders and they commonly include “customers, employees, suppliers, communities and financiers.” In addition to creating value for the owners, businesses should also consider how they can create value for each of their other stakeholders (Freeman et al. , 2010, p. 9). In addition, consistent with the theory of management control systems (Chenhall, 2003), the automatic processing of cashless transactions enables businesses to more efficiently record their earnings, commission payments (if applicable) and monitor cash collections. As all data are captured in an electronic format, they can easily understand their sales and profitability through user-friendly and visually appealing dashboards. This, in turn, enables them to obtain a more accurate and timely view of their business and they can appropriately adjust their operations and strategy as a result of this information. Finally, cashless payments enable more accurate and efficient reporting of information to taxing authorities, which decreases the possibility that the affected parties would underreport income and underpay taxes. This is similarly consistent with the theory of management control systems (Chenhall, 2003) because the improved systems of financial reporting assure compliance with tax laws and regulations. Research methodology This case was developed using both primary and secondary data sources. The authors interviewed the participants in London and the secondary data collection used relevant sources from appropriate literature and the popular press. Case overview/synopsis In London, consumer transactions were as plentiful as the eight million people who lived there. While cash was considered “king” in retail, cash payments dropped by 15% across the UK in 2017, and debit and credit cards became the predominant payment method (Kollewe, 2018). Cash represented only 40% of customer payments and was expected to drop to 21% by 2026 (Lyons et al. , 2018). This was likely driven by contactless payments whereby consumers preferred the speed and ease of being able to “tap and go.” As businesses were charged fees to accept credit card payments, many expected that small businesses would insist on cash for small transactions. Instead, some banished cash completely. Insights from two London businesses helped explain why some were dropping cash and completely embracing cards. Complexity academic level This case can be used in a variety of undergraduate level courses to discuss trends in customer payment methods and the decisions of some businesses to completely abandon cash. Some example courses and suggested supporting materials include the following: • Consumer behavior • Entrepreneurial finance • Survey of accounting • Introduction to financial accounting.</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2910038680</t>
+          <t>https://openalex.org/W2024720915</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>https://doi.org/10.18764/2446-6549.v4n15p170-196</t>
+          <t>https://doi.org/10.2469/faj.v62.n3.4155</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Rodrigues &amp; Dantas (2019)</t>
+          <t>Marciukaityte et al. (2006)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>TRANSMUTAÇÕES NO ESPAÇO NORDESTINO: ocupação, valorização e metropolização turística no litoral cearense</t>
+          <t>Governance and Performance Changes after Accusations of Corporate Fraud</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>TRANSMUTATIONS IN THE NORTHEAST SPACE: occupation, valuation and tourism metropolization in the cearense coastTRANSMUTACIÓN EN EL ESPACIO NORDESTINO: ocupación, valorización y metropolización turística en el litoral cearenseRESUMONesse artigo tem-se como objetivo central entender o processo de ocupação e valorização da zona costeira cearense. Busca-se compreender a partir das práticas marítimas modernas, como se deu a mudança de mentalidade da população citadina, que se abre para uma nova realidade e passa a ver por outro prisma as zonas de praia. A corrida para as áreas litorâneas e as políticas públicas que direcionam investimentos para o desenvolvimento do turismo ocasiona substanciais mudanças no tecido urbano da Metrópole cearense. Dessa forma, percebe-se na contemporaneidade um fenômeno denominado de metropolização turística. Para se alcançar os objetivos propostos realizou-se um estudo diacrônico do espaço, levantamento bibliográfico a partir de periódicos, livros, dissertações e teses que dessem subsídios para dialogar com o tema proposto. A pesquisa hemerográfica foi realizada a partir de diversas consultas ao acervo do Jornal O Povo, material jornalístico de importante circulação na capital cearense. Realizou-se levantamento de dados em sites específicos como do IBGE, IPECE, Ministério do Turismo – MTUR, Secretaria de Turismo do Ceará – SETUR. Os trabalhos de campo foram essenciais para compreender a dinâmica de valorização e ocupação do litoral cearense.Palavras-chave: Espaço; Turismo; Litoral; Metrópole.ABSTRACTIn this article we have as main objective to understand the process of occupation and valorization of the coastal zone of Ceará. It seeks to understand from the modern maritime practices, as it was the change of mentality of the city population, which opens to a new reality and now sees the beach zones from another perspective. The race to the coastal areas and the public policies that direct investments for the development of the tourism causes substantial changes in the urban fabric of the Ceará State. In this way, a phenomenon called tourism metropolization is perceived in the contemporary world. In order to reach the proposed objectives, a diachronic study of the space was carried out, a bibliographical survey from periodicals, books, dissertations and thesis that gave subsidies to dialogue with the proposed theme. The hemerographic research was carried out from several consultations to the collection of the O Povo, journalistic material of important circulation in the capital of Ceará. Data were collected on specific websites such as IBGE, IPECE, Ministry of Tourism - MTUR, Secretariat of Tourism of Ceará - SETUR. Fieldwork was essential to understand the dynamics of valorization and occupation of the coast of Ceará.Keywords: Space; Tourism; Coast; Metropolis.RESUMENEste artículo tiene como objetivo central entender el proceso de ocupación y valorización de la zona costera cearense. Se busca comprender a partir de las prácticas marítimas modernas, como se dio el cambio de mentalidad de la población urbana, que se abre a una nueva realidad y pasa a ver por otro prisma las zonas de playa. La carrera hacia las áreas costeras y las políticas públicas que dirigen inversiones para el desarrollo del turismo ocasionan sustanciales cambios en el tejido urbano de la Metrópolis cearense. De esta forma, se percibe en la contemporaneidad un fenómeno denominado de metropolización turística. Para alcanzar los objetivos propuestos se realizó un estudio diacrónico del espacio, levantamiento bibliográfico a partir de periódicos, libros, disertaciones y tesis que dieran subsidios para dialogar con el tema propuesto. La investigación hemerográfica fue realizada a partir de diversas consultas al acervo del periódico El Pueblo, material periodístico de importante circulación en la capital cearense. Se realizó el levantamiento de datos en sitios específicos como el IBGE, IPECE, Ministerio de Turismo - MTUR, Secretaría de Turismo de Ceará - SETUR. Los trabajos de campo fueron esenciales para comprender la dinámica de valorización y ocupación del litoral cearense.Palabras clave: Espacio; Turismo; Costa; Metrópolis.</t>
+          <t>AbstractUsing a sample of companies charged with government, financial reporting, or stakeholder fraud or regulatory violation in the United States during the 1978–2001 period, this study found that after the accusation of fraud, companies increased the proportion of outsider directors on their boards of directors and on the monitoring committees of the boards. Furthermore, the results show comparable long-run stock price and operating performance between companies charged with fraud and a matching sample of companies not accused of fraud. Collectively, these results suggest that improvements in internal control systems following accusations of fraud help repair a company’s damaged reputation and reinstate confidence in the company.The commission of corporate fraud is a glaring failure of a company’s internal control system. In previous studies, such failures have been shown to impose significant costs on shareholders. We examine whether the costs of corporate fraud are sufficiently high to motivate changes in internal control systems that may lower the likelihood of future commissions of fraud. We focus on changes in the structure of the board of directors and its committees after the accusation or revelation of fraud because the board stands at the apex of the company’s internal control system.Using press announcements of corporate frauds, we constructed a sample consisting of 133 pairs of “fraud” and “no-fraud” companies matched by industry and size. We found that companies increase the percentage of outside directors on their boards following accusations of corporate fraud and increase the proportion of independent outside directors on the boards’ oversight committees. These changes result in board and committee structures that are comparable to those of no-fraud companies, suggesting that fraud companies attempt to reduce further incidents of fraud.We also examined changes in corporate board structures before and following the 1991 corporate sentencing guidelines instituted by the U.S. Sentencing Commission and present evidence that market-imposed reputational costs alone are sufficient to induce positive changes in the boards of directors of fraud companies.Finally, we examined the long-term financial and operating performance of fraud companies. We found that the postfraud performance of fraud companies is comparable to that of the matched no-fraud companies, indicating that changes in internal control systems following accusations of fraud work toward restoration of the company’s reputation in financial and product markets.Our study has important implications for the ongoing debate on the appropriate size of penalties imposed on companies because our evidence suggests that civil and criminal penalties can be set at low levels. The evidence we present also has implications for recent reforms to reduce the occurrence of corporate fraud, including the Sarbanes–Oxley Act of 2002 and reforms initiated by the NYSE and NASDAQ. These reforms impose several governance provisions on publicly traded companies in the United States that increase the independence of corporate boards and their committees. Our study reinforces the reasoning underlying these reforms because our results indicate that the markets induce companies that have committed or been accused of committing fraud to alter their board structures in a manner consistent with these reforms. But this market-imposed transformation of board structure is largely reactive in nature. Sarbanes–Oxley and the NYSE and NASDAQ rules achieve the same by being proactive. We express our sincere thanks to seminar participants at the 2005 Multinational Finance Society Meeting. Professor Varma also gratefully acknowledges financial support provided by a summer research grant from the Department of Finance at the University of Delaware.</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2121742058</t>
+          <t>https://openalex.org/W2014757568</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>https://doi.org/10.18352/bmgn-lchr.9858</t>
+          <t>https://doi.org/10.4017/gt.2014.12.4.004.00</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Wouters (2014)</t>
+          <t>Morales‐Martínez &amp; Rivera-Meza (2014)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Social Reform in Times of Transition. Reflections on Martin Conway’s The Sorrows of Belgium</t>
+          <t>Public policy on aging and elderly: The case of Costa Rica</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>In his book The Sorrows of Belgium Martin Conway uses the Belgian case to look at the restoration of liberal parliamentary states in Europe between 1945 and 1947. Nico Wouters’ contribution focuses on three elements brought to the fore by Conway: 1) the essential yet ambivalent role played by local government (cities and municipalities), 2) the inability to institutionalise Belgian patriotism as binder for the nation-state and finally, 3) the rift between shifts in class relations and political institutional renewal. His contribution comments on each of these elements, by means of superficial comparisons with the Netherlands. As Conway shows, Belgium’s larger cities were laboratories for new political currents that in the end strengthened centrifugal, regionalist tendencies. On the other hand, the local level as an institutional part of state organisation had a reverse effect in the shorter term. The restoration after the liberation can only be understood when one takes into account how ‘local states’ imposed a compelling framework that limited the opportunities for political renewal. As such, Wouters hypothesises that these local states help to explain in part the institutional conservatism of Belgian elites, a core-element in Conway’s book. On this point Wouters sees mostly similarities with the Netherlands. A Belgian-Dutch difference on the other hand, is that the Dutch did succeed in seamlessly combining an equally conservative post-war restoration with restarting a revitalised collective national identity. Belgium’s failure in this regard was quite evident. Although it is obvious that by 1950 such a renewal had become impossible because of the Royal Question, it is still a question of the extent to which the Belgian state still had some leeway in 1945. The third and most important point is connected to the shifts in social class relations. This concerns mutual power relations, group identities, attitudes and political strategies. The genesis of post-war social reform is merely the tip of the iceberg in this regard. It is clear that there is still a lot of room for research, certainly in a comparative perspective with the Netherlands. This concerns topics such as social class-studies from below, but also their agency vis-à-vis the national state during these crucial years of transition. As such, this contribution primarily underscores the importance of a true social history of Belgium for the 1930s-1940s, a history that would be highly relevant in a comparative framework with the Netherlands, most notably when also analysing the interaction between these social evolutions and political reform in 1945-1947. This review is part of the discussion forum 'The Sorrows of Belgium' (Martin Conway). Sociale hervormingen tijdens transitiejaren. Overwegingen bij Martin Conway’s The Sorrows of BelgiumIn zijn boek The Sorrows of Belgium gebruikt Martin Conway de Belgische casus om te kijken naar het herstel van de liberaal-parlementaire staten in Europa tussen 1945 en 1947. Nico Wouters’ bijdrage richt zich op drie elementen die Conway zelf aanhaalt: 1) de belangrijke maar ambivalente rol van het lokale bestuur (steden en gemeenten), 2) het onvermogen om het Belgische patriottisme als bindmiddel voor de natiestaat institutioneel te verankeren en tot slot 3) de kloof tussen verschuivingen in klassenrelaties en politiek-institutionele vernieuwing. Via een oppervlakkige vergelijking met Nederland plaatst zijn bijdrage kanttekeningen bij elk van deze elementen. Zoals Conway aantoont, waren de grotere steden in België laboratoria voor nieuwe politieke stromingen die uiteindelijk de middelpuntvliedende, regionalistische tendensen versterkten. Anderzijds echter, had volgens Wouters het lokale niveau als administratief en institutioneel onderdeel van de staatsorganisatie op korte termijn een omgekeerd effect. De restauratie na de bevrijding kan enkel worden begrepen door in rekening te brengen dat ‘lokale staten’ een dwingend institutioneel raamwerk oplegden en zo de ruimte voor politieke vernieuwing verengden. Hij werpt dus de hypothese op dat deze lokale staten deels het institutionele conservatisme van de Belgische elites – een kernpunt in het boek van Conway – helpen verklaren. Hier zit zijn inziens vooral een overeenkomst met Nederland. Een Belgisch-Nederlands verschil is dan weer de manier waarop Nederland er wel in slaagde een in wezen even conservatieve naoorlogse restauratie succesvol te koppelen aan een hernieuwde doorstart van een collectieve nationale identiteit. België slaagt daar nogal manifest niet in. Hoewel duidelijk is dat dit wat België betreft tegen 1950 (de Koningskwestie) onmogelijk was geworden, blijft het een debat in hoeverre de Belgische staat hier in 1945 misschien nog wel enige speelruimte had. Het derde en meest belangrijke punt betreft de verschuivingen in sociale klassenverhoudingen. Dit betreft zowel de onderlinge machtsverhoudingen, de groepsidentiteiten, de attitudes als concrete politieke positioneringen. De genese van de naoorlogse sociale hervormingen zijn hier slechts het topje van de ijsberg. Zeker in vergelijking met Nederland wordt duidelijk dat hier nog veel ruimte ligt voor onderzoek. Het gaat dan om sociale studies van klassen van onderuit, maar ook hun agency tegenover de nationale staat tijdens de cruciale transitiejaren. Deze bijdrage onderstreept zo vooral het belang van een echte sociale geschiedenis van België voor de jaren 1930-1940. Wouters’ bijdrage argumenteert dat een Belgisch-Nederlands comparatief perspectief hier erg interessant zou zijn, met name ook voor de wisselwerking tussen deze sociale verschuivingen en de politieke hervormingen na 1945. Deze recensie maakt deel uit van het discussiedossier 'The Sorrows of Belgium' (Martin Conway).</t>
+          <t>Background The Republic of Costa Rica is a Central American country with almost 4,7 million inhabitants (July 2013). Its territory covers a total area of 51,100 km², it is bathed in the east by the Caribbean Sea and to the west by the Pacific Ocean. Regarding maritime boundaries, it borders Panama, Colombia, Nicaragua and Ecuador. Its capital, political and economic center is San Jose, and its official language is Spanish. Over the years, the Costa Rican people have created and inherited a deep sense of peaceful coexistence. Costa Rica has chosen, therefore, for a comprehensive, human-centered policy, marked by a profound respect for the rights and aspirations of the people. Ageing The positive social achievement of extended life expectancy, however, has highlighted the need to seriously address the challenges posed by the aging phenomenon and, especially, their consequences. In Costa Rica this began to occupy the attention of some professionals and institutions about 25 years ago. This led not only to some pioneering studies in the field of aging, but also to the development of important programs and institutions caring for the older person. But it was not until the late nineties that the country has started to enact specific legislation to address this important sector of the national population. Aim Analyzing the history and recent reforms about aging policies in Costa Rica including the evolution of the implemented strategies by the state addressing the situation of senior citizens. Results In this retrospective, it is found that the strong cultural influence of Costa Rica has allowed the state and civil society to develop actions in benefit of this population group, supported by the political constitution. Initially the focus was welfare and protectionist, followed by preventive, and nowadays it is of entitlement. The Comprehensive Law for the Older Adults No. 7935 and the creation of the National Council of the Older Adult as an attached organization of the Presidency of the Republic and governing body on aging have proven strong instruments. Both allow to impulse (i) qualitative changes in the promotion of the care of older adults (ii) a priority policy, conceptualized from the perspective of human rights and (iii) the networking that guarantees a comprehensive and timely care for every individual.  This has allowed the construction of a new culture from the strong compromise that all the policy, financial and social sectors have enacted together with older adults and their families.  It concludes by pointing out the importance of an active participation and stewardship of the older adults when it comes to consultation processes, alliance configuration and accountability about actions for their benefit. Also it stresses the importance of legal instruments concerning the specific necessities of older adults.</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4210368360</t>
+          <t>https://openalex.org/W2790332002</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>https://doi.org/10.5325/scriblerian.53.2.0232</t>
+          <t>https://doi.org/10.1213/ane.0000000000002746</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Kadane (2021)</t>
+          <t>Nickerson &amp; Chikumba (2018)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>&lt;i&gt;Religion in Enlightenment England: An Anthology of Sources&lt;/i&gt;, ed. Jayne Elizabeth Lewis.</t>
+          <t>Access to Medicines for Improving Access to Safe Anesthetic Care</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>This collection of primary sources, the third installment in Baylor University Press’s Documents of Anglophone Christianity series, covers the experience of English Protestants between 1660 and 1750. Jayne Lewis has a record of choosing interesting and revealing sources, and contextualizing them well, as anyone who has used her sourcebook on the trial of Mary Queen of Scots will know. Continuing in this vein, her new collection includes familiar figures—Defoe, Bunyan, Richard Baxter, John Wesley, Isaac Watts, Samuel Clarke, and Tillotson—but also gives attention to overlooked authors, especially women, alongside her thoughtful commentary.The section on spiritual autobiography is a case in point. Included with Bunyan’s Grace Abounding to the Chief of Sinners (1666), an important template for godly autobiographers and diarists, is the autobiography of the Calvinist Baptist Anne Dutton (1750), which offers evidence of the vibrancy of spiritual self-writing well into the eighteenth century and gives ideal expression to the genre. Dutton saw herself as mired in sin, ultimately because of Adam’s sin. With a sense of self-loathing and watchfulness encouraged by her devoutness, she was convinced of her “real inability to do anything that was spiritually good.” That may sound like failure, but the whole point of godly self-writing was to look back over your life and trace, as Lewis puts it, “the arc from sin to grace.” Recognizing that you were “the chief of sinners” was necessary before you could then turn to Christ for reformation.But it is also in sources like Dutton’s autobiography that there is evidence of a tension, rarely felt in Bunyan’s day, between Reformed orthodoxy and the Enlightenment ethos. Dutton’s major premise that moral confidence and behavior were not good enough for salvation—“I’m more vile than any one/of wretched Adam’s race,” she wrote (quoting Thomas Shepherd)—stands in stark contrast to Enlightenment religious thought, which held out the Pelagian promise of moral conduct, considered its divinity reasonable rather than wrathful, and felt an assurance that, despite the Fall, “man” still reflected the divine image in which he was made.If these differences between godly authors and the Enlightenment ethos pervade much of her source material, Lewis’s stated aim was to redraw “the familiar picture of enlightened England as secular, rational, materialist.” Admittedly, and as so many of her sources demonstrate, eighteenth-century Britain in general was not synonymous with these characteristics, but her material also makes clear that the country and enlightened culture should not be conflated. She is eloquent in her introduction in pointing out the overlap between the experiential nature of religious forms like self-writing and the experimental tendencies found in natural philosophy, both of which embody an inductive instinct to draw conclusions from the myriad experiences of daily life. But the effort to find commonalities between Puritan and Enlightenment traditions gets taken too far, as when Anthony Collins is described as “unswervingly a confessed Christian.” Collins applied the skeptical methods he picked up from Pierre Bayle to undermine belief in the Trinity, the immaterial soul, the clergy, the compatibility between the Old and New Testaments, and the doctrine of human depravity. Contemporaries understood what he was after. His books were burned by the common hangman, read as thinly disguised atheism by a who’s who of religious authors (Clarke, Berkeley, Swift, Bentley, Hoadley, etc.), and venerated by French atheists like Baron d’Holbach and Jacques-André Naigeon.Religion in Enlightenment England is, ultimately, less about the Enlightenment, or how enlightened authors viewed religion, than it is about the varieties of English Protestantism during the “age of Enlightenment.” Or just during some part of it—more than half of the excerpted sources come from the seventeenth century and none was written after 1750. This is also a book about Protestantism rather than Christianity. There is little to be learned here about the vibrant and intellectually curious Catholic community in Britain in the same years Lewis covers, and even less about the period’s enthusiasm for Islam, a religion that heretical Protestants found exemplary if only because it said nothing about the Trinity or original sin. The “England” in the title is accurate, considering the contents, but given the fact that “by the second decade of the eighteenth century,” as Lewis writes in her introduction, “all [English religious authors] had reason to think of themselves as Brsitish, and as such they often pondered what many regarded as Britain’s special responsibility in a changing Christian world,” it should not be. Sources on religious issues that underpinned the fraught relationship during this era between England, Scotland, and Ireland, not to mention the burgeoning empire, were unfortunately not included.All of this may indicate that the book does not live up to the promise of its title, but Lewis should be commended for what it offers: a well-framed collection of primary texts on the experience of English Protestants at a time when their orthodoxy was under continual attack.</t>
+          <t xml:space="preserve">Beginning in the 1970s, the concept of essential medicines as a central part of an efficient and equitable health system became the focus of considerable advocacy, research, and policy reforms. The development of essential medicine lists, including national lists and, internationally, the World Health Organization’s (WHO) Model List of Essential Medicines,1 creates a framework of minimum standards for medicines that need to be available in health systems to meet the basic health needs of populations. Indeed, medicines and other health products are one of the health system building blocks, along with the health workforce, health service delivery, financing, leadership, and information systems, that are essential for building equitable and responsive health systems as identified by the WHO.2 More obviously, the practice of anesthesia is inextricably linked to the availability of reliable supplies of high-quality medicines; without anesthetic medicines, the safe provision of anesthetic care is virtually impossible. The impediments to accessing safe, affordable, and reliable medicines, however, are numerous, including legislative and regulatory barriers, market dynamics, supply chains, pharmaceutical companies’ priorities, and others. Despite the centrality of medicines (and the other building blocks) in the delivery of health services, many health programs focused on capacity building in low- and middle-income countries (LMICs) do not adequately address the connections and relationships between the health system building blocks, particularly related to access to medicines.3 A trained health workforce with no medicines, little financial stability, or nowhere to deliver clinical care will be severely limited in their impact. Surgery and anesthesia are, regrettably, not exceptions to this imbalance in priorities, particularly as they relate to health programming in LMICs.4 Indeed, while much work has been done to estimate and reduce the burden of surgical diseases, a global understanding of the barriers to accessing the medicines that are necessary to sustain gains that are made in global surgical care is surprisingly limited. GENERAL OVERVIEW Here, we present an overview of some of the challenges and barriers that patients, providers, and health systems face in improving access to essential anesthetic medicines. We focus on the problems rather than the solutions simply because, in the absence of understanding the problems, it is not possible to propose solutions. Furthermore, we present a global assessment of possible and probable barriers to accessing anesthetic medicines. The reality of medicines and other health technologies is that barriers and facilitators of their availability are nuanced to specific contexts and subject to influences that may or may not be universally present. Economic factors may play an oversized role in some contexts, while regulatory barriers dominate in others. The salient point is that the continuous availability of high-quality anesthetic medicines is subject to many factors, most of which have gone unaddressed by surgery and anesthesia development programs in LMICs, and are poorly understood globally, including in high-income countries, which are also far from immune from things like drug shortages.5 Failing to understand the dynamics of medicines specific to anesthesia clearly comes at a detriment to safe perioperative care for numerous reasons, most notably being that the absence of only a handful of essential medicines such as ketamine, propofol, or thiopentone can cripple a health system’s ability to deliver safe anesthetic care. As the importance of safe surgical care gains traction among policymakers internationally and becomes integrated into universal health coverage, addressing barriers to accessing the medicines essential for delivering safe anesthesia is a vital component in addressing the global burden of unmet surgical needs.6 POSSIBLE ROLE OF ACTIVISTS Decades of activism by patients, local health actors, and international organizations to improve access to medicines in other disease areas (eg, tuberculosis, malaria, and human immunodeficiency virus/acquired immune deficiency syndrome (HIV/AIDS)) and therapeutic classes have resulted in significant policy reforms and programming, as well as a better understanding of the global pharmaceutical landscape and market dynamics for them. These improvements have not been negligible: millions of people today are on antiretroviral medicines that prolong and improve lives and yet did not exist 20 years ago. Activism by patients, civil society, and local and international health actors around access to medicines, specifically, has fostered a productive response to these global health challenges. Indeed, significant gains have been made to scale up care for people living with HIV globally, for example, precisely because of a more nuanced understanding of the antiretroviral market and facilitators (and barriers) for access. While </t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2585536376</t>
+          <t>https://openalex.org/W2041885185</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>https://doi.org/10.24949/njes.v3i1.18</t>
+          <t>https://doi.org/10.1353/jjs.2012.0065</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Siddiq et al. (2010)</t>
+          <t>Gaunder (2012)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Solar Thermal Energy Storage using Liquid Ammonia Systems in Industry</t>
+          <t>&lt;i&gt;Decoding Boundaries in Contemporary Japan: The Koizumi Administration and Beyond&lt;/i&gt; (review)</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>The success of solar thermal systems for electricity production hinges very crucially on the selection, mechanical design and optimal operation of an energy storage system which can enable the continuous operation of a power plant. The energy storage systems being investigated include solid graphite, encapsulated Phase Change Materials (PCMs) and liquids such as water and ammonia. A storage option being investigated for large solar-thermal systems is liquid ammonia which by its endothermic dissociation converts to nitrogen and hydrogen gases, and can be synthesized exothermically to recover heat when required. Ammonia is an abundantly produced chemical, globally and in Pakistan. The synthesis of ammonia with carbon dioxide results in the formation of urea fertilizer, or carbamide (NH2)2 CO at pressures and temperatures of the order of 150atm and 600K respectively. In Pakistan there are eight large urea fertilizer plants based on the reforming and synthesis of natural gas mainly from the Sui and Marri gas fields. This work considers the potential of liquid ammonia as a storage medium especially with regards to its integration into a urea fertilizer Chemical Process Industry (CPI) infrastructure. We discuss essential thermodynamic and reaction kinetic features underlying the process and then focus on the energy balance of a solar thermal plant which requires compressed syngas for an ammonia reactor. A mathematical model, based on the material and energy conservation of constituent gases is used to obtain information on the process dynamics in a synthesis convertor. From this, the energy production from synthesis is estimated and compared with the compression energy requirement. We are able to demonstrate that compression power is a major concern for future thermal storage systems and may well be the single determining factor in the viability of such renewable energy systems.</t>
+          <t>Reviewed by: Decoding Boundaries in Contemporary Japan: The Koizumi Administration and Beyond Alisa Gaunder (bio) Decoding Boundaries in Contemporary Japan: The Koizumi Administration and Beyond. Edited by Glenn D. Hook. Routledge, London, 2011. xvi, 270 pages. $140.00. Decoding Boundaries in Contemporary Japan explores political, economic, and social boundaries in Japan to address why these constraints exist as well as how and why some of these boundaries have shifted in recent years. The administration of Prime Minister Koizumi Jun’ichirō is taken as a point of departure given that its push for both increased international activity and domestic reform shifted many existing boundaries and created new ones. As Glenn Hook explains in the introduction to this edited volume, “The central argument of the book is that, in order to achieve the twin goals of greater international proactivity and domestic reform, the government and other actors supporting the new direction for Japan pushed forward by the Koizumi administration needed to take action in order to destabilize and reformulate a range of extant boundaries” (p. 2). Before boundaries can be “decoded,” though, they must be defined. The introductory chapter by Glenn Hook begins this endeavor by asserting “whether physical or metaphysical, boundaries serve most fundamentally to distinguish between insiders and outsiders” (p. 2). Hook then discusses several different types of boundaries: physical, legal, political, social, and symbolic. As Hook points out, many of these boundaries are invisible; indeed, the concept of a boundary is a heuristic used to gain a better grasp of changes occurring at the international and domestic levels in the economic, political, and social realms. At the international level, Hook argues that the initiatives of the Koizumi administration pushed Japan away from the identity of a “peace state” toward the “role for the nation as an international ally of the United States, as seen in the prime minister’s support for the wars in Afghanistan and Iraq” (p. 4). This shift in policy called into question boundaries set by the constitution and the boundaries of the U.S.-Japan alliance. Unfortunately, the chapters in the volume that focus on international boundaries do little to develop these assertions. Domestically, Hook argues, structural reform and deregulation led to shifts in the boundaries between state, market, and society. Market and state relations after Koizumi’s reform efforts are explicitly addressed in several of the chapters on domestic politics, most directly in Peter von Staden’s chapter on business and government relations postreform and Hasegawa Harukiyo’s chapter on Keidanren and labor unions. State-society boundaries are discussed in Muto Hiromi’s chapter on municipal mergers, Patricia [End Page 473] Steinhoff’s chapter on the criminal justice system, and Roger Goodman’s chapter on education reform. Although the introduction defines boundaries and provides useful distinctions among types of boundaries, the chapter is rather brief. The theoretical discussion of boundaries is contained in eight pages before the introduction of the chapters to follow. This limited discussion of boundaries provides only a basic theoretical understanding and very little common ground for the chapters that follow. Each contributor adopts the language of boundaries; however, few consider boundaries theoretically. It is not completely clear how one can determine the existence of a boundary or measure shifts that occur. The mechanisms that can lead to shifts in boundaries are also underexplored. On the whole, the book would be strengthened by developing more common theoretical ground up front. Nevertheless, the boundary heuristic lends itself to the discussion of insiders and outsiders in the international realm. Several of the chapters nicely discuss the negotiation of boundaries in international society. For example, Hugo Dobson’s chapter on Japan’s attempts to influence membership in the G8 argues that in certain instances Japan has been able to instrumentalize liminality to promote the inclusion in the G8 of new states such as Indonesia, Australia, and China, thereby redefining an existing boundary. Still, Dobson acknowledges that in other cases the “nature, membership, and other characteristics of institutions” are more significant in determining inclusion (Russia) and exclusion (North Korea) (p. 31). Overall, the concept of liminality makes a strong contribution to the discussion of the boundaries of multilateralism. The chapters on piracy and rogue states...</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2054073236</t>
+          <t>https://openalex.org/W4385597147</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1038/150158a0</t>
+          <t>https://doi.org/10.34257/gjmbrbvol23is4pg29</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Stephenson (1942)</t>
+          <t>Chijikwa (2023)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>CAUSES OF INTERTIDAL ZONATION</t>
+          <t>Does the Zambian Legal Environment Support Informal Enterprises `Transition into the Formal Economy?</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>ON June 18 and July 9, the Linnean Society of London, under the chairmanship of the president, Dr. E. S. Russell, discussed the causes of the intertidal zonation of plants and Animals. The discussion was opened by Prof. T. A. Stephenson, who attempted to elucidate the reasons for both the vertical zonation and the horizontal distribution round the coast of the common intertidal organisms of South Africa, as observed by himself and his collaborators during the years 1931-40 (see NATURE, 143, 503 ; 1939). In his introductory remarks Prof. Stephenson stressed the importance of field observation, as well as that of laboratory and field experiment, for the interpretation of intertidal phenomena, and pointed out also that since much of what is observed between tidemarks is evidently due to the operation of complexes of factors, it is doubtful whether much is to be gained by too great insistence on the part played by each individual factor in a complex. After a review of a number of the factors which may be expected to be concerned in intertidal processes (nature of substratum, desiccation, temperature, wave-action, feeding-habits, competition for food and space, salinity, submergence and emergence, oxygen, carbon dioxide and hydrogen ion concentration, nutritive salts, light and taxes) the conclusion was reached that there is scarcely any factor the effect of which between tidemarks can be imagined which is unable to produce some effect on zonation, although certain factors are undoubtedly more important than others; and that the effect of some factors is much more local than that of others. It was further concluded that the principal agent responsible for the horizontal distribution of organisms around South Africa is sea temperature ; that for zonation on open rock the controllers of primary importance are degree of exposure to the desiccation-heat-light complex acting together with degree of exposure to wave action ; that for zonation in rock-pools the leading factors appear to be variations in temperature and salinity ; and that light is probably more generally effective in determining the segregation of shade-loving from surface species than in contributing to the actual zonation. In all cases there are subsidiary effects due to causes other than the major ones.</t>
+          <t>This article provides findings from a study which examined ways in which the Zambian legal environment supports informal enterprises` transition into the formal economy. This qualitative study adopted a phenomenological research design. Data was collected via structured interviews from 11 respondents who were purposively selected. Thematic and content analysis of the data were used to come up with the findings of the study. The findings established that a few laws and policies support and facilitate transitioning from informal to the formal Zambian economy. Further, the findings indicated that enterprises were critical to the economy because of the contribution they made through employment creation and poverty reduction activities, against the desired outcome by government? to have a smaller informal economy in relation to the formal economy. The study also established reasons why some informal enterprises are non-compliant to government compliance requirements. Based on the finding of the study, it was recommended that regulatory institutions be lenient and flexible to allow noncompliant enterprises to smoothly transition to formal economy. It is further recommended that more investment in the change management and education of the informal enterprises is made for owners to value formalisation.</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>https://openalex.org/W1749165747</t>
+          <t>https://openalex.org/W3120613754</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1088/1755-1315/624/1/012195</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Deas &amp; Doyle (2013)</t>
+          <t>Chebochakov et al. (2021)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Building community capacity under ?austerity urbanism?: stimulating, supporting and maintaining resident engagement in neighbourhood regeneration in Manchester</t>
+          <t>Socio-economic problems of agriculture of the Republic of Khakassia during the reform</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>The decline or withdrawal of funding for targeted regeneration programmes in England, linked to the wider programme of austerity in public finances, presents major challenges for deprived neighbourhoods. Government?s expectation is that the demise of most neighbourhood-focused regeneration initiatives will be offset by increased involvement of a host of local, voluntary and private sector actors, as part of a wider programme of localism in which civil society assumes responsibility for public policy and service delivery functions previously exercised by the state. The paper assesses the scope for and likelihood of this radical transformation by considering the experience of four neighbourhoods in Manchester. Through a programme of interviews with a range of stakeholders, the paper explores the implications posed by recent policy reforms for levels of resident activism and engagement, and considers the degree to which neighbourhood actors can build capacity in order to contribute meaningfully to future regeneration efforts. The paper concludes that sustained intervention is needed to ensure that raised levels of social capital resulting from past policy initiatives do not dissipate. Developing community capacity in deprived neighbourhoods, the paper concludes, requires concerted and concentrated policy intervention that is at odds with government?s current emphasis on laissez-faire localism.</t>
+          <t>Abstract The article shows that the socio-economic conditions in the agriculture of the Republic of Khakassia, located in the south of Central Siberia, is undergoing significant changes for 25–28 years after the transition from public to private property. Land use, agricultural products, population size and migration are considered at different periods of reform. During the transition from public ownership to private ownership, a substantial redistribution of arable land occurred.</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4388034470</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.1215/00703370-11037907</t>
+          <t>https://openalex.org/W1875942789</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Kalil et al. (2023)</t>
+          <t>Fernandes et al. (2009)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Welfare Reform and the Quality of Young Children's Home Environments</t>
+          <t>Teaching psychiatric nursing/mental health: its interface with the Brazilian Psychiatric Reform and national curriculum guidelines</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Abstract This study investigates the effects of welfare reform—a major policy shift in the United States that increased low-income mothers' employment and reliance on earnings instead of cash assistance—on the quality of the home environments mothers provide for their preschool-age children. Using empirical methods designed to identify plausibly causal effects, we estimate the effects of welfare reform on validated survey and observational measures of maternal behaviors that support children's cognitive skills and emotional adjustment and the material goods that parents purchase to stimulate their children's skill development. The results suggest that welfare reform did not affect the amount of time and material resources mothers devoted to cognitively stimulating activities with their young children. However, it significantly decreased emotional support provision scores, by approximately 0.3–0.4 standard deviations. The effects appear to be stronger for mothers with lower human capital. The findings provide evidence that welfare reform came at a cost to children in the form of lower quality parenting. They also underscore the importance of considering quality, and not just quantity, in assessing the effects of maternal work-incentive policies on parenting and children's home environments.</t>
+          <t>This theoretical study addresses the education system for Psychiatric Nursing in an increasingly changing world of accelerated scientific and technological modernization. The objective is to discuss the pedagogy in Psychiatric Nursing, and its interface with the principles of the Brazilian psychiatric reform and national curriculum guidelines of nursing undergraduate courses. The theoretical foundation of the study consisted of constructs of the Brazilian psychiatric reform and national curriculum guidelines of nursing undergraduate courses and their relationship to factors constituting the pedagogy in psychiatric nursing. The study shows that it is not enough to identify technical issues regarding contents and teaching, didactic procedures, methods and pedagogical techniques; it is necessary to implement changes, using a new perspective and by daring to question the nature of knowledge and institutional psychiatric practices.</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2036260149</t>
+          <t>https://openalex.org/W2324065595</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1353/aph.1994.0130</t>
+          <t>https://doi.org/10.4157/grj.12.352</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Bishop (1994)</t>
+          <t>Noh &amp; Yosizaki (1936)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>No Santa Claus in Appalachia</t>
+          <t>Terrace Cultivation in Japan. A Geographical Study of Cultural Terraces, as an Element of Cultural Landscape</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>No Santa Claus in Appalachia Bill Bishop Americans think anything's for sale. Fame, good looks, freedom—they all can be bought. And, by God, so can prosperity. That is the attitude these days, as states and cities have committed billions of dollars (in roads, sewers, grants, and taxes foregone) to attract new business to their jurisdictions. It is a national free lunch, a $253million entree for the Mercedes company in Alabama, a $163 million finger sandwich for Disney in Virginia and, in Kentucky, a full-course meal for a variety of companies at a potential cost nearing $3 billion. And the portions are getting bigger. Nissan received a $11,000 per job package when it moved to Symrna, Tennessee, in 1980. Last year, Alabama ladled close to $200,000 per employee for Mercedes and Kentucky granted tax exemptions worth a maximum of $350,000 per job to a small Canadian steel maker. The easy explanation is that this is a modern war between the states, a test of manhood between governors. It's that and more. The incentives given so freely by the states aren't just the result of opportunistic politics. There is in all these high-bid battles a sense that our policies and politics are stuck. We don't know what makes us rich—as an economy or as a people. So we do what we've always done, even if it doesn't make complete sense. As a result, states flounder. They look for a quick solution. And the quickest way to wealth, they think, is also the oldest. They buy what they can—and then steal the rest. The Mercedes deal in Alabama is the latest, largest example of this attempt to purchase prosperity. But it is by no means new. The use of low taxes and government largesse to lure industry is an old Southern tradition. Mississippi pioneered the technique in the 1930s, with a Bill Bishop is a columnistfor the Lexington Herald-Leader, and before that was a news reporterfor the Mountain Eagle in Whitesburg, Kentucky. At one time he and his wife owned and operated a weekly newspaper, The Bastrop County Times, in Smithfield, Texas. program it called BAWI, Balance Agriculture With Industry. BAWI opened the state's purse to out-of-state industries. The state offered Northern business low taxes, free land, and cheap labor. In exchange, the state won Northern-style industry and jobs. The thinking behind BAWI and its progeny was, and is, simple—and, therefore, powerful. Rural, nonindustrial regions need a jumpstart into a modern economy. If a state can reduce the cost of doing business within its borders by lowering taxes, the cost of land and average wages, it can gain an advantage over its industrialized neighbors. That advantage will be enough to attract industries from higher-cost regions. Any job is better than no job, developers said then and now, so states accept low-wage businesses. That's okay, the theory goes, because this is a natural progression. Higher-wage jobs come only after low-wage development . The walk-before-you-can-run analogy receives heavy use by these developers. BAWI was copied, mostly by Mississippi's Deep South neighbors. By the mid-1960s, five of the seven states most generous in handing out tax exemptions were from the South. From the beginning, the program was a loser. W. J. Cash, in his 1941 book The Mind ofthe South, summarized the effects of BAWI and its imitators. "Through its own connivance and at its own desire," Cash wrote, "Dixie was now being worse exploited than even the tariff gang ever dreamed of. What with free sites and the waiving of taxes, about all it was getting out of the removal of the New England mills was the stingy sums paid in wages, which were in turn paid out to the merchants —this and the patriotic exultation of the conviction that it was somehow making the land rich and great." Cash was dead-solid right. Tax abatements for the rural South weren't just a benign policy choice. At times they made things worse. Arkansas, for example, traded low taxes for low-wage jobs in the...</t>
+          <t>As the result of geographical researches on the distribution of terrace cultivation in Japan, the authors conclude that cultivation of this kind in Japan could be classified into three types. I. The first type, which is purely ethnographical, is cultivation by particular races in special districts, e. g. the millet-fields of the natives in the high mountain districts of Taiwan (Formosa). II. The second type is the terraces of rice-paddies, which is the most important in Japan where rice, being the food, is the chief crop. During the long period of feudalism in Japan, the labour of farmers practically counted for nothing, while the farmers were heavily taxed by their landlords, which fact inevitably forced them to cultivate such lands. Thus many slopes were changed into rice-paddies, which naturally took the form of terraces. But obviously, this saturation in the distribution of fields was unnatural. As the result of the result of the great economic revolution that swept over Japan, this unnatural tension had to be eliminated, the direct impetus of which came was the general estimation of the value of labour, and the increased cultivation of crops. This type of terraces is now decreasing in area of distribution. III. The third type is rather new. This is the terraces of such crops as are convenient for planting on slopes, examples of which are the orchards of peaches, oranges, etc, along the coast of the Inland-Sea, or that of mandarin-oranges on the Pacific coast of Sizuoka Prefecture. This type of land-utilization certainly increasing, and is likely to continue to do so in the future.</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2276728518</t>
+          <t>https://openalex.org/W2737160024</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1080/0965156x.2016.1260206</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Benković (2007)</t>
+          <t>Aliyev (2016)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Benchmarking structural and institutional changes of the labour market during the process of integration: Implications for Croatia</t>
+          <t>End to informality? Examining the impact of institutional reforms on informal institutions in post-Euromaidan Ukraine</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Each Eastern European transition country, including Croatia, has experienced a radical_x000D_
-structural change of production and employment since 1990. On the one hand, this_x000D_
-development was and is internally driven by price liberalization, privatization, creation of_x000D_
-financial markets and the restructuring of enterprises. On the other hand, the external_x000D_
-liberalization, the enforced international division of labour and the catching-up process to the_x000D_
-economies of the EU-15 intensified the transformation of the economic structure. These_x000D_
-developments led to a de-industrialization and tertiarization process, whereby the importance_x000D_
-of the service sector for the labour market conditions increased. Due to these structural_x000D_
-changes, institutional conditions of labour markets had to adjust to new challenges which_x000D_
-influence the competitiveness of the Croatian enterprises._x000D_
-The focus in this paper will be on the changes in the employment structure. The measuring of_x000D_
-the extent of labour market reallocation takes place within a qualitative framework of_x000D_
-institutional characteristics consisting of the theoretical implications of Esping-Andersen (e.g._x000D_
-1990). This division contradicts the thesis of ‘Eurosclerosis’ that describes the European labour_x000D_
-markets as rigid model which is unable to adjust changes in economic environment. In fact,_x000D_
-the European labour markets reflect country-specific history and show a low level of_x000D_
-integration through different tax and social security systems. Because of cultural and language_x000D_
-barriers, low transnational labour mobility is possible (North, 1994). The main hypothesis of_x000D_
-Esping-Andersen is that there are in fact three types of arrangements in employment policies.</t>
+          <t>What happens to informal institutions in the process of institutional reforms? This article aims to examine one particular aspect of the complex interaction between institutional reforms and informality; the impact of reforms on informal political institutions. The success of Ukraine’s Euromaidan in overthrowing the autocratic government of Viktor Yanukovich in 2014 has ushered a wind of change into the post-Soviet political landscape, for decades dominated by authoritarian and semi-authoritarian forms of governance and the reliance on informal institutions engraved in political traditions. This study is among the first to question as to whether an ambitious reform agenda currently being implemented by the Ukraine’s post-Euromaidan government has had a notable impact on the deeply rooted informal relations in the political sphere. Drawing its empirical insights from a series of in-depth interviews conducted in Kiev in 2015, this study shows that while informal relations have become increasingly vulnerable to formalization efforts and, as a result, various informal institutions in present-day Ukrainian politics have lost their functions and influence, other informal institutions are not only being preserved by the political elites, but also are being employed to promote the reform processes.</t>
         </is>
       </c>
     </row>

</xml_diff>